<commit_message>
2024 seed starting updates
</commit_message>
<xml_diff>
--- a/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
+++ b/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
@@ -13,11 +13,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="242" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="298" uniqueCount="210">
   <si>
     <t>crop</t>
   </si>
   <si>
+    <t>garlic- german extra hardy hardneck</t>
+  </si>
+  <si>
     <t>kale- lacinato</t>
   </si>
   <si>
@@ -72,22 +75,73 @@
     <t>pepper- pimenta puma</t>
   </si>
   <si>
+    <t>tomato- amish</t>
+  </si>
+  <si>
+    <t>tomato- cherry roma</t>
+  </si>
+  <si>
+    <t>tomato- roma</t>
+  </si>
+  <si>
+    <t>tomato- fresh salsa hybrid</t>
+  </si>
+  <si>
+    <t>broccoli- calabrese</t>
+  </si>
+  <si>
+    <t>basil- sweet</t>
+  </si>
+  <si>
+    <t>catnip</t>
+  </si>
+  <si>
+    <t>cilantro</t>
+  </si>
+  <si>
+    <t>cilantro- calypse</t>
+  </si>
+  <si>
+    <t>coleus- chocolate covered cherry</t>
+  </si>
+  <si>
+    <t>marigold- queen sophia</t>
+  </si>
+  <si>
+    <t>coreopsis- ruby kiss</t>
+  </si>
+  <si>
+    <t>salvia- victoria</t>
+  </si>
+  <si>
     <t>sow_type</t>
   </si>
   <si>
+    <t>outdoor seed</t>
+  </si>
+  <si>
     <t>indoor seed</t>
   </si>
   <si>
     <t>sow_date</t>
   </si>
   <si>
+    <t>2023-11-04</t>
+  </si>
+  <si>
     <t>2024-02-25</t>
   </si>
   <si>
-    <t>2023-03-12</t>
+    <t>2023-02-25</t>
+  </si>
+  <si>
+    <t>2024-03-11</t>
   </si>
   <si>
     <t>sow_med</t>
+  </si>
+  <si>
+    <t>raised bed- ground</t>
   </si>
   <si>
     <t>soilless</t>
@@ -634,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FN19"/>
+  <dimension ref="A1:FN33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -645,511 +699,511 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="N1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="P1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="Q1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="R1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="S1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="T1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="U1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="V1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="W1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="X1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="Y1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="Z1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="AA1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="AB1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="AC1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="AD1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="AE1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="AF1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="AG1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="AH1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="AI1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="AJ1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="AK1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="AL1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="AM1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="AN1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="AO1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="AP1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="AQ1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="AR1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="AS1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="AT1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="AU1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="AV1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="AW1" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="AX1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="AY1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="AZ1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="BA1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="BB1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="BC1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="BD1" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="BE1" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="BF1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="BG1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="BH1" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="BI1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="BJ1" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="BK1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="BL1" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="BM1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="BN1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="BO1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="BP1" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="BQ1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="BR1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="BS1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="BT1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="BU1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="BV1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="BW1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="BX1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="BY1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="BZ1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="CA1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="CB1" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="CC1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="CD1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="CE1" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="CF1" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="CG1" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="CH1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="CI1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="CJ1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="CK1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="CL1" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="CM1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="CN1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="CO1" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="CP1" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="CQ1" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="CR1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="CS1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="CT1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="CU1" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="CV1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="CW1" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="CX1" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="CY1" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="CZ1" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="DA1" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="DB1" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="DC1" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="DD1" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="DE1" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="DF1" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="DG1" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="DH1" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="DI1" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="DJ1" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="DK1" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="DL1" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="DM1" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="DN1" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="DO1" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="DP1" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="DQ1" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="DR1" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="DS1" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="DT1" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="DU1" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="DV1" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="DW1" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="DX1" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="DY1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="DZ1" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="EA1" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="EB1" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="EC1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="ED1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="EE1" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="EF1" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="EG1" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="EH1" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="EI1" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="EJ1" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="EK1" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="EL1" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="EM1" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="EN1" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="EO1" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="EP1" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="EQ1" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="ER1" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="ES1" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="ET1" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="EU1" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="EV1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="EW1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="EX1" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="EY1" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="EZ1" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="FA1" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="FB1" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="FC1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="FD1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="FE1" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="FF1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="FG1" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="FH1" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="FI1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="FJ1" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="FK1" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="FL1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="FM1" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="FN1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2">
@@ -1157,22 +1211,24 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1">
-        <v>50</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>18</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1341,13 +1397,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1">
         <v>50</v>
@@ -1355,9 +1411,15 @@
       <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>6</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1525,26 +1587,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1">
         <v>50</v>
       </c>
       <c r="F4" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
         <v>4</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
       <c r="I4" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1713,13 +1777,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1">
         <v>50</v>
@@ -1730,9 +1794,11 @@
       <c r="G5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
       <c r="I5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1901,13 +1967,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1">
         <v>50</v>
@@ -1918,9 +1984,11 @@
       <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
       <c r="I6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2089,13 +2157,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1">
         <v>50</v>
@@ -2106,9 +2174,11 @@
       <c r="G7" s="1">
         <v>4</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
       <c r="I7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -2277,25 +2347,29 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E8" s="1">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
         <v>4</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -2463,25 +2537,29 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1">
         <v>32</v>
       </c>
       <c r="F9" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1">
         <v>4</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -2649,25 +2727,29 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1">
         <v>32</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>11</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -2835,25 +2917,29 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>32</v>
       </c>
       <c r="F11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>4</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>12</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -3021,25 +3107,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1">
         <v>32</v>
       </c>
       <c r="F12" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G12" s="1">
         <v>4</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>12</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -3207,25 +3297,29 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1">
         <v>32</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1">
         <v>4</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>9</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -3393,25 +3487,29 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1">
         <v>32</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="1">
         <v>4</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="H14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>10</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -3579,25 +3677,29 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1">
         <v>32</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
         <v>4</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1">
+        <v>10</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3765,25 +3867,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1">
         <v>32</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
         <v>4</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>12</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -3951,13 +4057,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E17" s="1">
         <v>32</v>
@@ -3968,8 +4074,12 @@
       <c r="G17" s="1">
         <v>4</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>11</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -4137,13 +4247,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E18" s="1">
         <v>32</v>
@@ -4154,8 +4264,12 @@
       <c r="G18" s="1">
         <v>4</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>13</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -4323,13 +4437,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1">
         <v>32</v>
@@ -4340,8 +4454,12 @@
       <c r="G19" s="1">
         <v>4</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>12</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -4504,6 +4622,2614 @@
       <c r="FM19" s="1"/>
       <c r="FN19" s="1"/>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="1">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>10</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="1"/>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="1"/>
+      <c r="AX20" s="1"/>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="1"/>
+      <c r="BA20" s="1"/>
+      <c r="BB20" s="1"/>
+      <c r="BC20" s="1"/>
+      <c r="BD20" s="1"/>
+      <c r="BE20" s="1"/>
+      <c r="BF20" s="1"/>
+      <c r="BG20" s="1"/>
+      <c r="BH20" s="1"/>
+      <c r="BI20" s="1"/>
+      <c r="BJ20" s="1"/>
+      <c r="BK20" s="1"/>
+      <c r="BL20" s="1"/>
+      <c r="BM20" s="1"/>
+      <c r="BN20" s="1"/>
+      <c r="BO20" s="1"/>
+      <c r="BP20" s="1"/>
+      <c r="BQ20" s="1"/>
+      <c r="BR20" s="1"/>
+      <c r="BS20" s="1"/>
+      <c r="BT20" s="1"/>
+      <c r="BU20" s="1"/>
+      <c r="BV20" s="1"/>
+      <c r="BW20" s="1"/>
+      <c r="BX20" s="1"/>
+      <c r="BY20" s="1"/>
+      <c r="BZ20" s="1"/>
+      <c r="CA20" s="1"/>
+      <c r="CB20" s="1"/>
+      <c r="CC20" s="1"/>
+      <c r="CD20" s="1"/>
+      <c r="CE20" s="1"/>
+      <c r="CF20" s="1"/>
+      <c r="CG20" s="1"/>
+      <c r="CH20" s="1"/>
+      <c r="CI20" s="1"/>
+      <c r="CJ20" s="1"/>
+      <c r="CK20" s="1"/>
+      <c r="CL20" s="1"/>
+      <c r="CM20" s="1"/>
+      <c r="CN20" s="1"/>
+      <c r="CO20" s="1"/>
+      <c r="CP20" s="1"/>
+      <c r="CQ20" s="1"/>
+      <c r="CR20" s="1"/>
+      <c r="CS20" s="1"/>
+      <c r="CT20" s="1"/>
+      <c r="CU20" s="1"/>
+      <c r="CV20" s="1"/>
+      <c r="CW20" s="1"/>
+      <c r="CX20" s="1"/>
+      <c r="CY20" s="1"/>
+      <c r="CZ20" s="1"/>
+      <c r="DA20" s="1"/>
+      <c r="DB20" s="1"/>
+      <c r="DC20" s="1"/>
+      <c r="DD20" s="1"/>
+      <c r="DE20" s="1"/>
+      <c r="DF20" s="1"/>
+      <c r="DG20" s="1"/>
+      <c r="DH20" s="1"/>
+      <c r="DI20" s="1"/>
+      <c r="DJ20" s="1"/>
+      <c r="DK20" s="1"/>
+      <c r="DL20" s="1"/>
+      <c r="DM20" s="1"/>
+      <c r="DN20" s="1"/>
+      <c r="DO20" s="1"/>
+      <c r="DP20" s="1"/>
+      <c r="DQ20" s="1"/>
+      <c r="DR20" s="1"/>
+      <c r="DS20" s="1"/>
+      <c r="DT20" s="1"/>
+      <c r="DU20" s="1"/>
+      <c r="DV20" s="1"/>
+      <c r="DW20" s="1"/>
+      <c r="DX20" s="1"/>
+      <c r="DY20" s="1"/>
+      <c r="DZ20" s="1"/>
+      <c r="EA20" s="1"/>
+      <c r="EB20" s="1"/>
+      <c r="EC20" s="1"/>
+      <c r="ED20" s="1"/>
+      <c r="EE20" s="1"/>
+      <c r="EF20" s="1"/>
+      <c r="EG20" s="1"/>
+      <c r="EH20" s="1"/>
+      <c r="EI20" s="1"/>
+      <c r="EJ20" s="1"/>
+      <c r="EK20" s="1"/>
+      <c r="EL20" s="1"/>
+      <c r="EM20" s="1"/>
+      <c r="EN20" s="1"/>
+      <c r="EO20" s="1"/>
+      <c r="EP20" s="1"/>
+      <c r="EQ20" s="1"/>
+      <c r="ER20" s="1"/>
+      <c r="ES20" s="1"/>
+      <c r="ET20" s="1"/>
+      <c r="EU20" s="1"/>
+      <c r="EV20" s="1"/>
+      <c r="EW20" s="1"/>
+      <c r="EX20" s="1"/>
+      <c r="EY20" s="1"/>
+      <c r="EZ20" s="1"/>
+      <c r="FA20" s="1"/>
+      <c r="FB20" s="1"/>
+      <c r="FC20" s="1"/>
+      <c r="FD20" s="1"/>
+      <c r="FE20" s="1"/>
+      <c r="FF20" s="1"/>
+      <c r="FG20" s="1"/>
+      <c r="FH20" s="1"/>
+      <c r="FI20" s="1"/>
+      <c r="FJ20" s="1"/>
+      <c r="FK20" s="1"/>
+      <c r="FL20" s="1"/>
+      <c r="FM20" s="1"/>
+      <c r="FN20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="1"/>
+      <c r="BB21" s="1"/>
+      <c r="BC21" s="1"/>
+      <c r="BD21" s="1"/>
+      <c r="BE21" s="1"/>
+      <c r="BF21" s="1"/>
+      <c r="BG21" s="1"/>
+      <c r="BH21" s="1"/>
+      <c r="BI21" s="1"/>
+      <c r="BJ21" s="1"/>
+      <c r="BK21" s="1"/>
+      <c r="BL21" s="1"/>
+      <c r="BM21" s="1"/>
+      <c r="BN21" s="1"/>
+      <c r="BO21" s="1"/>
+      <c r="BP21" s="1"/>
+      <c r="BQ21" s="1"/>
+      <c r="BR21" s="1"/>
+      <c r="BS21" s="1"/>
+      <c r="BT21" s="1"/>
+      <c r="BU21" s="1"/>
+      <c r="BV21" s="1"/>
+      <c r="BW21" s="1"/>
+      <c r="BX21" s="1"/>
+      <c r="BY21" s="1"/>
+      <c r="BZ21" s="1"/>
+      <c r="CA21" s="1"/>
+      <c r="CB21" s="1"/>
+      <c r="CC21" s="1"/>
+      <c r="CD21" s="1"/>
+      <c r="CE21" s="1"/>
+      <c r="CF21" s="1"/>
+      <c r="CG21" s="1"/>
+      <c r="CH21" s="1"/>
+      <c r="CI21" s="1"/>
+      <c r="CJ21" s="1"/>
+      <c r="CK21" s="1"/>
+      <c r="CL21" s="1"/>
+      <c r="CM21" s="1"/>
+      <c r="CN21" s="1"/>
+      <c r="CO21" s="1"/>
+      <c r="CP21" s="1"/>
+      <c r="CQ21" s="1"/>
+      <c r="CR21" s="1"/>
+      <c r="CS21" s="1"/>
+      <c r="CT21" s="1"/>
+      <c r="CU21" s="1"/>
+      <c r="CV21" s="1"/>
+      <c r="CW21" s="1"/>
+      <c r="CX21" s="1"/>
+      <c r="CY21" s="1"/>
+      <c r="CZ21" s="1"/>
+      <c r="DA21" s="1"/>
+      <c r="DB21" s="1"/>
+      <c r="DC21" s="1"/>
+      <c r="DD21" s="1"/>
+      <c r="DE21" s="1"/>
+      <c r="DF21" s="1"/>
+      <c r="DG21" s="1"/>
+      <c r="DH21" s="1"/>
+      <c r="DI21" s="1"/>
+      <c r="DJ21" s="1"/>
+      <c r="DK21" s="1"/>
+      <c r="DL21" s="1"/>
+      <c r="DM21" s="1"/>
+      <c r="DN21" s="1"/>
+      <c r="DO21" s="1"/>
+      <c r="DP21" s="1"/>
+      <c r="DQ21" s="1"/>
+      <c r="DR21" s="1"/>
+      <c r="DS21" s="1"/>
+      <c r="DT21" s="1"/>
+      <c r="DU21" s="1"/>
+      <c r="DV21" s="1"/>
+      <c r="DW21" s="1"/>
+      <c r="DX21" s="1"/>
+      <c r="DY21" s="1"/>
+      <c r="DZ21" s="1"/>
+      <c r="EA21" s="1"/>
+      <c r="EB21" s="1"/>
+      <c r="EC21" s="1"/>
+      <c r="ED21" s="1"/>
+      <c r="EE21" s="1"/>
+      <c r="EF21" s="1"/>
+      <c r="EG21" s="1"/>
+      <c r="EH21" s="1"/>
+      <c r="EI21" s="1"/>
+      <c r="EJ21" s="1"/>
+      <c r="EK21" s="1"/>
+      <c r="EL21" s="1"/>
+      <c r="EM21" s="1"/>
+      <c r="EN21" s="1"/>
+      <c r="EO21" s="1"/>
+      <c r="EP21" s="1"/>
+      <c r="EQ21" s="1"/>
+      <c r="ER21" s="1"/>
+      <c r="ES21" s="1"/>
+      <c r="ET21" s="1"/>
+      <c r="EU21" s="1"/>
+      <c r="EV21" s="1"/>
+      <c r="EW21" s="1"/>
+      <c r="EX21" s="1"/>
+      <c r="EY21" s="1"/>
+      <c r="EZ21" s="1"/>
+      <c r="FA21" s="1"/>
+      <c r="FB21" s="1"/>
+      <c r="FC21" s="1"/>
+      <c r="FD21" s="1"/>
+      <c r="FE21" s="1"/>
+      <c r="FF21" s="1"/>
+      <c r="FG21" s="1"/>
+      <c r="FH21" s="1"/>
+      <c r="FI21" s="1"/>
+      <c r="FJ21" s="1"/>
+      <c r="FK21" s="1"/>
+      <c r="FL21" s="1"/>
+      <c r="FM21" s="1"/>
+      <c r="FN21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="1">
+        <v>32</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="1"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="1"/>
+      <c r="BA22" s="1"/>
+      <c r="BB22" s="1"/>
+      <c r="BC22" s="1"/>
+      <c r="BD22" s="1"/>
+      <c r="BE22" s="1"/>
+      <c r="BF22" s="1"/>
+      <c r="BG22" s="1"/>
+      <c r="BH22" s="1"/>
+      <c r="BI22" s="1"/>
+      <c r="BJ22" s="1"/>
+      <c r="BK22" s="1"/>
+      <c r="BL22" s="1"/>
+      <c r="BM22" s="1"/>
+      <c r="BN22" s="1"/>
+      <c r="BO22" s="1"/>
+      <c r="BP22" s="1"/>
+      <c r="BQ22" s="1"/>
+      <c r="BR22" s="1"/>
+      <c r="BS22" s="1"/>
+      <c r="BT22" s="1"/>
+      <c r="BU22" s="1"/>
+      <c r="BV22" s="1"/>
+      <c r="BW22" s="1"/>
+      <c r="BX22" s="1"/>
+      <c r="BY22" s="1"/>
+      <c r="BZ22" s="1"/>
+      <c r="CA22" s="1"/>
+      <c r="CB22" s="1"/>
+      <c r="CC22" s="1"/>
+      <c r="CD22" s="1"/>
+      <c r="CE22" s="1"/>
+      <c r="CF22" s="1"/>
+      <c r="CG22" s="1"/>
+      <c r="CH22" s="1"/>
+      <c r="CI22" s="1"/>
+      <c r="CJ22" s="1"/>
+      <c r="CK22" s="1"/>
+      <c r="CL22" s="1"/>
+      <c r="CM22" s="1"/>
+      <c r="CN22" s="1"/>
+      <c r="CO22" s="1"/>
+      <c r="CP22" s="1"/>
+      <c r="CQ22" s="1"/>
+      <c r="CR22" s="1"/>
+      <c r="CS22" s="1"/>
+      <c r="CT22" s="1"/>
+      <c r="CU22" s="1"/>
+      <c r="CV22" s="1"/>
+      <c r="CW22" s="1"/>
+      <c r="CX22" s="1"/>
+      <c r="CY22" s="1"/>
+      <c r="CZ22" s="1"/>
+      <c r="DA22" s="1"/>
+      <c r="DB22" s="1"/>
+      <c r="DC22" s="1"/>
+      <c r="DD22" s="1"/>
+      <c r="DE22" s="1"/>
+      <c r="DF22" s="1"/>
+      <c r="DG22" s="1"/>
+      <c r="DH22" s="1"/>
+      <c r="DI22" s="1"/>
+      <c r="DJ22" s="1"/>
+      <c r="DK22" s="1"/>
+      <c r="DL22" s="1"/>
+      <c r="DM22" s="1"/>
+      <c r="DN22" s="1"/>
+      <c r="DO22" s="1"/>
+      <c r="DP22" s="1"/>
+      <c r="DQ22" s="1"/>
+      <c r="DR22" s="1"/>
+      <c r="DS22" s="1"/>
+      <c r="DT22" s="1"/>
+      <c r="DU22" s="1"/>
+      <c r="DV22" s="1"/>
+      <c r="DW22" s="1"/>
+      <c r="DX22" s="1"/>
+      <c r="DY22" s="1"/>
+      <c r="DZ22" s="1"/>
+      <c r="EA22" s="1"/>
+      <c r="EB22" s="1"/>
+      <c r="EC22" s="1"/>
+      <c r="ED22" s="1"/>
+      <c r="EE22" s="1"/>
+      <c r="EF22" s="1"/>
+      <c r="EG22" s="1"/>
+      <c r="EH22" s="1"/>
+      <c r="EI22" s="1"/>
+      <c r="EJ22" s="1"/>
+      <c r="EK22" s="1"/>
+      <c r="EL22" s="1"/>
+      <c r="EM22" s="1"/>
+      <c r="EN22" s="1"/>
+      <c r="EO22" s="1"/>
+      <c r="EP22" s="1"/>
+      <c r="EQ22" s="1"/>
+      <c r="ER22" s="1"/>
+      <c r="ES22" s="1"/>
+      <c r="ET22" s="1"/>
+      <c r="EU22" s="1"/>
+      <c r="EV22" s="1"/>
+      <c r="EW22" s="1"/>
+      <c r="EX22" s="1"/>
+      <c r="EY22" s="1"/>
+      <c r="EZ22" s="1"/>
+      <c r="FA22" s="1"/>
+      <c r="FB22" s="1"/>
+      <c r="FC22" s="1"/>
+      <c r="FD22" s="1"/>
+      <c r="FE22" s="1"/>
+      <c r="FF22" s="1"/>
+      <c r="FG22" s="1"/>
+      <c r="FH22" s="1"/>
+      <c r="FI22" s="1"/>
+      <c r="FJ22" s="1"/>
+      <c r="FK22" s="1"/>
+      <c r="FL22" s="1"/>
+      <c r="FM22" s="1"/>
+      <c r="FN22" s="1"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="1"/>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="1"/>
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="1"/>
+      <c r="AU23" s="1"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="1"/>
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="1"/>
+      <c r="BA23" s="1"/>
+      <c r="BB23" s="1"/>
+      <c r="BC23" s="1"/>
+      <c r="BD23" s="1"/>
+      <c r="BE23" s="1"/>
+      <c r="BF23" s="1"/>
+      <c r="BG23" s="1"/>
+      <c r="BH23" s="1"/>
+      <c r="BI23" s="1"/>
+      <c r="BJ23" s="1"/>
+      <c r="BK23" s="1"/>
+      <c r="BL23" s="1"/>
+      <c r="BM23" s="1"/>
+      <c r="BN23" s="1"/>
+      <c r="BO23" s="1"/>
+      <c r="BP23" s="1"/>
+      <c r="BQ23" s="1"/>
+      <c r="BR23" s="1"/>
+      <c r="BS23" s="1"/>
+      <c r="BT23" s="1"/>
+      <c r="BU23" s="1"/>
+      <c r="BV23" s="1"/>
+      <c r="BW23" s="1"/>
+      <c r="BX23" s="1"/>
+      <c r="BY23" s="1"/>
+      <c r="BZ23" s="1"/>
+      <c r="CA23" s="1"/>
+      <c r="CB23" s="1"/>
+      <c r="CC23" s="1"/>
+      <c r="CD23" s="1"/>
+      <c r="CE23" s="1"/>
+      <c r="CF23" s="1"/>
+      <c r="CG23" s="1"/>
+      <c r="CH23" s="1"/>
+      <c r="CI23" s="1"/>
+      <c r="CJ23" s="1"/>
+      <c r="CK23" s="1"/>
+      <c r="CL23" s="1"/>
+      <c r="CM23" s="1"/>
+      <c r="CN23" s="1"/>
+      <c r="CO23" s="1"/>
+      <c r="CP23" s="1"/>
+      <c r="CQ23" s="1"/>
+      <c r="CR23" s="1"/>
+      <c r="CS23" s="1"/>
+      <c r="CT23" s="1"/>
+      <c r="CU23" s="1"/>
+      <c r="CV23" s="1"/>
+      <c r="CW23" s="1"/>
+      <c r="CX23" s="1"/>
+      <c r="CY23" s="1"/>
+      <c r="CZ23" s="1"/>
+      <c r="DA23" s="1"/>
+      <c r="DB23" s="1"/>
+      <c r="DC23" s="1"/>
+      <c r="DD23" s="1"/>
+      <c r="DE23" s="1"/>
+      <c r="DF23" s="1"/>
+      <c r="DG23" s="1"/>
+      <c r="DH23" s="1"/>
+      <c r="DI23" s="1"/>
+      <c r="DJ23" s="1"/>
+      <c r="DK23" s="1"/>
+      <c r="DL23" s="1"/>
+      <c r="DM23" s="1"/>
+      <c r="DN23" s="1"/>
+      <c r="DO23" s="1"/>
+      <c r="DP23" s="1"/>
+      <c r="DQ23" s="1"/>
+      <c r="DR23" s="1"/>
+      <c r="DS23" s="1"/>
+      <c r="DT23" s="1"/>
+      <c r="DU23" s="1"/>
+      <c r="DV23" s="1"/>
+      <c r="DW23" s="1"/>
+      <c r="DX23" s="1"/>
+      <c r="DY23" s="1"/>
+      <c r="DZ23" s="1"/>
+      <c r="EA23" s="1"/>
+      <c r="EB23" s="1"/>
+      <c r="EC23" s="1"/>
+      <c r="ED23" s="1"/>
+      <c r="EE23" s="1"/>
+      <c r="EF23" s="1"/>
+      <c r="EG23" s="1"/>
+      <c r="EH23" s="1"/>
+      <c r="EI23" s="1"/>
+      <c r="EJ23" s="1"/>
+      <c r="EK23" s="1"/>
+      <c r="EL23" s="1"/>
+      <c r="EM23" s="1"/>
+      <c r="EN23" s="1"/>
+      <c r="EO23" s="1"/>
+      <c r="EP23" s="1"/>
+      <c r="EQ23" s="1"/>
+      <c r="ER23" s="1"/>
+      <c r="ES23" s="1"/>
+      <c r="ET23" s="1"/>
+      <c r="EU23" s="1"/>
+      <c r="EV23" s="1"/>
+      <c r="EW23" s="1"/>
+      <c r="EX23" s="1"/>
+      <c r="EY23" s="1"/>
+      <c r="EZ23" s="1"/>
+      <c r="FA23" s="1"/>
+      <c r="FB23" s="1"/>
+      <c r="FC23" s="1"/>
+      <c r="FD23" s="1"/>
+      <c r="FE23" s="1"/>
+      <c r="FF23" s="1"/>
+      <c r="FG23" s="1"/>
+      <c r="FH23" s="1"/>
+      <c r="FI23" s="1"/>
+      <c r="FJ23" s="1"/>
+      <c r="FK23" s="1"/>
+      <c r="FL23" s="1"/>
+      <c r="FM23" s="1"/>
+      <c r="FN23" s="1"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="1">
+        <v>32</v>
+      </c>
+      <c r="F24" s="1">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="1"/>
+      <c r="BB24" s="1"/>
+      <c r="BC24" s="1"/>
+      <c r="BD24" s="1"/>
+      <c r="BE24" s="1"/>
+      <c r="BF24" s="1"/>
+      <c r="BG24" s="1"/>
+      <c r="BH24" s="1"/>
+      <c r="BI24" s="1"/>
+      <c r="BJ24" s="1"/>
+      <c r="BK24" s="1"/>
+      <c r="BL24" s="1"/>
+      <c r="BM24" s="1"/>
+      <c r="BN24" s="1"/>
+      <c r="BO24" s="1"/>
+      <c r="BP24" s="1"/>
+      <c r="BQ24" s="1"/>
+      <c r="BR24" s="1"/>
+      <c r="BS24" s="1"/>
+      <c r="BT24" s="1"/>
+      <c r="BU24" s="1"/>
+      <c r="BV24" s="1"/>
+      <c r="BW24" s="1"/>
+      <c r="BX24" s="1"/>
+      <c r="BY24" s="1"/>
+      <c r="BZ24" s="1"/>
+      <c r="CA24" s="1"/>
+      <c r="CB24" s="1"/>
+      <c r="CC24" s="1"/>
+      <c r="CD24" s="1"/>
+      <c r="CE24" s="1"/>
+      <c r="CF24" s="1"/>
+      <c r="CG24" s="1"/>
+      <c r="CH24" s="1"/>
+      <c r="CI24" s="1"/>
+      <c r="CJ24" s="1"/>
+      <c r="CK24" s="1"/>
+      <c r="CL24" s="1"/>
+      <c r="CM24" s="1"/>
+      <c r="CN24" s="1"/>
+      <c r="CO24" s="1"/>
+      <c r="CP24" s="1"/>
+      <c r="CQ24" s="1"/>
+      <c r="CR24" s="1"/>
+      <c r="CS24" s="1"/>
+      <c r="CT24" s="1"/>
+      <c r="CU24" s="1"/>
+      <c r="CV24" s="1"/>
+      <c r="CW24" s="1"/>
+      <c r="CX24" s="1"/>
+      <c r="CY24" s="1"/>
+      <c r="CZ24" s="1"/>
+      <c r="DA24" s="1"/>
+      <c r="DB24" s="1"/>
+      <c r="DC24" s="1"/>
+      <c r="DD24" s="1"/>
+      <c r="DE24" s="1"/>
+      <c r="DF24" s="1"/>
+      <c r="DG24" s="1"/>
+      <c r="DH24" s="1"/>
+      <c r="DI24" s="1"/>
+      <c r="DJ24" s="1"/>
+      <c r="DK24" s="1"/>
+      <c r="DL24" s="1"/>
+      <c r="DM24" s="1"/>
+      <c r="DN24" s="1"/>
+      <c r="DO24" s="1"/>
+      <c r="DP24" s="1"/>
+      <c r="DQ24" s="1"/>
+      <c r="DR24" s="1"/>
+      <c r="DS24" s="1"/>
+      <c r="DT24" s="1"/>
+      <c r="DU24" s="1"/>
+      <c r="DV24" s="1"/>
+      <c r="DW24" s="1"/>
+      <c r="DX24" s="1"/>
+      <c r="DY24" s="1"/>
+      <c r="DZ24" s="1"/>
+      <c r="EA24" s="1"/>
+      <c r="EB24" s="1"/>
+      <c r="EC24" s="1"/>
+      <c r="ED24" s="1"/>
+      <c r="EE24" s="1"/>
+      <c r="EF24" s="1"/>
+      <c r="EG24" s="1"/>
+      <c r="EH24" s="1"/>
+      <c r="EI24" s="1"/>
+      <c r="EJ24" s="1"/>
+      <c r="EK24" s="1"/>
+      <c r="EL24" s="1"/>
+      <c r="EM24" s="1"/>
+      <c r="EN24" s="1"/>
+      <c r="EO24" s="1"/>
+      <c r="EP24" s="1"/>
+      <c r="EQ24" s="1"/>
+      <c r="ER24" s="1"/>
+      <c r="ES24" s="1"/>
+      <c r="ET24" s="1"/>
+      <c r="EU24" s="1"/>
+      <c r="EV24" s="1"/>
+      <c r="EW24" s="1"/>
+      <c r="EX24" s="1"/>
+      <c r="EY24" s="1"/>
+      <c r="EZ24" s="1"/>
+      <c r="FA24" s="1"/>
+      <c r="FB24" s="1"/>
+      <c r="FC24" s="1"/>
+      <c r="FD24" s="1"/>
+      <c r="FE24" s="1"/>
+      <c r="FF24" s="1"/>
+      <c r="FG24" s="1"/>
+      <c r="FH24" s="1"/>
+      <c r="FI24" s="1"/>
+      <c r="FJ24" s="1"/>
+      <c r="FK24" s="1"/>
+      <c r="FL24" s="1"/>
+      <c r="FM24" s="1"/>
+      <c r="FN24" s="1"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="1">
+        <v>32</v>
+      </c>
+      <c r="F25" s="1">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="1"/>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1"/>
+      <c r="BA25" s="1"/>
+      <c r="BB25" s="1"/>
+      <c r="BC25" s="1"/>
+      <c r="BD25" s="1"/>
+      <c r="BE25" s="1"/>
+      <c r="BF25" s="1"/>
+      <c r="BG25" s="1"/>
+      <c r="BH25" s="1"/>
+      <c r="BI25" s="1"/>
+      <c r="BJ25" s="1"/>
+      <c r="BK25" s="1"/>
+      <c r="BL25" s="1"/>
+      <c r="BM25" s="1"/>
+      <c r="BN25" s="1"/>
+      <c r="BO25" s="1"/>
+      <c r="BP25" s="1"/>
+      <c r="BQ25" s="1"/>
+      <c r="BR25" s="1"/>
+      <c r="BS25" s="1"/>
+      <c r="BT25" s="1"/>
+      <c r="BU25" s="1"/>
+      <c r="BV25" s="1"/>
+      <c r="BW25" s="1"/>
+      <c r="BX25" s="1"/>
+      <c r="BY25" s="1"/>
+      <c r="BZ25" s="1"/>
+      <c r="CA25" s="1"/>
+      <c r="CB25" s="1"/>
+      <c r="CC25" s="1"/>
+      <c r="CD25" s="1"/>
+      <c r="CE25" s="1"/>
+      <c r="CF25" s="1"/>
+      <c r="CG25" s="1"/>
+      <c r="CH25" s="1"/>
+      <c r="CI25" s="1"/>
+      <c r="CJ25" s="1"/>
+      <c r="CK25" s="1"/>
+      <c r="CL25" s="1"/>
+      <c r="CM25" s="1"/>
+      <c r="CN25" s="1"/>
+      <c r="CO25" s="1"/>
+      <c r="CP25" s="1"/>
+      <c r="CQ25" s="1"/>
+      <c r="CR25" s="1"/>
+      <c r="CS25" s="1"/>
+      <c r="CT25" s="1"/>
+      <c r="CU25" s="1"/>
+      <c r="CV25" s="1"/>
+      <c r="CW25" s="1"/>
+      <c r="CX25" s="1"/>
+      <c r="CY25" s="1"/>
+      <c r="CZ25" s="1"/>
+      <c r="DA25" s="1"/>
+      <c r="DB25" s="1"/>
+      <c r="DC25" s="1"/>
+      <c r="DD25" s="1"/>
+      <c r="DE25" s="1"/>
+      <c r="DF25" s="1"/>
+      <c r="DG25" s="1"/>
+      <c r="DH25" s="1"/>
+      <c r="DI25" s="1"/>
+      <c r="DJ25" s="1"/>
+      <c r="DK25" s="1"/>
+      <c r="DL25" s="1"/>
+      <c r="DM25" s="1"/>
+      <c r="DN25" s="1"/>
+      <c r="DO25" s="1"/>
+      <c r="DP25" s="1"/>
+      <c r="DQ25" s="1"/>
+      <c r="DR25" s="1"/>
+      <c r="DS25" s="1"/>
+      <c r="DT25" s="1"/>
+      <c r="DU25" s="1"/>
+      <c r="DV25" s="1"/>
+      <c r="DW25" s="1"/>
+      <c r="DX25" s="1"/>
+      <c r="DY25" s="1"/>
+      <c r="DZ25" s="1"/>
+      <c r="EA25" s="1"/>
+      <c r="EB25" s="1"/>
+      <c r="EC25" s="1"/>
+      <c r="ED25" s="1"/>
+      <c r="EE25" s="1"/>
+      <c r="EF25" s="1"/>
+      <c r="EG25" s="1"/>
+      <c r="EH25" s="1"/>
+      <c r="EI25" s="1"/>
+      <c r="EJ25" s="1"/>
+      <c r="EK25" s="1"/>
+      <c r="EL25" s="1"/>
+      <c r="EM25" s="1"/>
+      <c r="EN25" s="1"/>
+      <c r="EO25" s="1"/>
+      <c r="EP25" s="1"/>
+      <c r="EQ25" s="1"/>
+      <c r="ER25" s="1"/>
+      <c r="ES25" s="1"/>
+      <c r="ET25" s="1"/>
+      <c r="EU25" s="1"/>
+      <c r="EV25" s="1"/>
+      <c r="EW25" s="1"/>
+      <c r="EX25" s="1"/>
+      <c r="EY25" s="1"/>
+      <c r="EZ25" s="1"/>
+      <c r="FA25" s="1"/>
+      <c r="FB25" s="1"/>
+      <c r="FC25" s="1"/>
+      <c r="FD25" s="1"/>
+      <c r="FE25" s="1"/>
+      <c r="FF25" s="1"/>
+      <c r="FG25" s="1"/>
+      <c r="FH25" s="1"/>
+      <c r="FI25" s="1"/>
+      <c r="FJ25" s="1"/>
+      <c r="FK25" s="1"/>
+      <c r="FL25" s="1"/>
+      <c r="FM25" s="1"/>
+      <c r="FN25" s="1"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="1">
+        <v>50</v>
+      </c>
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="1"/>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+      <c r="AV26" s="1"/>
+      <c r="AW26" s="1"/>
+      <c r="AX26" s="1"/>
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="1"/>
+      <c r="BA26" s="1"/>
+      <c r="BB26" s="1"/>
+      <c r="BC26" s="1"/>
+      <c r="BD26" s="1"/>
+      <c r="BE26" s="1"/>
+      <c r="BF26" s="1"/>
+      <c r="BG26" s="1"/>
+      <c r="BH26" s="1"/>
+      <c r="BI26" s="1"/>
+      <c r="BJ26" s="1"/>
+      <c r="BK26" s="1"/>
+      <c r="BL26" s="1"/>
+      <c r="BM26" s="1"/>
+      <c r="BN26" s="1"/>
+      <c r="BO26" s="1"/>
+      <c r="BP26" s="1"/>
+      <c r="BQ26" s="1"/>
+      <c r="BR26" s="1"/>
+      <c r="BS26" s="1"/>
+      <c r="BT26" s="1"/>
+      <c r="BU26" s="1"/>
+      <c r="BV26" s="1"/>
+      <c r="BW26" s="1"/>
+      <c r="BX26" s="1"/>
+      <c r="BY26" s="1"/>
+      <c r="BZ26" s="1"/>
+      <c r="CA26" s="1"/>
+      <c r="CB26" s="1"/>
+      <c r="CC26" s="1"/>
+      <c r="CD26" s="1"/>
+      <c r="CE26" s="1"/>
+      <c r="CF26" s="1"/>
+      <c r="CG26" s="1"/>
+      <c r="CH26" s="1"/>
+      <c r="CI26" s="1"/>
+      <c r="CJ26" s="1"/>
+      <c r="CK26" s="1"/>
+      <c r="CL26" s="1"/>
+      <c r="CM26" s="1"/>
+      <c r="CN26" s="1"/>
+      <c r="CO26" s="1"/>
+      <c r="CP26" s="1"/>
+      <c r="CQ26" s="1"/>
+      <c r="CR26" s="1"/>
+      <c r="CS26" s="1"/>
+      <c r="CT26" s="1"/>
+      <c r="CU26" s="1"/>
+      <c r="CV26" s="1"/>
+      <c r="CW26" s="1"/>
+      <c r="CX26" s="1"/>
+      <c r="CY26" s="1"/>
+      <c r="CZ26" s="1"/>
+      <c r="DA26" s="1"/>
+      <c r="DB26" s="1"/>
+      <c r="DC26" s="1"/>
+      <c r="DD26" s="1"/>
+      <c r="DE26" s="1"/>
+      <c r="DF26" s="1"/>
+      <c r="DG26" s="1"/>
+      <c r="DH26" s="1"/>
+      <c r="DI26" s="1"/>
+      <c r="DJ26" s="1"/>
+      <c r="DK26" s="1"/>
+      <c r="DL26" s="1"/>
+      <c r="DM26" s="1"/>
+      <c r="DN26" s="1"/>
+      <c r="DO26" s="1"/>
+      <c r="DP26" s="1"/>
+      <c r="DQ26" s="1"/>
+      <c r="DR26" s="1"/>
+      <c r="DS26" s="1"/>
+      <c r="DT26" s="1"/>
+      <c r="DU26" s="1"/>
+      <c r="DV26" s="1"/>
+      <c r="DW26" s="1"/>
+      <c r="DX26" s="1"/>
+      <c r="DY26" s="1"/>
+      <c r="DZ26" s="1"/>
+      <c r="EA26" s="1"/>
+      <c r="EB26" s="1"/>
+      <c r="EC26" s="1"/>
+      <c r="ED26" s="1"/>
+      <c r="EE26" s="1"/>
+      <c r="EF26" s="1"/>
+      <c r="EG26" s="1"/>
+      <c r="EH26" s="1"/>
+      <c r="EI26" s="1"/>
+      <c r="EJ26" s="1"/>
+      <c r="EK26" s="1"/>
+      <c r="EL26" s="1"/>
+      <c r="EM26" s="1"/>
+      <c r="EN26" s="1"/>
+      <c r="EO26" s="1"/>
+      <c r="EP26" s="1"/>
+      <c r="EQ26" s="1"/>
+      <c r="ER26" s="1"/>
+      <c r="ES26" s="1"/>
+      <c r="ET26" s="1"/>
+      <c r="EU26" s="1"/>
+      <c r="EV26" s="1"/>
+      <c r="EW26" s="1"/>
+      <c r="EX26" s="1"/>
+      <c r="EY26" s="1"/>
+      <c r="EZ26" s="1"/>
+      <c r="FA26" s="1"/>
+      <c r="FB26" s="1"/>
+      <c r="FC26" s="1"/>
+      <c r="FD26" s="1"/>
+      <c r="FE26" s="1"/>
+      <c r="FF26" s="1"/>
+      <c r="FG26" s="1"/>
+      <c r="FH26" s="1"/>
+      <c r="FI26" s="1"/>
+      <c r="FJ26" s="1"/>
+      <c r="FK26" s="1"/>
+      <c r="FL26" s="1"/>
+      <c r="FM26" s="1"/>
+      <c r="FN26" s="1"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="1">
+        <v>50</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="1"/>
+      <c r="BA27" s="1"/>
+      <c r="BB27" s="1"/>
+      <c r="BC27" s="1"/>
+      <c r="BD27" s="1"/>
+      <c r="BE27" s="1"/>
+      <c r="BF27" s="1"/>
+      <c r="BG27" s="1"/>
+      <c r="BH27" s="1"/>
+      <c r="BI27" s="1"/>
+      <c r="BJ27" s="1"/>
+      <c r="BK27" s="1"/>
+      <c r="BL27" s="1"/>
+      <c r="BM27" s="1"/>
+      <c r="BN27" s="1"/>
+      <c r="BO27" s="1"/>
+      <c r="BP27" s="1"/>
+      <c r="BQ27" s="1"/>
+      <c r="BR27" s="1"/>
+      <c r="BS27" s="1"/>
+      <c r="BT27" s="1"/>
+      <c r="BU27" s="1"/>
+      <c r="BV27" s="1"/>
+      <c r="BW27" s="1"/>
+      <c r="BX27" s="1"/>
+      <c r="BY27" s="1"/>
+      <c r="BZ27" s="1"/>
+      <c r="CA27" s="1"/>
+      <c r="CB27" s="1"/>
+      <c r="CC27" s="1"/>
+      <c r="CD27" s="1"/>
+      <c r="CE27" s="1"/>
+      <c r="CF27" s="1"/>
+      <c r="CG27" s="1"/>
+      <c r="CH27" s="1"/>
+      <c r="CI27" s="1"/>
+      <c r="CJ27" s="1"/>
+      <c r="CK27" s="1"/>
+      <c r="CL27" s="1"/>
+      <c r="CM27" s="1"/>
+      <c r="CN27" s="1"/>
+      <c r="CO27" s="1"/>
+      <c r="CP27" s="1"/>
+      <c r="CQ27" s="1"/>
+      <c r="CR27" s="1"/>
+      <c r="CS27" s="1"/>
+      <c r="CT27" s="1"/>
+      <c r="CU27" s="1"/>
+      <c r="CV27" s="1"/>
+      <c r="CW27" s="1"/>
+      <c r="CX27" s="1"/>
+      <c r="CY27" s="1"/>
+      <c r="CZ27" s="1"/>
+      <c r="DA27" s="1"/>
+      <c r="DB27" s="1"/>
+      <c r="DC27" s="1"/>
+      <c r="DD27" s="1"/>
+      <c r="DE27" s="1"/>
+      <c r="DF27" s="1"/>
+      <c r="DG27" s="1"/>
+      <c r="DH27" s="1"/>
+      <c r="DI27" s="1"/>
+      <c r="DJ27" s="1"/>
+      <c r="DK27" s="1"/>
+      <c r="DL27" s="1"/>
+      <c r="DM27" s="1"/>
+      <c r="DN27" s="1"/>
+      <c r="DO27" s="1"/>
+      <c r="DP27" s="1"/>
+      <c r="DQ27" s="1"/>
+      <c r="DR27" s="1"/>
+      <c r="DS27" s="1"/>
+      <c r="DT27" s="1"/>
+      <c r="DU27" s="1"/>
+      <c r="DV27" s="1"/>
+      <c r="DW27" s="1"/>
+      <c r="DX27" s="1"/>
+      <c r="DY27" s="1"/>
+      <c r="DZ27" s="1"/>
+      <c r="EA27" s="1"/>
+      <c r="EB27" s="1"/>
+      <c r="EC27" s="1"/>
+      <c r="ED27" s="1"/>
+      <c r="EE27" s="1"/>
+      <c r="EF27" s="1"/>
+      <c r="EG27" s="1"/>
+      <c r="EH27" s="1"/>
+      <c r="EI27" s="1"/>
+      <c r="EJ27" s="1"/>
+      <c r="EK27" s="1"/>
+      <c r="EL27" s="1"/>
+      <c r="EM27" s="1"/>
+      <c r="EN27" s="1"/>
+      <c r="EO27" s="1"/>
+      <c r="EP27" s="1"/>
+      <c r="EQ27" s="1"/>
+      <c r="ER27" s="1"/>
+      <c r="ES27" s="1"/>
+      <c r="ET27" s="1"/>
+      <c r="EU27" s="1"/>
+      <c r="EV27" s="1"/>
+      <c r="EW27" s="1"/>
+      <c r="EX27" s="1"/>
+      <c r="EY27" s="1"/>
+      <c r="EZ27" s="1"/>
+      <c r="FA27" s="1"/>
+      <c r="FB27" s="1"/>
+      <c r="FC27" s="1"/>
+      <c r="FD27" s="1"/>
+      <c r="FE27" s="1"/>
+      <c r="FF27" s="1"/>
+      <c r="FG27" s="1"/>
+      <c r="FH27" s="1"/>
+      <c r="FI27" s="1"/>
+      <c r="FJ27" s="1"/>
+      <c r="FK27" s="1"/>
+      <c r="FL27" s="1"/>
+      <c r="FM27" s="1"/>
+      <c r="FN27" s="1"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1">
+        <v>50</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="1"/>
+      <c r="BC28" s="1"/>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+      <c r="BI28" s="1"/>
+      <c r="BJ28" s="1"/>
+      <c r="BK28" s="1"/>
+      <c r="BL28" s="1"/>
+      <c r="BM28" s="1"/>
+      <c r="BN28" s="1"/>
+      <c r="BO28" s="1"/>
+      <c r="BP28" s="1"/>
+      <c r="BQ28" s="1"/>
+      <c r="BR28" s="1"/>
+      <c r="BS28" s="1"/>
+      <c r="BT28" s="1"/>
+      <c r="BU28" s="1"/>
+      <c r="BV28" s="1"/>
+      <c r="BW28" s="1"/>
+      <c r="BX28" s="1"/>
+      <c r="BY28" s="1"/>
+      <c r="BZ28" s="1"/>
+      <c r="CA28" s="1"/>
+      <c r="CB28" s="1"/>
+      <c r="CC28" s="1"/>
+      <c r="CD28" s="1"/>
+      <c r="CE28" s="1"/>
+      <c r="CF28" s="1"/>
+      <c r="CG28" s="1"/>
+      <c r="CH28" s="1"/>
+      <c r="CI28" s="1"/>
+      <c r="CJ28" s="1"/>
+      <c r="CK28" s="1"/>
+      <c r="CL28" s="1"/>
+      <c r="CM28" s="1"/>
+      <c r="CN28" s="1"/>
+      <c r="CO28" s="1"/>
+      <c r="CP28" s="1"/>
+      <c r="CQ28" s="1"/>
+      <c r="CR28" s="1"/>
+      <c r="CS28" s="1"/>
+      <c r="CT28" s="1"/>
+      <c r="CU28" s="1"/>
+      <c r="CV28" s="1"/>
+      <c r="CW28" s="1"/>
+      <c r="CX28" s="1"/>
+      <c r="CY28" s="1"/>
+      <c r="CZ28" s="1"/>
+      <c r="DA28" s="1"/>
+      <c r="DB28" s="1"/>
+      <c r="DC28" s="1"/>
+      <c r="DD28" s="1"/>
+      <c r="DE28" s="1"/>
+      <c r="DF28" s="1"/>
+      <c r="DG28" s="1"/>
+      <c r="DH28" s="1"/>
+      <c r="DI28" s="1"/>
+      <c r="DJ28" s="1"/>
+      <c r="DK28" s="1"/>
+      <c r="DL28" s="1"/>
+      <c r="DM28" s="1"/>
+      <c r="DN28" s="1"/>
+      <c r="DO28" s="1"/>
+      <c r="DP28" s="1"/>
+      <c r="DQ28" s="1"/>
+      <c r="DR28" s="1"/>
+      <c r="DS28" s="1"/>
+      <c r="DT28" s="1"/>
+      <c r="DU28" s="1"/>
+      <c r="DV28" s="1"/>
+      <c r="DW28" s="1"/>
+      <c r="DX28" s="1"/>
+      <c r="DY28" s="1"/>
+      <c r="DZ28" s="1"/>
+      <c r="EA28" s="1"/>
+      <c r="EB28" s="1"/>
+      <c r="EC28" s="1"/>
+      <c r="ED28" s="1"/>
+      <c r="EE28" s="1"/>
+      <c r="EF28" s="1"/>
+      <c r="EG28" s="1"/>
+      <c r="EH28" s="1"/>
+      <c r="EI28" s="1"/>
+      <c r="EJ28" s="1"/>
+      <c r="EK28" s="1"/>
+      <c r="EL28" s="1"/>
+      <c r="EM28" s="1"/>
+      <c r="EN28" s="1"/>
+      <c r="EO28" s="1"/>
+      <c r="EP28" s="1"/>
+      <c r="EQ28" s="1"/>
+      <c r="ER28" s="1"/>
+      <c r="ES28" s="1"/>
+      <c r="ET28" s="1"/>
+      <c r="EU28" s="1"/>
+      <c r="EV28" s="1"/>
+      <c r="EW28" s="1"/>
+      <c r="EX28" s="1"/>
+      <c r="EY28" s="1"/>
+      <c r="EZ28" s="1"/>
+      <c r="FA28" s="1"/>
+      <c r="FB28" s="1"/>
+      <c r="FC28" s="1"/>
+      <c r="FD28" s="1"/>
+      <c r="FE28" s="1"/>
+      <c r="FF28" s="1"/>
+      <c r="FG28" s="1"/>
+      <c r="FH28" s="1"/>
+      <c r="FI28" s="1"/>
+      <c r="FJ28" s="1"/>
+      <c r="FK28" s="1"/>
+      <c r="FL28" s="1"/>
+      <c r="FM28" s="1"/>
+      <c r="FN28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="1">
+        <v>50</v>
+      </c>
+      <c r="F29" s="1">
+        <v>5</v>
+      </c>
+      <c r="G29" s="1">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="1"/>
+      <c r="AR29" s="1"/>
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="1"/>
+      <c r="AY29" s="1"/>
+      <c r="AZ29" s="1"/>
+      <c r="BA29" s="1"/>
+      <c r="BB29" s="1"/>
+      <c r="BC29" s="1"/>
+      <c r="BD29" s="1"/>
+      <c r="BE29" s="1"/>
+      <c r="BF29" s="1"/>
+      <c r="BG29" s="1"/>
+      <c r="BH29" s="1"/>
+      <c r="BI29" s="1"/>
+      <c r="BJ29" s="1"/>
+      <c r="BK29" s="1"/>
+      <c r="BL29" s="1"/>
+      <c r="BM29" s="1"/>
+      <c r="BN29" s="1"/>
+      <c r="BO29" s="1"/>
+      <c r="BP29" s="1"/>
+      <c r="BQ29" s="1"/>
+      <c r="BR29" s="1"/>
+      <c r="BS29" s="1"/>
+      <c r="BT29" s="1"/>
+      <c r="BU29" s="1"/>
+      <c r="BV29" s="1"/>
+      <c r="BW29" s="1"/>
+      <c r="BX29" s="1"/>
+      <c r="BY29" s="1"/>
+      <c r="BZ29" s="1"/>
+      <c r="CA29" s="1"/>
+      <c r="CB29" s="1"/>
+      <c r="CC29" s="1"/>
+      <c r="CD29" s="1"/>
+      <c r="CE29" s="1"/>
+      <c r="CF29" s="1"/>
+      <c r="CG29" s="1"/>
+      <c r="CH29" s="1"/>
+      <c r="CI29" s="1"/>
+      <c r="CJ29" s="1"/>
+      <c r="CK29" s="1"/>
+      <c r="CL29" s="1"/>
+      <c r="CM29" s="1"/>
+      <c r="CN29" s="1"/>
+      <c r="CO29" s="1"/>
+      <c r="CP29" s="1"/>
+      <c r="CQ29" s="1"/>
+      <c r="CR29" s="1"/>
+      <c r="CS29" s="1"/>
+      <c r="CT29" s="1"/>
+      <c r="CU29" s="1"/>
+      <c r="CV29" s="1"/>
+      <c r="CW29" s="1"/>
+      <c r="CX29" s="1"/>
+      <c r="CY29" s="1"/>
+      <c r="CZ29" s="1"/>
+      <c r="DA29" s="1"/>
+      <c r="DB29" s="1"/>
+      <c r="DC29" s="1"/>
+      <c r="DD29" s="1"/>
+      <c r="DE29" s="1"/>
+      <c r="DF29" s="1"/>
+      <c r="DG29" s="1"/>
+      <c r="DH29" s="1"/>
+      <c r="DI29" s="1"/>
+      <c r="DJ29" s="1"/>
+      <c r="DK29" s="1"/>
+      <c r="DL29" s="1"/>
+      <c r="DM29" s="1"/>
+      <c r="DN29" s="1"/>
+      <c r="DO29" s="1"/>
+      <c r="DP29" s="1"/>
+      <c r="DQ29" s="1"/>
+      <c r="DR29" s="1"/>
+      <c r="DS29" s="1"/>
+      <c r="DT29" s="1"/>
+      <c r="DU29" s="1"/>
+      <c r="DV29" s="1"/>
+      <c r="DW29" s="1"/>
+      <c r="DX29" s="1"/>
+      <c r="DY29" s="1"/>
+      <c r="DZ29" s="1"/>
+      <c r="EA29" s="1"/>
+      <c r="EB29" s="1"/>
+      <c r="EC29" s="1"/>
+      <c r="ED29" s="1"/>
+      <c r="EE29" s="1"/>
+      <c r="EF29" s="1"/>
+      <c r="EG29" s="1"/>
+      <c r="EH29" s="1"/>
+      <c r="EI29" s="1"/>
+      <c r="EJ29" s="1"/>
+      <c r="EK29" s="1"/>
+      <c r="EL29" s="1"/>
+      <c r="EM29" s="1"/>
+      <c r="EN29" s="1"/>
+      <c r="EO29" s="1"/>
+      <c r="EP29" s="1"/>
+      <c r="EQ29" s="1"/>
+      <c r="ER29" s="1"/>
+      <c r="ES29" s="1"/>
+      <c r="ET29" s="1"/>
+      <c r="EU29" s="1"/>
+      <c r="EV29" s="1"/>
+      <c r="EW29" s="1"/>
+      <c r="EX29" s="1"/>
+      <c r="EY29" s="1"/>
+      <c r="EZ29" s="1"/>
+      <c r="FA29" s="1"/>
+      <c r="FB29" s="1"/>
+      <c r="FC29" s="1"/>
+      <c r="FD29" s="1"/>
+      <c r="FE29" s="1"/>
+      <c r="FF29" s="1"/>
+      <c r="FG29" s="1"/>
+      <c r="FH29" s="1"/>
+      <c r="FI29" s="1"/>
+      <c r="FJ29" s="1"/>
+      <c r="FK29" s="1"/>
+      <c r="FL29" s="1"/>
+      <c r="FM29" s="1"/>
+      <c r="FN29" s="1"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="1">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="1"/>
+      <c r="AP30" s="1"/>
+      <c r="AQ30" s="1"/>
+      <c r="AR30" s="1"/>
+      <c r="AS30" s="1"/>
+      <c r="AT30" s="1"/>
+      <c r="AU30" s="1"/>
+      <c r="AV30" s="1"/>
+      <c r="AW30" s="1"/>
+      <c r="AX30" s="1"/>
+      <c r="AY30" s="1"/>
+      <c r="AZ30" s="1"/>
+      <c r="BA30" s="1"/>
+      <c r="BB30" s="1"/>
+      <c r="BC30" s="1"/>
+      <c r="BD30" s="1"/>
+      <c r="BE30" s="1"/>
+      <c r="BF30" s="1"/>
+      <c r="BG30" s="1"/>
+      <c r="BH30" s="1"/>
+      <c r="BI30" s="1"/>
+      <c r="BJ30" s="1"/>
+      <c r="BK30" s="1"/>
+      <c r="BL30" s="1"/>
+      <c r="BM30" s="1"/>
+      <c r="BN30" s="1"/>
+      <c r="BO30" s="1"/>
+      <c r="BP30" s="1"/>
+      <c r="BQ30" s="1"/>
+      <c r="BR30" s="1"/>
+      <c r="BS30" s="1"/>
+      <c r="BT30" s="1"/>
+      <c r="BU30" s="1"/>
+      <c r="BV30" s="1"/>
+      <c r="BW30" s="1"/>
+      <c r="BX30" s="1"/>
+      <c r="BY30" s="1"/>
+      <c r="BZ30" s="1"/>
+      <c r="CA30" s="1"/>
+      <c r="CB30" s="1"/>
+      <c r="CC30" s="1"/>
+      <c r="CD30" s="1"/>
+      <c r="CE30" s="1"/>
+      <c r="CF30" s="1"/>
+      <c r="CG30" s="1"/>
+      <c r="CH30" s="1"/>
+      <c r="CI30" s="1"/>
+      <c r="CJ30" s="1"/>
+      <c r="CK30" s="1"/>
+      <c r="CL30" s="1"/>
+      <c r="CM30" s="1"/>
+      <c r="CN30" s="1"/>
+      <c r="CO30" s="1"/>
+      <c r="CP30" s="1"/>
+      <c r="CQ30" s="1"/>
+      <c r="CR30" s="1"/>
+      <c r="CS30" s="1"/>
+      <c r="CT30" s="1"/>
+      <c r="CU30" s="1"/>
+      <c r="CV30" s="1"/>
+      <c r="CW30" s="1"/>
+      <c r="CX30" s="1"/>
+      <c r="CY30" s="1"/>
+      <c r="CZ30" s="1"/>
+      <c r="DA30" s="1"/>
+      <c r="DB30" s="1"/>
+      <c r="DC30" s="1"/>
+      <c r="DD30" s="1"/>
+      <c r="DE30" s="1"/>
+      <c r="DF30" s="1"/>
+      <c r="DG30" s="1"/>
+      <c r="DH30" s="1"/>
+      <c r="DI30" s="1"/>
+      <c r="DJ30" s="1"/>
+      <c r="DK30" s="1"/>
+      <c r="DL30" s="1"/>
+      <c r="DM30" s="1"/>
+      <c r="DN30" s="1"/>
+      <c r="DO30" s="1"/>
+      <c r="DP30" s="1"/>
+      <c r="DQ30" s="1"/>
+      <c r="DR30" s="1"/>
+      <c r="DS30" s="1"/>
+      <c r="DT30" s="1"/>
+      <c r="DU30" s="1"/>
+      <c r="DV30" s="1"/>
+      <c r="DW30" s="1"/>
+      <c r="DX30" s="1"/>
+      <c r="DY30" s="1"/>
+      <c r="DZ30" s="1"/>
+      <c r="EA30" s="1"/>
+      <c r="EB30" s="1"/>
+      <c r="EC30" s="1"/>
+      <c r="ED30" s="1"/>
+      <c r="EE30" s="1"/>
+      <c r="EF30" s="1"/>
+      <c r="EG30" s="1"/>
+      <c r="EH30" s="1"/>
+      <c r="EI30" s="1"/>
+      <c r="EJ30" s="1"/>
+      <c r="EK30" s="1"/>
+      <c r="EL30" s="1"/>
+      <c r="EM30" s="1"/>
+      <c r="EN30" s="1"/>
+      <c r="EO30" s="1"/>
+      <c r="EP30" s="1"/>
+      <c r="EQ30" s="1"/>
+      <c r="ER30" s="1"/>
+      <c r="ES30" s="1"/>
+      <c r="ET30" s="1"/>
+      <c r="EU30" s="1"/>
+      <c r="EV30" s="1"/>
+      <c r="EW30" s="1"/>
+      <c r="EX30" s="1"/>
+      <c r="EY30" s="1"/>
+      <c r="EZ30" s="1"/>
+      <c r="FA30" s="1"/>
+      <c r="FB30" s="1"/>
+      <c r="FC30" s="1"/>
+      <c r="FD30" s="1"/>
+      <c r="FE30" s="1"/>
+      <c r="FF30" s="1"/>
+      <c r="FG30" s="1"/>
+      <c r="FH30" s="1"/>
+      <c r="FI30" s="1"/>
+      <c r="FJ30" s="1"/>
+      <c r="FK30" s="1"/>
+      <c r="FL30" s="1"/>
+      <c r="FM30" s="1"/>
+      <c r="FN30" s="1"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="1">
+        <v>50</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1"/>
+      <c r="AQ31" s="1"/>
+      <c r="AR31" s="1"/>
+      <c r="AS31" s="1"/>
+      <c r="AT31" s="1"/>
+      <c r="AU31" s="1"/>
+      <c r="AV31" s="1"/>
+      <c r="AW31" s="1"/>
+      <c r="AX31" s="1"/>
+      <c r="AY31" s="1"/>
+      <c r="AZ31" s="1"/>
+      <c r="BA31" s="1"/>
+      <c r="BB31" s="1"/>
+      <c r="BC31" s="1"/>
+      <c r="BD31" s="1"/>
+      <c r="BE31" s="1"/>
+      <c r="BF31" s="1"/>
+      <c r="BG31" s="1"/>
+      <c r="BH31" s="1"/>
+      <c r="BI31" s="1"/>
+      <c r="BJ31" s="1"/>
+      <c r="BK31" s="1"/>
+      <c r="BL31" s="1"/>
+      <c r="BM31" s="1"/>
+      <c r="BN31" s="1"/>
+      <c r="BO31" s="1"/>
+      <c r="BP31" s="1"/>
+      <c r="BQ31" s="1"/>
+      <c r="BR31" s="1"/>
+      <c r="BS31" s="1"/>
+      <c r="BT31" s="1"/>
+      <c r="BU31" s="1"/>
+      <c r="BV31" s="1"/>
+      <c r="BW31" s="1"/>
+      <c r="BX31" s="1"/>
+      <c r="BY31" s="1"/>
+      <c r="BZ31" s="1"/>
+      <c r="CA31" s="1"/>
+      <c r="CB31" s="1"/>
+      <c r="CC31" s="1"/>
+      <c r="CD31" s="1"/>
+      <c r="CE31" s="1"/>
+      <c r="CF31" s="1"/>
+      <c r="CG31" s="1"/>
+      <c r="CH31" s="1"/>
+      <c r="CI31" s="1"/>
+      <c r="CJ31" s="1"/>
+      <c r="CK31" s="1"/>
+      <c r="CL31" s="1"/>
+      <c r="CM31" s="1"/>
+      <c r="CN31" s="1"/>
+      <c r="CO31" s="1"/>
+      <c r="CP31" s="1"/>
+      <c r="CQ31" s="1"/>
+      <c r="CR31" s="1"/>
+      <c r="CS31" s="1"/>
+      <c r="CT31" s="1"/>
+      <c r="CU31" s="1"/>
+      <c r="CV31" s="1"/>
+      <c r="CW31" s="1"/>
+      <c r="CX31" s="1"/>
+      <c r="CY31" s="1"/>
+      <c r="CZ31" s="1"/>
+      <c r="DA31" s="1"/>
+      <c r="DB31" s="1"/>
+      <c r="DC31" s="1"/>
+      <c r="DD31" s="1"/>
+      <c r="DE31" s="1"/>
+      <c r="DF31" s="1"/>
+      <c r="DG31" s="1"/>
+      <c r="DH31" s="1"/>
+      <c r="DI31" s="1"/>
+      <c r="DJ31" s="1"/>
+      <c r="DK31" s="1"/>
+      <c r="DL31" s="1"/>
+      <c r="DM31" s="1"/>
+      <c r="DN31" s="1"/>
+      <c r="DO31" s="1"/>
+      <c r="DP31" s="1"/>
+      <c r="DQ31" s="1"/>
+      <c r="DR31" s="1"/>
+      <c r="DS31" s="1"/>
+      <c r="DT31" s="1"/>
+      <c r="DU31" s="1"/>
+      <c r="DV31" s="1"/>
+      <c r="DW31" s="1"/>
+      <c r="DX31" s="1"/>
+      <c r="DY31" s="1"/>
+      <c r="DZ31" s="1"/>
+      <c r="EA31" s="1"/>
+      <c r="EB31" s="1"/>
+      <c r="EC31" s="1"/>
+      <c r="ED31" s="1"/>
+      <c r="EE31" s="1"/>
+      <c r="EF31" s="1"/>
+      <c r="EG31" s="1"/>
+      <c r="EH31" s="1"/>
+      <c r="EI31" s="1"/>
+      <c r="EJ31" s="1"/>
+      <c r="EK31" s="1"/>
+      <c r="EL31" s="1"/>
+      <c r="EM31" s="1"/>
+      <c r="EN31" s="1"/>
+      <c r="EO31" s="1"/>
+      <c r="EP31" s="1"/>
+      <c r="EQ31" s="1"/>
+      <c r="ER31" s="1"/>
+      <c r="ES31" s="1"/>
+      <c r="ET31" s="1"/>
+      <c r="EU31" s="1"/>
+      <c r="EV31" s="1"/>
+      <c r="EW31" s="1"/>
+      <c r="EX31" s="1"/>
+      <c r="EY31" s="1"/>
+      <c r="EZ31" s="1"/>
+      <c r="FA31" s="1"/>
+      <c r="FB31" s="1"/>
+      <c r="FC31" s="1"/>
+      <c r="FD31" s="1"/>
+      <c r="FE31" s="1"/>
+      <c r="FF31" s="1"/>
+      <c r="FG31" s="1"/>
+      <c r="FH31" s="1"/>
+      <c r="FI31" s="1"/>
+      <c r="FJ31" s="1"/>
+      <c r="FK31" s="1"/>
+      <c r="FL31" s="1"/>
+      <c r="FM31" s="1"/>
+      <c r="FN31" s="1"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="1">
+        <v>50</v>
+      </c>
+      <c r="F32" s="1">
+        <v>5</v>
+      </c>
+      <c r="G32" s="1">
+        <v>4</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+      <c r="AK32" s="1"/>
+      <c r="AL32" s="1"/>
+      <c r="AM32" s="1"/>
+      <c r="AN32" s="1"/>
+      <c r="AO32" s="1"/>
+      <c r="AP32" s="1"/>
+      <c r="AQ32" s="1"/>
+      <c r="AR32" s="1"/>
+      <c r="AS32" s="1"/>
+      <c r="AT32" s="1"/>
+      <c r="AU32" s="1"/>
+      <c r="AV32" s="1"/>
+      <c r="AW32" s="1"/>
+      <c r="AX32" s="1"/>
+      <c r="AY32" s="1"/>
+      <c r="AZ32" s="1"/>
+      <c r="BA32" s="1"/>
+      <c r="BB32" s="1"/>
+      <c r="BC32" s="1"/>
+      <c r="BD32" s="1"/>
+      <c r="BE32" s="1"/>
+      <c r="BF32" s="1"/>
+      <c r="BG32" s="1"/>
+      <c r="BH32" s="1"/>
+      <c r="BI32" s="1"/>
+      <c r="BJ32" s="1"/>
+      <c r="BK32" s="1"/>
+      <c r="BL32" s="1"/>
+      <c r="BM32" s="1"/>
+      <c r="BN32" s="1"/>
+      <c r="BO32" s="1"/>
+      <c r="BP32" s="1"/>
+      <c r="BQ32" s="1"/>
+      <c r="BR32" s="1"/>
+      <c r="BS32" s="1"/>
+      <c r="BT32" s="1"/>
+      <c r="BU32" s="1"/>
+      <c r="BV32" s="1"/>
+      <c r="BW32" s="1"/>
+      <c r="BX32" s="1"/>
+      <c r="BY32" s="1"/>
+      <c r="BZ32" s="1"/>
+      <c r="CA32" s="1"/>
+      <c r="CB32" s="1"/>
+      <c r="CC32" s="1"/>
+      <c r="CD32" s="1"/>
+      <c r="CE32" s="1"/>
+      <c r="CF32" s="1"/>
+      <c r="CG32" s="1"/>
+      <c r="CH32" s="1"/>
+      <c r="CI32" s="1"/>
+      <c r="CJ32" s="1"/>
+      <c r="CK32" s="1"/>
+      <c r="CL32" s="1"/>
+      <c r="CM32" s="1"/>
+      <c r="CN32" s="1"/>
+      <c r="CO32" s="1"/>
+      <c r="CP32" s="1"/>
+      <c r="CQ32" s="1"/>
+      <c r="CR32" s="1"/>
+      <c r="CS32" s="1"/>
+      <c r="CT32" s="1"/>
+      <c r="CU32" s="1"/>
+      <c r="CV32" s="1"/>
+      <c r="CW32" s="1"/>
+      <c r="CX32" s="1"/>
+      <c r="CY32" s="1"/>
+      <c r="CZ32" s="1"/>
+      <c r="DA32" s="1"/>
+      <c r="DB32" s="1"/>
+      <c r="DC32" s="1"/>
+      <c r="DD32" s="1"/>
+      <c r="DE32" s="1"/>
+      <c r="DF32" s="1"/>
+      <c r="DG32" s="1"/>
+      <c r="DH32" s="1"/>
+      <c r="DI32" s="1"/>
+      <c r="DJ32" s="1"/>
+      <c r="DK32" s="1"/>
+      <c r="DL32" s="1"/>
+      <c r="DM32" s="1"/>
+      <c r="DN32" s="1"/>
+      <c r="DO32" s="1"/>
+      <c r="DP32" s="1"/>
+      <c r="DQ32" s="1"/>
+      <c r="DR32" s="1"/>
+      <c r="DS32" s="1"/>
+      <c r="DT32" s="1"/>
+      <c r="DU32" s="1"/>
+      <c r="DV32" s="1"/>
+      <c r="DW32" s="1"/>
+      <c r="DX32" s="1"/>
+      <c r="DY32" s="1"/>
+      <c r="DZ32" s="1"/>
+      <c r="EA32" s="1"/>
+      <c r="EB32" s="1"/>
+      <c r="EC32" s="1"/>
+      <c r="ED32" s="1"/>
+      <c r="EE32" s="1"/>
+      <c r="EF32" s="1"/>
+      <c r="EG32" s="1"/>
+      <c r="EH32" s="1"/>
+      <c r="EI32" s="1"/>
+      <c r="EJ32" s="1"/>
+      <c r="EK32" s="1"/>
+      <c r="EL32" s="1"/>
+      <c r="EM32" s="1"/>
+      <c r="EN32" s="1"/>
+      <c r="EO32" s="1"/>
+      <c r="EP32" s="1"/>
+      <c r="EQ32" s="1"/>
+      <c r="ER32" s="1"/>
+      <c r="ES32" s="1"/>
+      <c r="ET32" s="1"/>
+      <c r="EU32" s="1"/>
+      <c r="EV32" s="1"/>
+      <c r="EW32" s="1"/>
+      <c r="EX32" s="1"/>
+      <c r="EY32" s="1"/>
+      <c r="EZ32" s="1"/>
+      <c r="FA32" s="1"/>
+      <c r="FB32" s="1"/>
+      <c r="FC32" s="1"/>
+      <c r="FD32" s="1"/>
+      <c r="FE32" s="1"/>
+      <c r="FF32" s="1"/>
+      <c r="FG32" s="1"/>
+      <c r="FH32" s="1"/>
+      <c r="FI32" s="1"/>
+      <c r="FJ32" s="1"/>
+      <c r="FK32" s="1"/>
+      <c r="FL32" s="1"/>
+      <c r="FM32" s="1"/>
+      <c r="FN32" s="1"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="1">
+        <v>50</v>
+      </c>
+      <c r="F33" s="1">
+        <v>5</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
+      <c r="AK33" s="1"/>
+      <c r="AL33" s="1"/>
+      <c r="AM33" s="1"/>
+      <c r="AN33" s="1"/>
+      <c r="AO33" s="1"/>
+      <c r="AP33" s="1"/>
+      <c r="AQ33" s="1"/>
+      <c r="AR33" s="1"/>
+      <c r="AS33" s="1"/>
+      <c r="AT33" s="1"/>
+      <c r="AU33" s="1"/>
+      <c r="AV33" s="1"/>
+      <c r="AW33" s="1"/>
+      <c r="AX33" s="1"/>
+      <c r="AY33" s="1"/>
+      <c r="AZ33" s="1"/>
+      <c r="BA33" s="1"/>
+      <c r="BB33" s="1"/>
+      <c r="BC33" s="1"/>
+      <c r="BD33" s="1"/>
+      <c r="BE33" s="1"/>
+      <c r="BF33" s="1"/>
+      <c r="BG33" s="1"/>
+      <c r="BH33" s="1"/>
+      <c r="BI33" s="1"/>
+      <c r="BJ33" s="1"/>
+      <c r="BK33" s="1"/>
+      <c r="BL33" s="1"/>
+      <c r="BM33" s="1"/>
+      <c r="BN33" s="1"/>
+      <c r="BO33" s="1"/>
+      <c r="BP33" s="1"/>
+      <c r="BQ33" s="1"/>
+      <c r="BR33" s="1"/>
+      <c r="BS33" s="1"/>
+      <c r="BT33" s="1"/>
+      <c r="BU33" s="1"/>
+      <c r="BV33" s="1"/>
+      <c r="BW33" s="1"/>
+      <c r="BX33" s="1"/>
+      <c r="BY33" s="1"/>
+      <c r="BZ33" s="1"/>
+      <c r="CA33" s="1"/>
+      <c r="CB33" s="1"/>
+      <c r="CC33" s="1"/>
+      <c r="CD33" s="1"/>
+      <c r="CE33" s="1"/>
+      <c r="CF33" s="1"/>
+      <c r="CG33" s="1"/>
+      <c r="CH33" s="1"/>
+      <c r="CI33" s="1"/>
+      <c r="CJ33" s="1"/>
+      <c r="CK33" s="1"/>
+      <c r="CL33" s="1"/>
+      <c r="CM33" s="1"/>
+      <c r="CN33" s="1"/>
+      <c r="CO33" s="1"/>
+      <c r="CP33" s="1"/>
+      <c r="CQ33" s="1"/>
+      <c r="CR33" s="1"/>
+      <c r="CS33" s="1"/>
+      <c r="CT33" s="1"/>
+      <c r="CU33" s="1"/>
+      <c r="CV33" s="1"/>
+      <c r="CW33" s="1"/>
+      <c r="CX33" s="1"/>
+      <c r="CY33" s="1"/>
+      <c r="CZ33" s="1"/>
+      <c r="DA33" s="1"/>
+      <c r="DB33" s="1"/>
+      <c r="DC33" s="1"/>
+      <c r="DD33" s="1"/>
+      <c r="DE33" s="1"/>
+      <c r="DF33" s="1"/>
+      <c r="DG33" s="1"/>
+      <c r="DH33" s="1"/>
+      <c r="DI33" s="1"/>
+      <c r="DJ33" s="1"/>
+      <c r="DK33" s="1"/>
+      <c r="DL33" s="1"/>
+      <c r="DM33" s="1"/>
+      <c r="DN33" s="1"/>
+      <c r="DO33" s="1"/>
+      <c r="DP33" s="1"/>
+      <c r="DQ33" s="1"/>
+      <c r="DR33" s="1"/>
+      <c r="DS33" s="1"/>
+      <c r="DT33" s="1"/>
+      <c r="DU33" s="1"/>
+      <c r="DV33" s="1"/>
+      <c r="DW33" s="1"/>
+      <c r="DX33" s="1"/>
+      <c r="DY33" s="1"/>
+      <c r="DZ33" s="1"/>
+      <c r="EA33" s="1"/>
+      <c r="EB33" s="1"/>
+      <c r="EC33" s="1"/>
+      <c r="ED33" s="1"/>
+      <c r="EE33" s="1"/>
+      <c r="EF33" s="1"/>
+      <c r="EG33" s="1"/>
+      <c r="EH33" s="1"/>
+      <c r="EI33" s="1"/>
+      <c r="EJ33" s="1"/>
+      <c r="EK33" s="1"/>
+      <c r="EL33" s="1"/>
+      <c r="EM33" s="1"/>
+      <c r="EN33" s="1"/>
+      <c r="EO33" s="1"/>
+      <c r="EP33" s="1"/>
+      <c r="EQ33" s="1"/>
+      <c r="ER33" s="1"/>
+      <c r="ES33" s="1"/>
+      <c r="ET33" s="1"/>
+      <c r="EU33" s="1"/>
+      <c r="EV33" s="1"/>
+      <c r="EW33" s="1"/>
+      <c r="EX33" s="1"/>
+      <c r="EY33" s="1"/>
+      <c r="EZ33" s="1"/>
+      <c r="FA33" s="1"/>
+      <c r="FB33" s="1"/>
+      <c r="FC33" s="1"/>
+      <c r="FD33" s="1"/>
+      <c r="FE33" s="1"/>
+      <c r="FF33" s="1"/>
+      <c r="FG33" s="1"/>
+      <c r="FH33" s="1"/>
+      <c r="FI33" s="1"/>
+      <c r="FJ33" s="1"/>
+      <c r="FK33" s="1"/>
+      <c r="FL33" s="1"/>
+      <c r="FM33" s="1"/>
+      <c r="FN33" s="1"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to 2024 crop data and Stata data cleaning codes
</commit_message>
<xml_diff>
--- a/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
+++ b/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1659" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1659" uniqueCount="267">
   <si>
     <t>crop</t>
   </si>
@@ -330,6 +330,12 @@
     <t>2024-04-24</t>
   </si>
   <si>
+    <t>11may2024</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>transp_harden_date_end</t>
   </si>
   <si>
@@ -342,6 +348,9 @@
     <t>2024-05-13</t>
   </si>
   <si>
+    <t>08may2024</t>
+  </si>
+  <si>
     <t>transp_date_1</t>
   </si>
   <si>
@@ -363,7 +372,7 @@
     <t>32</t>
   </si>
   <si>
-    <t>p</t>
+    <t>container- indoor</t>
   </si>
   <si>
     <t>4.5.d</t>
@@ -390,6 +399,9 @@
     <t>raised bed- frame</t>
   </si>
   <si>
+    <t>container- outdoor</t>
+  </si>
+  <si>
     <t>transp_no_srt_2</t>
   </si>
   <si>
@@ -790,6 +802,9 @@
   </si>
   <si>
     <t>1 was potted as gift during second transplant; 4 of 20 transplanted to catio were in a large container</t>
+  </si>
+  <si>
+    <t>These stayed in the 4.5.d pots indefinitely in the catio after transplant 1</t>
   </si>
   <si>
     <t>3 were potted as gift during second transplant</t>
@@ -957,421 +972,421 @@
         <v>103</v>
       </c>
       <c r="AJ1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AK1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AL1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AM1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AN1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AO1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AP1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AQ1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="AR1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AS1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AT1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="AU1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AV1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AW1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="AX1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="AY1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="AZ1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="BA1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="BB1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="BC1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="BD1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="BE1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="BF1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="BG1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="BH1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="BI1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="BJ1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="BK1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="BL1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="BM1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="BN1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="BO1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="BP1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="BQ1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="BR1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="BS1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="BT1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="BU1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="BV1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="BW1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="BX1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="BY1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="BZ1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="CA1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="CB1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="CC1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="CD1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="CE1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="CF1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="CG1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="CH1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="CI1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="CJ1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="CK1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="CL1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="CM1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="CN1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="CO1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="CP1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="CQ1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="CR1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="CS1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="CT1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="CU1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="CV1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="CW1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="CX1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="CY1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="CZ1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="DA1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="DB1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="DC1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="DD1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="DE1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="DF1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="DG1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="DH1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="DI1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="DJ1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="DK1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="DL1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="DM1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="DN1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="DO1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="DP1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="DQ1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="DR1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="DS1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="DT1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="DU1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="DV1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="DW1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="DX1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="DY1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="DZ1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="EA1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="EB1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="EC1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="ED1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="EE1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="EF1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="EG1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="EH1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="EI1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="EJ1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="EK1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="EL1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="EM1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="EN1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="EO1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="EP1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="EQ1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="ER1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="ES1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="ET1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="EU1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="EV1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="EW1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="EX1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="EY1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="EZ1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="FA1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="FB1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="FC1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="FD1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="FE1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="FF1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="FG1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="FH1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="FI1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="FJ1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="FK1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="FL1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="FM1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="FN1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="FO1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="FP1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="FQ1" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="FR1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2">
@@ -1732,10 +1747,10 @@
         <v>73</v>
       </c>
       <c r="AK3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AL3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM3" s="1">
         <v>8</v>
@@ -1747,7 +1762,7 @@
         <v>73</v>
       </c>
       <c r="AP3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AQ3" s="1">
         <v>8</v>
@@ -1996,10 +2011,10 @@
         <v>62</v>
       </c>
       <c r="AK4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AL4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM4" s="1">
         <v>1</v>
@@ -2251,13 +2266,13 @@
         <v>48</v>
       </c>
       <c r="AJ5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AK5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AL5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM5" s="1">
         <v>19</v>
@@ -2266,13 +2281,17 @@
         <v>19</v>
       </c>
       <c r="AO5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AP5" t="s">
         <v>52</v>
       </c>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
+      <c r="AQ5" s="1">
+        <v>19</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>19</v>
+      </c>
       <c r="AS5" s="1"/>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -2511,13 +2530,13 @@
         <v>48</v>
       </c>
       <c r="AJ6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AK6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AL6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM6" s="1">
         <v>18</v>
@@ -2526,13 +2545,17 @@
         <v>18</v>
       </c>
       <c r="AO6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AP6" t="s">
         <v>52</v>
       </c>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
+      <c r="AQ6" s="1">
+        <v>18</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>17</v>
+      </c>
       <c r="AS6" s="1"/>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
@@ -2771,13 +2794,13 @@
         <v>48</v>
       </c>
       <c r="AJ7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AK7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AL7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM7" s="1">
         <v>20</v>
@@ -2786,15 +2809,17 @@
         <v>20</v>
       </c>
       <c r="AO7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AP7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AQ7" s="1">
         <v>20</v>
       </c>
-      <c r="AR7" s="1"/>
+      <c r="AR7" s="1">
+        <v>20</v>
+      </c>
       <c r="AS7" s="1"/>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
@@ -3033,13 +3058,13 @@
         <v>48</v>
       </c>
       <c r="AJ8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AK8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AL8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM8" s="1">
         <v>20</v>
@@ -3048,15 +3073,17 @@
         <v>20</v>
       </c>
       <c r="AO8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AP8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AQ8" s="1">
         <v>20</v>
       </c>
-      <c r="AR8" s="1"/>
+      <c r="AR8" s="1">
+        <v>20</v>
+      </c>
       <c r="AS8" s="1"/>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
@@ -3294,7 +3321,7 @@
         <v>82</v>
       </c>
       <c r="AI9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ9" t="s">
         <v>62</v>
@@ -3303,7 +3330,7 @@
         <v>104</v>
       </c>
       <c r="AL9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM9" s="1">
         <v>16</v>
@@ -3449,7 +3476,7 @@
       <c r="FP9" s="1"/>
       <c r="FQ9" s="1"/>
       <c r="FR9" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10">
@@ -3556,16 +3583,16 @@
         <v>82</v>
       </c>
       <c r="AI10" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ10" t="s">
         <v>62</v>
       </c>
       <c r="AK10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM10" s="1">
         <v>12</v>
@@ -3816,16 +3843,16 @@
         <v>82</v>
       </c>
       <c r="AI11" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ11" t="s">
         <v>62</v>
       </c>
       <c r="AK11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM11" s="1">
         <v>3</v>
@@ -4076,16 +4103,16 @@
         <v>82</v>
       </c>
       <c r="AI12" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ12" t="s">
         <v>62</v>
       </c>
       <c r="AK12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM12" s="1">
         <v>4</v>
@@ -4336,16 +4363,16 @@
         <v>82</v>
       </c>
       <c r="AI13" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ13" t="s">
         <v>62</v>
       </c>
       <c r="AK13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM13" s="1">
         <v>25</v>
@@ -4596,16 +4623,16 @@
         <v>82</v>
       </c>
       <c r="AI14" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ14" t="s">
         <v>62</v>
       </c>
       <c r="AK14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM14" s="1">
         <v>5</v>
@@ -4856,16 +4883,16 @@
         <v>82</v>
       </c>
       <c r="AI15" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="AJ15" t="s">
         <v>62</v>
       </c>
       <c r="AK15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL15" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM15" s="1">
         <v>3</v>
@@ -5116,16 +5143,16 @@
         <v>82</v>
       </c>
       <c r="AI16" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="AJ16" t="s">
         <v>62</v>
       </c>
       <c r="AK16" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM16" s="1">
         <v>6</v>
@@ -5376,16 +5403,16 @@
         <v>82</v>
       </c>
       <c r="AI17" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="AJ17" t="s">
         <v>62</v>
       </c>
       <c r="AK17" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL17" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM17" s="1">
         <v>2</v>
@@ -5636,16 +5663,16 @@
         <v>82</v>
       </c>
       <c r="AI18" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ18" t="s">
         <v>62</v>
       </c>
       <c r="AK18" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL18" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM18" s="1">
         <v>1</v>
@@ -5896,16 +5923,16 @@
         <v>82</v>
       </c>
       <c r="AI19" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ19" t="s">
         <v>62</v>
       </c>
       <c r="AK19" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL19" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM19" s="1">
         <v>2</v>
@@ -6156,16 +6183,16 @@
         <v>82</v>
       </c>
       <c r="AI20" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="AJ20" t="s">
         <v>62</v>
       </c>
       <c r="AK20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AL20" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AM20" s="1">
         <v>3</v>
@@ -6419,13 +6446,13 @@
         <v>104</v>
       </c>
       <c r="AJ21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK21" t="s">
         <v>104</v>
       </c>
       <c r="AL21" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM21" s="1">
         <v>16</v>
@@ -6434,7 +6461,7 @@
         <v>15</v>
       </c>
       <c r="AO21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AP21" t="s">
         <v>52</v>
@@ -6683,13 +6710,13 @@
         <v>104</v>
       </c>
       <c r="AJ22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK22" t="s">
         <v>104</v>
       </c>
       <c r="AL22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM22" s="1">
         <v>16</v>
@@ -6698,7 +6725,7 @@
         <v>15</v>
       </c>
       <c r="AO22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AP22" t="s">
         <v>52</v>
@@ -6947,13 +6974,13 @@
         <v>104</v>
       </c>
       <c r="AJ23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK23" t="s">
         <v>104</v>
       </c>
       <c r="AL23" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM23" s="1">
         <v>12</v>
@@ -6962,7 +6989,7 @@
         <v>12</v>
       </c>
       <c r="AO23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AP23" t="s">
         <v>52</v>
@@ -7211,13 +7238,13 @@
         <v>104</v>
       </c>
       <c r="AJ24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK24" t="s">
         <v>104</v>
       </c>
       <c r="AL24" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM24" s="1">
         <v>13</v>
@@ -7226,7 +7253,7 @@
         <v>12</v>
       </c>
       <c r="AO24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AP24" t="s">
         <v>52</v>
@@ -7481,7 +7508,7 @@
         <v>104</v>
       </c>
       <c r="AL25" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AM25" s="1">
         <v>8</v>
@@ -7493,7 +7520,7 @@
         <v>73</v>
       </c>
       <c r="AP25" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="AQ25" s="1">
         <v>8</v>
@@ -7738,16 +7765,16 @@
         <v>62</v>
       </c>
       <c r="AI26" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ26" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="AK26" t="s">
         <v>104</v>
       </c>
       <c r="AL26" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AM26" s="1">
         <v>21</v>
@@ -7756,15 +7783,17 @@
         <v>21</v>
       </c>
       <c r="AO26" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AP26" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AQ26" s="1">
         <v>20</v>
       </c>
-      <c r="AR26" s="1"/>
+      <c r="AR26" s="1">
+        <v>19</v>
+      </c>
       <c r="AS26" s="1"/>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
@@ -7895,7 +7924,7 @@
       <c r="FP26" s="1"/>
       <c r="FQ26" s="1"/>
       <c r="FR26" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27">
@@ -8002,16 +8031,16 @@
         <v>62</v>
       </c>
       <c r="AI27" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="AJ27" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="AK27" t="s">
         <v>104</v>
       </c>
       <c r="AL27" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AM27" s="1">
         <v>3</v>
@@ -8262,16 +8291,16 @@
         <v>62</v>
       </c>
       <c r="AI28" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ28" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="AK28" t="s">
         <v>104</v>
       </c>
       <c r="AL28" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AM28" s="1">
         <v>3</v>
@@ -8415,7 +8444,7 @@
       <c r="FP28" s="1"/>
       <c r="FQ28" s="1"/>
       <c r="FR28" t="s">
-        <v>62</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29">
@@ -8522,16 +8551,16 @@
         <v>62</v>
       </c>
       <c r="AI29" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ29" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="AK29" t="s">
         <v>104</v>
       </c>
       <c r="AL29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AM29" s="1">
         <v>6</v>
@@ -8675,7 +8704,7 @@
       <c r="FP29" s="1"/>
       <c r="FQ29" s="1"/>
       <c r="FR29" t="s">
-        <v>62</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30">
@@ -8782,7 +8811,7 @@
         <v>62</v>
       </c>
       <c r="AI30" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ30" t="s">
         <v>62</v>
@@ -8791,7 +8820,7 @@
         <v>104</v>
       </c>
       <c r="AL30" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM30" s="1">
         <v>12</v>
@@ -9042,7 +9071,7 @@
         <v>62</v>
       </c>
       <c r="AI31" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ31" t="s">
         <v>62</v>
@@ -9051,7 +9080,7 @@
         <v>104</v>
       </c>
       <c r="AL31" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM31" s="1">
         <v>15</v>
@@ -9195,7 +9224,7 @@
       <c r="FP31" s="1"/>
       <c r="FQ31" s="1"/>
       <c r="FR31" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32">
@@ -9302,7 +9331,7 @@
         <v>62</v>
       </c>
       <c r="AI32" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ32" t="s">
         <v>62</v>
@@ -9311,7 +9340,7 @@
         <v>104</v>
       </c>
       <c r="AL32" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM32" s="1">
         <v>11</v>
@@ -9455,7 +9484,7 @@
       <c r="FP32" s="1"/>
       <c r="FQ32" s="1"/>
       <c r="FR32" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
@@ -9562,7 +9591,7 @@
         <v>62</v>
       </c>
       <c r="AI33" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AJ33" t="s">
         <v>62</v>
@@ -9571,7 +9600,7 @@
         <v>104</v>
       </c>
       <c r="AL33" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AM33" s="1">
         <v>15</v>
@@ -9715,7 +9744,7 @@
       <c r="FP33" s="1"/>
       <c r="FQ33" s="1"/>
       <c r="FR33" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34">
@@ -11016,7 +11045,9 @@
       <c r="I39" s="1">
         <v>3</v>
       </c>
-      <c r="J39" s="1"/>
+      <c r="J39" s="1">
+        <v>3</v>
+      </c>
       <c r="K39" t="s">
         <v>64</v>
       </c>
@@ -11268,7 +11299,9 @@
       <c r="I40" s="1">
         <v>2</v>
       </c>
-      <c r="J40" s="1"/>
+      <c r="J40" s="1">
+        <v>2</v>
+      </c>
       <c r="K40" t="s">
         <v>64</v>
       </c>
@@ -11520,7 +11553,9 @@
       <c r="I41" s="1">
         <v>2</v>
       </c>
-      <c r="J41" s="1"/>
+      <c r="J41" s="1">
+        <v>2</v>
+      </c>
       <c r="K41" t="s">
         <v>64</v>
       </c>
@@ -11772,7 +11807,9 @@
       <c r="I42" s="1">
         <v>3</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="1">
+        <v>3</v>
+      </c>
       <c r="K42" t="s">
         <v>64</v>
       </c>
@@ -12024,7 +12061,9 @@
       <c r="I43" s="1">
         <v>3</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="1">
+        <v>3</v>
+      </c>
       <c r="K43" t="s">
         <v>64</v>
       </c>
@@ -12491,7 +12530,7 @@
       <c r="FP44" s="1"/>
       <c r="FQ44" s="1"/>
       <c r="FR44" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="45">
@@ -12737,7 +12776,7 @@
       <c r="FP45" s="1"/>
       <c r="FQ45" s="1"/>
       <c r="FR45" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46">

</xml_diff>

<commit_message>
updates to 2024 crop data and Stata programs
</commit_message>
<xml_diff>
--- a/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
+++ b/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1659" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1843" uniqueCount="272">
   <si>
     <t>crop</t>
   </si>
@@ -270,6 +270,9 @@
     <t>2024-04-15</t>
   </si>
   <si>
+    <t>2024-05-23</t>
+  </si>
+  <si>
     <t>sow_fert_type_npk_2</t>
   </si>
   <si>
@@ -322,6 +325,18 @@
   </si>
   <si>
     <t>sow_fert_dose_5</t>
+  </si>
+  <si>
+    <t>sow_fert_date_6</t>
+  </si>
+  <si>
+    <t>sow_fert_type_npk_6</t>
+  </si>
+  <si>
+    <t>sow_fert_type_name_6</t>
+  </si>
+  <si>
+    <t>sow_fert_dose_6</t>
   </si>
   <si>
     <t>transp_harden_date_srt</t>
@@ -859,7 +874,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FR46"/>
+  <dimension ref="A1:FV46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -924,469 +939,481 @@
         <v>83</v>
       </c>
       <c r="T1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="U1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Y1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Z1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AA1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AB1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AC1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AD1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AE1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AG1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AH1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AI1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AJ1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL1" t="s">
         <v>107</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN1" t="s">
         <v>112</v>
       </c>
-      <c r="AL1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>122</v>
-      </c>
       <c r="AO1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="AP1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AQ1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AR1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT1" t="s">
         <v>130</v>
       </c>
-      <c r="AS1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>132</v>
-      </c>
       <c r="AU1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AV1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AW1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AX1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AY1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AZ1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BA1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BB1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BC1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BD1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BE1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="BF1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BG1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="BH1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="BI1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="BJ1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="BK1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="BL1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="BM1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="BN1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="BO1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="BP1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="BQ1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="BR1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="BS1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="BT1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="BU1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="BV1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="BW1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BX1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BY1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CA1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CB1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CC1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CD1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CE1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CF1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CG1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CH1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CI1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CJ1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="CK1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="CL1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="CM1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="CN1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="CO1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="CP1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="CQ1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="CR1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CS1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="CT1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="CU1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="CV1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CW1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="CX1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="CY1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CZ1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="DA1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="DB1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="DC1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="DD1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="DE1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="DF1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="DG1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="DH1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="DI1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="DJ1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="DK1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="DL1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="DM1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="DN1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="DO1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="DP1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="DQ1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="DR1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="DS1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="DT1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="DU1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="DV1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="DW1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="DX1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="DY1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="DZ1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="EA1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="EB1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="EC1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="ED1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="EE1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="EF1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="EG1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="EH1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="EI1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="EJ1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="EK1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="EL1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="EM1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="EN1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="EO1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="EP1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="EQ1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="ER1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="ES1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="ET1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="EU1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="EV1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="EW1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="EX1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="EY1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="EZ1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="FA1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="FB1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="FC1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="FD1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="FE1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="FF1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="FG1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="FH1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="FI1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="FJ1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="FK1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="FL1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="FM1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="FN1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="FO1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="FP1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="FQ1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="FR1" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="FS1" t="s">
+        <v>262</v>
+      </c>
+      <c r="FT1" t="s">
+        <v>263</v>
+      </c>
+      <c r="FU1" t="s">
+        <v>264</v>
+      </c>
+      <c r="FV1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="2">
@@ -1496,8 +1523,12 @@
       <c r="AL2" t="s">
         <v>62</v>
       </c>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
+      <c r="AM2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>62</v>
+      </c>
       <c r="AO2" t="s">
         <v>62</v>
       </c>
@@ -1506,8 +1537,12 @@
       </c>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
+      <c r="AS2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>62</v>
+      </c>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
@@ -1635,7 +1670,11 @@
       <c r="FO2" s="1"/>
       <c r="FP2" s="1"/>
       <c r="FQ2" s="1"/>
-      <c r="FR2" t="s">
+      <c r="FR2" s="1"/>
+      <c r="FS2" s="1"/>
+      <c r="FT2" s="1"/>
+      <c r="FU2" s="1"/>
+      <c r="FV2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1705,7 +1744,7 @@
         <v>82</v>
       </c>
       <c r="W3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X3" t="s">
         <v>76</v>
@@ -1741,28 +1780,28 @@
         <v>62</v>
       </c>
       <c r="AI3" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN3" t="s">
         <v>73</v>
       </c>
-      <c r="AK3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM3" s="1">
-        <v>8</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>8</v>
-      </c>
       <c r="AO3" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="AP3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AQ3" s="1">
         <v>8</v>
@@ -1770,10 +1809,18 @@
       <c r="AR3" s="1">
         <v>8</v>
       </c>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
+      <c r="AS3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>8</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>8</v>
+      </c>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
@@ -1899,7 +1946,11 @@
       <c r="FO3" s="1"/>
       <c r="FP3" s="1"/>
       <c r="FQ3" s="1"/>
-      <c r="FR3" t="s">
+      <c r="FR3" s="1"/>
+      <c r="FS3" s="1"/>
+      <c r="FT3" s="1"/>
+      <c r="FU3" s="1"/>
+      <c r="FV3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1969,7 +2020,7 @@
         <v>82</v>
       </c>
       <c r="W4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X4" t="s">
         <v>76</v>
@@ -2011,25 +2062,33 @@
         <v>62</v>
       </c>
       <c r="AK4" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="AL4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM4" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ4" s="1">
         <v>1</v>
       </c>
-      <c r="AN4" s="1"/>
-      <c r="AO4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
+      <c r="AS4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>62</v>
+      </c>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
@@ -2157,7 +2216,11 @@
       <c r="FO4" s="1"/>
       <c r="FP4" s="1"/>
       <c r="FQ4" s="1"/>
-      <c r="FR4" t="s">
+      <c r="FR4" s="1"/>
+      <c r="FS4" s="1"/>
+      <c r="FT4" s="1"/>
+      <c r="FU4" s="1"/>
+      <c r="FV4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2263,28 +2326,28 @@
         <v>62</v>
       </c>
       <c r="AI5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM5" t="s">
         <v>48</v>
       </c>
-      <c r="AJ5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK5" t="s">
+      <c r="AN5" t="s">
         <v>113</v>
       </c>
-      <c r="AL5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM5" s="1">
-        <v>19</v>
-      </c>
-      <c r="AN5" s="1">
-        <v>19</v>
-      </c>
       <c r="AO5" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="AP5" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="AQ5" s="1">
         <v>19</v>
@@ -2292,10 +2355,18 @@
       <c r="AR5" s="1">
         <v>19</v>
       </c>
-      <c r="AS5" s="1"/>
-      <c r="AT5" s="1"/>
-      <c r="AU5" s="1"/>
-      <c r="AV5" s="1"/>
+      <c r="AS5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>19</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>19</v>
+      </c>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
@@ -2421,7 +2492,11 @@
       <c r="FO5" s="1"/>
       <c r="FP5" s="1"/>
       <c r="FQ5" s="1"/>
-      <c r="FR5" t="s">
+      <c r="FR5" s="1"/>
+      <c r="FS5" s="1"/>
+      <c r="FT5" s="1"/>
+      <c r="FU5" s="1"/>
+      <c r="FV5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2527,39 +2602,47 @@
         <v>62</v>
       </c>
       <c r="AI6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM6" t="s">
         <v>48</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM6" s="1">
-        <v>18</v>
-      </c>
-      <c r="AN6" s="1">
-        <v>18</v>
+      <c r="AN6" t="s">
+        <v>114</v>
       </c>
       <c r="AO6" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="AP6" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="AQ6" s="1">
         <v>18</v>
       </c>
       <c r="AR6" s="1">
+        <v>18</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>18</v>
+      </c>
+      <c r="AV6" s="1">
         <v>17</v>
       </c>
-      <c r="AS6" s="1"/>
-      <c r="AT6" s="1"/>
-      <c r="AU6" s="1"/>
-      <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
@@ -2685,7 +2768,11 @@
       <c r="FO6" s="1"/>
       <c r="FP6" s="1"/>
       <c r="FQ6" s="1"/>
-      <c r="FR6" t="s">
+      <c r="FR6" s="1"/>
+      <c r="FS6" s="1"/>
+      <c r="FT6" s="1"/>
+      <c r="FU6" s="1"/>
+      <c r="FV6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2791,28 +2878,28 @@
         <v>62</v>
       </c>
       <c r="AI7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM7" t="s">
         <v>48</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM7" s="1">
-        <v>20</v>
-      </c>
-      <c r="AN7" s="1">
-        <v>20</v>
+      <c r="AN7" t="s">
+        <v>114</v>
       </c>
       <c r="AO7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AP7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AQ7" s="1">
         <v>20</v>
@@ -2820,10 +2907,18 @@
       <c r="AR7" s="1">
         <v>20</v>
       </c>
-      <c r="AS7" s="1"/>
-      <c r="AT7" s="1"/>
-      <c r="AU7" s="1"/>
-      <c r="AV7" s="1"/>
+      <c r="AS7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>20</v>
+      </c>
+      <c r="AV7" s="1">
+        <v>20</v>
+      </c>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1"/>
       <c r="AY7" s="1"/>
@@ -2949,7 +3044,11 @@
       <c r="FO7" s="1"/>
       <c r="FP7" s="1"/>
       <c r="FQ7" s="1"/>
-      <c r="FR7" t="s">
+      <c r="FR7" s="1"/>
+      <c r="FS7" s="1"/>
+      <c r="FT7" s="1"/>
+      <c r="FU7" s="1"/>
+      <c r="FV7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3055,28 +3154,28 @@
         <v>62</v>
       </c>
       <c r="AI8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM8" t="s">
         <v>48</v>
       </c>
-      <c r="AJ8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM8" s="1">
-        <v>20</v>
-      </c>
-      <c r="AN8" s="1">
-        <v>20</v>
+      <c r="AN8" t="s">
+        <v>114</v>
       </c>
       <c r="AO8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AP8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AQ8" s="1">
         <v>20</v>
@@ -3084,10 +3183,18 @@
       <c r="AR8" s="1">
         <v>20</v>
       </c>
-      <c r="AS8" s="1"/>
-      <c r="AT8" s="1"/>
-      <c r="AU8" s="1"/>
-      <c r="AV8" s="1"/>
+      <c r="AS8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU8" s="1">
+        <v>20</v>
+      </c>
+      <c r="AV8" s="1">
+        <v>20</v>
+      </c>
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
       <c r="AY8" s="1"/>
@@ -3213,7 +3320,11 @@
       <c r="FO8" s="1"/>
       <c r="FP8" s="1"/>
       <c r="FQ8" s="1"/>
-      <c r="FR8" t="s">
+      <c r="FR8" s="1"/>
+      <c r="FS8" s="1"/>
+      <c r="FT8" s="1"/>
+      <c r="FU8" s="1"/>
+      <c r="FV8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3297,7 +3408,7 @@
         <v>82</v>
       </c>
       <c r="AA9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB9" t="s">
         <v>76</v>
@@ -3321,33 +3432,41 @@
         <v>82</v>
       </c>
       <c r="AI9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM9" t="s">
         <v>73</v>
       </c>
-      <c r="AJ9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>104</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM9" s="1">
+      <c r="AN9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ9" s="1">
         <v>16</v>
       </c>
-      <c r="AN9" s="1">
+      <c r="AR9" s="1">
         <v>16</v>
       </c>
-      <c r="AO9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
+      <c r="AS9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>62</v>
+      </c>
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
@@ -3475,8 +3594,12 @@
       <c r="FO9" s="1"/>
       <c r="FP9" s="1"/>
       <c r="FQ9" s="1"/>
-      <c r="FR9" t="s">
-        <v>261</v>
+      <c r="FR9" s="1"/>
+      <c r="FS9" s="1"/>
+      <c r="FT9" s="1"/>
+      <c r="FU9" s="1"/>
+      <c r="FV9" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="10">
@@ -3559,7 +3682,7 @@
         <v>82</v>
       </c>
       <c r="AA10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB10" t="s">
         <v>76</v>
@@ -3571,7 +3694,7 @@
         <v>82</v>
       </c>
       <c r="AE10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF10" t="s">
         <v>76</v>
@@ -3583,31 +3706,39 @@
         <v>82</v>
       </c>
       <c r="AI10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM10" t="s">
         <v>73</v>
       </c>
-      <c r="AJ10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM10" s="1">
+      <c r="AN10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ10" s="1">
         <v>12</v>
       </c>
-      <c r="AN10" s="1"/>
-      <c r="AO10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ10" s="1"/>
       <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" s="1"/>
+      <c r="AS10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>62</v>
+      </c>
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
@@ -3735,7 +3866,11 @@
       <c r="FO10" s="1"/>
       <c r="FP10" s="1"/>
       <c r="FQ10" s="1"/>
-      <c r="FR10" t="s">
+      <c r="FR10" s="1"/>
+      <c r="FS10" s="1"/>
+      <c r="FT10" s="1"/>
+      <c r="FU10" s="1"/>
+      <c r="FV10" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3819,7 +3954,7 @@
         <v>82</v>
       </c>
       <c r="AA11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB11" t="s">
         <v>76</v>
@@ -3831,7 +3966,7 @@
         <v>82</v>
       </c>
       <c r="AE11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF11" t="s">
         <v>76</v>
@@ -3843,31 +3978,39 @@
         <v>82</v>
       </c>
       <c r="AI11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM11" t="s">
         <v>73</v>
       </c>
-      <c r="AJ11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM11" s="1">
+      <c r="AN11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ11" s="1">
         <v>3</v>
       </c>
-      <c r="AN11" s="1"/>
-      <c r="AO11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ11" s="1"/>
       <c r="AR11" s="1"/>
-      <c r="AS11" s="1"/>
-      <c r="AT11" s="1"/>
+      <c r="AS11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>62</v>
+      </c>
       <c r="AU11" s="1"/>
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
@@ -3995,7 +4138,11 @@
       <c r="FO11" s="1"/>
       <c r="FP11" s="1"/>
       <c r="FQ11" s="1"/>
-      <c r="FR11" t="s">
+      <c r="FR11" s="1"/>
+      <c r="FS11" s="1"/>
+      <c r="FT11" s="1"/>
+      <c r="FU11" s="1"/>
+      <c r="FV11" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4079,7 +4226,7 @@
         <v>82</v>
       </c>
       <c r="AA12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB12" t="s">
         <v>76</v>
@@ -4091,7 +4238,7 @@
         <v>82</v>
       </c>
       <c r="AE12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF12" t="s">
         <v>76</v>
@@ -4103,31 +4250,39 @@
         <v>82</v>
       </c>
       <c r="AI12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM12" t="s">
         <v>73</v>
       </c>
-      <c r="AJ12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM12" s="1">
+      <c r="AN12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ12" s="1">
         <v>4</v>
       </c>
-      <c r="AN12" s="1"/>
-      <c r="AO12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ12" s="1"/>
       <c r="AR12" s="1"/>
-      <c r="AS12" s="1"/>
-      <c r="AT12" s="1"/>
+      <c r="AS12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>62</v>
+      </c>
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
@@ -4255,7 +4410,11 @@
       <c r="FO12" s="1"/>
       <c r="FP12" s="1"/>
       <c r="FQ12" s="1"/>
-      <c r="FR12" t="s">
+      <c r="FR12" s="1"/>
+      <c r="FS12" s="1"/>
+      <c r="FT12" s="1"/>
+      <c r="FU12" s="1"/>
+      <c r="FV12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4339,7 +4498,7 @@
         <v>82</v>
       </c>
       <c r="AA13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB13" t="s">
         <v>76</v>
@@ -4351,7 +4510,7 @@
         <v>82</v>
       </c>
       <c r="AE13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF13" t="s">
         <v>76</v>
@@ -4363,31 +4522,39 @@
         <v>82</v>
       </c>
       <c r="AI13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM13" t="s">
         <v>73</v>
       </c>
-      <c r="AJ13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM13" s="1">
+      <c r="AN13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ13" s="1">
         <v>25</v>
       </c>
-      <c r="AN13" s="1"/>
-      <c r="AO13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ13" s="1"/>
       <c r="AR13" s="1"/>
-      <c r="AS13" s="1"/>
-      <c r="AT13" s="1"/>
+      <c r="AS13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>62</v>
+      </c>
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
@@ -4515,7 +4682,11 @@
       <c r="FO13" s="1"/>
       <c r="FP13" s="1"/>
       <c r="FQ13" s="1"/>
-      <c r="FR13" t="s">
+      <c r="FR13" s="1"/>
+      <c r="FS13" s="1"/>
+      <c r="FT13" s="1"/>
+      <c r="FU13" s="1"/>
+      <c r="FV13" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4599,7 +4770,7 @@
         <v>82</v>
       </c>
       <c r="AA14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB14" t="s">
         <v>76</v>
@@ -4611,7 +4782,7 @@
         <v>82</v>
       </c>
       <c r="AE14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF14" t="s">
         <v>76</v>
@@ -4623,31 +4794,39 @@
         <v>82</v>
       </c>
       <c r="AI14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM14" t="s">
         <v>73</v>
       </c>
-      <c r="AJ14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM14" s="1">
+      <c r="AN14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ14" s="1">
         <v>5</v>
       </c>
-      <c r="AN14" s="1"/>
-      <c r="AO14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ14" s="1"/>
       <c r="AR14" s="1"/>
-      <c r="AS14" s="1"/>
-      <c r="AT14" s="1"/>
+      <c r="AS14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>62</v>
+      </c>
       <c r="AU14" s="1"/>
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
@@ -4775,7 +4954,11 @@
       <c r="FO14" s="1"/>
       <c r="FP14" s="1"/>
       <c r="FQ14" s="1"/>
-      <c r="FR14" t="s">
+      <c r="FR14" s="1"/>
+      <c r="FS14" s="1"/>
+      <c r="FT14" s="1"/>
+      <c r="FU14" s="1"/>
+      <c r="FV14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4859,7 +5042,7 @@
         <v>82</v>
       </c>
       <c r="AA15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB15" t="s">
         <v>76</v>
@@ -4871,7 +5054,7 @@
         <v>82</v>
       </c>
       <c r="AE15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF15" t="s">
         <v>76</v>
@@ -4883,31 +5066,39 @@
         <v>82</v>
       </c>
       <c r="AI15" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="AJ15" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="AK15" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="AL15" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM15" s="1">
+        <v>82</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ15" s="1">
         <v>3</v>
       </c>
-      <c r="AN15" s="1"/>
-      <c r="AO15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ15" s="1"/>
       <c r="AR15" s="1"/>
-      <c r="AS15" s="1"/>
-      <c r="AT15" s="1"/>
+      <c r="AS15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>62</v>
+      </c>
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
@@ -5035,7 +5226,11 @@
       <c r="FO15" s="1"/>
       <c r="FP15" s="1"/>
       <c r="FQ15" s="1"/>
-      <c r="FR15" t="s">
+      <c r="FR15" s="1"/>
+      <c r="FS15" s="1"/>
+      <c r="FT15" s="1"/>
+      <c r="FU15" s="1"/>
+      <c r="FV15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5119,7 +5314,7 @@
         <v>82</v>
       </c>
       <c r="AA16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB16" t="s">
         <v>76</v>
@@ -5131,7 +5326,7 @@
         <v>82</v>
       </c>
       <c r="AE16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF16" t="s">
         <v>76</v>
@@ -5143,31 +5338,39 @@
         <v>82</v>
       </c>
       <c r="AI16" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="AJ16" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="AK16" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="AL16" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM16" s="1">
+        <v>82</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ16" s="1">
         <v>6</v>
       </c>
-      <c r="AN16" s="1"/>
-      <c r="AO16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ16" s="1"/>
       <c r="AR16" s="1"/>
-      <c r="AS16" s="1"/>
-      <c r="AT16" s="1"/>
+      <c r="AS16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>62</v>
+      </c>
       <c r="AU16" s="1"/>
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
@@ -5295,7 +5498,11 @@
       <c r="FO16" s="1"/>
       <c r="FP16" s="1"/>
       <c r="FQ16" s="1"/>
-      <c r="FR16" t="s">
+      <c r="FR16" s="1"/>
+      <c r="FS16" s="1"/>
+      <c r="FT16" s="1"/>
+      <c r="FU16" s="1"/>
+      <c r="FV16" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5379,7 +5586,7 @@
         <v>82</v>
       </c>
       <c r="AA17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB17" t="s">
         <v>76</v>
@@ -5391,7 +5598,7 @@
         <v>82</v>
       </c>
       <c r="AE17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF17" t="s">
         <v>76</v>
@@ -5403,31 +5610,39 @@
         <v>82</v>
       </c>
       <c r="AI17" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="AJ17" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="AK17" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="AL17" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM17" s="1">
+        <v>82</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ17" s="1">
         <v>2</v>
       </c>
-      <c r="AN17" s="1"/>
-      <c r="AO17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
-      <c r="AS17" s="1"/>
-      <c r="AT17" s="1"/>
+      <c r="AS17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>62</v>
+      </c>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
@@ -5555,7 +5770,11 @@
       <c r="FO17" s="1"/>
       <c r="FP17" s="1"/>
       <c r="FQ17" s="1"/>
-      <c r="FR17" t="s">
+      <c r="FR17" s="1"/>
+      <c r="FS17" s="1"/>
+      <c r="FT17" s="1"/>
+      <c r="FU17" s="1"/>
+      <c r="FV17" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5639,7 +5858,7 @@
         <v>82</v>
       </c>
       <c r="AA18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB18" t="s">
         <v>76</v>
@@ -5651,7 +5870,7 @@
         <v>82</v>
       </c>
       <c r="AE18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF18" t="s">
         <v>76</v>
@@ -5663,31 +5882,39 @@
         <v>82</v>
       </c>
       <c r="AI18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM18" t="s">
         <v>73</v>
       </c>
-      <c r="AJ18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM18" s="1">
+      <c r="AN18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ18" s="1">
         <v>1</v>
       </c>
-      <c r="AN18" s="1"/>
-      <c r="AO18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ18" s="1"/>
       <c r="AR18" s="1"/>
-      <c r="AS18" s="1"/>
-      <c r="AT18" s="1"/>
+      <c r="AS18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>62</v>
+      </c>
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
@@ -5815,7 +6042,11 @@
       <c r="FO18" s="1"/>
       <c r="FP18" s="1"/>
       <c r="FQ18" s="1"/>
-      <c r="FR18" t="s">
+      <c r="FR18" s="1"/>
+      <c r="FS18" s="1"/>
+      <c r="FT18" s="1"/>
+      <c r="FU18" s="1"/>
+      <c r="FV18" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5899,7 +6130,7 @@
         <v>82</v>
       </c>
       <c r="AA19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB19" t="s">
         <v>76</v>
@@ -5911,7 +6142,7 @@
         <v>82</v>
       </c>
       <c r="AE19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF19" t="s">
         <v>76</v>
@@ -5923,31 +6154,39 @@
         <v>82</v>
       </c>
       <c r="AI19" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM19" t="s">
         <v>73</v>
       </c>
-      <c r="AJ19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM19" s="1">
+      <c r="AN19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ19" s="1">
         <v>2</v>
       </c>
-      <c r="AN19" s="1"/>
-      <c r="AO19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ19" s="1"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="1"/>
-      <c r="AT19" s="1"/>
+      <c r="AS19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>62</v>
+      </c>
       <c r="AU19" s="1"/>
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
@@ -6075,7 +6314,11 @@
       <c r="FO19" s="1"/>
       <c r="FP19" s="1"/>
       <c r="FQ19" s="1"/>
-      <c r="FR19" t="s">
+      <c r="FR19" s="1"/>
+      <c r="FS19" s="1"/>
+      <c r="FT19" s="1"/>
+      <c r="FU19" s="1"/>
+      <c r="FV19" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6159,7 +6402,7 @@
         <v>82</v>
       </c>
       <c r="AA20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB20" t="s">
         <v>76</v>
@@ -6171,7 +6414,7 @@
         <v>82</v>
       </c>
       <c r="AE20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF20" t="s">
         <v>76</v>
@@ -6183,31 +6426,39 @@
         <v>82</v>
       </c>
       <c r="AI20" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM20" t="s">
         <v>73</v>
       </c>
-      <c r="AJ20" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL20" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM20" s="1">
+      <c r="AN20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ20" s="1">
         <v>3</v>
       </c>
-      <c r="AN20" s="1"/>
-      <c r="AO20" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP20" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ20" s="1"/>
       <c r="AR20" s="1"/>
-      <c r="AS20" s="1"/>
-      <c r="AT20" s="1"/>
+      <c r="AS20" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>62</v>
+      </c>
       <c r="AU20" s="1"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
@@ -6335,7 +6586,11 @@
       <c r="FO20" s="1"/>
       <c r="FP20" s="1"/>
       <c r="FQ20" s="1"/>
-      <c r="FR20" t="s">
+      <c r="FR20" s="1"/>
+      <c r="FS20" s="1"/>
+      <c r="FT20" s="1"/>
+      <c r="FU20" s="1"/>
+      <c r="FV20" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6407,7 +6662,7 @@
         <v>82</v>
       </c>
       <c r="W21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X21" t="s">
         <v>76</v>
@@ -6443,36 +6698,44 @@
         <v>82</v>
       </c>
       <c r="AI21" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ21" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="AK21" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL21" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM21" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>115</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ21" s="1">
         <v>16</v>
       </c>
-      <c r="AN21" s="1">
+      <c r="AR21" s="1">
         <v>15</v>
       </c>
-      <c r="AO21" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP21" t="s">
+      <c r="AS21" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT21" t="s">
         <v>52</v>
       </c>
-      <c r="AQ21" s="1">
+      <c r="AU21" s="1">
         <v>9</v>
       </c>
-      <c r="AR21" s="1"/>
-      <c r="AS21" s="1"/>
-      <c r="AT21" s="1"/>
-      <c r="AU21" s="1"/>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
@@ -6599,7 +6862,11 @@
       <c r="FO21" s="1"/>
       <c r="FP21" s="1"/>
       <c r="FQ21" s="1"/>
-      <c r="FR21" t="s">
+      <c r="FR21" s="1"/>
+      <c r="FS21" s="1"/>
+      <c r="FT21" s="1"/>
+      <c r="FU21" s="1"/>
+      <c r="FV21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6671,7 +6938,7 @@
         <v>82</v>
       </c>
       <c r="W22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X22" t="s">
         <v>76</v>
@@ -6707,36 +6974,44 @@
         <v>82</v>
       </c>
       <c r="AI22" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ22" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="AK22" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL22" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM22" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>115</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ22" s="1">
         <v>16</v>
       </c>
-      <c r="AN22" s="1">
+      <c r="AR22" s="1">
         <v>15</v>
       </c>
-      <c r="AO22" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP22" t="s">
+      <c r="AS22" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT22" t="s">
         <v>52</v>
       </c>
-      <c r="AQ22" s="1">
+      <c r="AU22" s="1">
         <v>9</v>
       </c>
-      <c r="AR22" s="1"/>
-      <c r="AS22" s="1"/>
-      <c r="AT22" s="1"/>
-      <c r="AU22" s="1"/>
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
       <c r="AX22" s="1"/>
@@ -6863,7 +7138,11 @@
       <c r="FO22" s="1"/>
       <c r="FP22" s="1"/>
       <c r="FQ22" s="1"/>
-      <c r="FR22" t="s">
+      <c r="FR22" s="1"/>
+      <c r="FS22" s="1"/>
+      <c r="FT22" s="1"/>
+      <c r="FU22" s="1"/>
+      <c r="FV22" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6935,7 +7214,7 @@
         <v>82</v>
       </c>
       <c r="W23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X23" t="s">
         <v>76</v>
@@ -6971,36 +7250,44 @@
         <v>82</v>
       </c>
       <c r="AI23" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ23" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="AK23" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL23" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM23" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>115</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ23" s="1">
         <v>12</v>
       </c>
-      <c r="AN23" s="1">
+      <c r="AR23" s="1">
         <v>12</v>
       </c>
-      <c r="AO23" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP23" t="s">
+      <c r="AS23" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT23" t="s">
         <v>52</v>
       </c>
-      <c r="AQ23" s="1">
+      <c r="AU23" s="1">
         <v>8</v>
       </c>
-      <c r="AR23" s="1"/>
-      <c r="AS23" s="1"/>
-      <c r="AT23" s="1"/>
-      <c r="AU23" s="1"/>
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
@@ -7127,7 +7414,11 @@
       <c r="FO23" s="1"/>
       <c r="FP23" s="1"/>
       <c r="FQ23" s="1"/>
-      <c r="FR23" t="s">
+      <c r="FR23" s="1"/>
+      <c r="FS23" s="1"/>
+      <c r="FT23" s="1"/>
+      <c r="FU23" s="1"/>
+      <c r="FV23" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7199,7 +7490,7 @@
         <v>82</v>
       </c>
       <c r="W24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X24" t="s">
         <v>76</v>
@@ -7235,36 +7526,44 @@
         <v>82</v>
       </c>
       <c r="AI24" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ24" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="AK24" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL24" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM24" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN24" t="s">
+        <v>115</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ24" s="1">
         <v>13</v>
       </c>
-      <c r="AN24" s="1">
+      <c r="AR24" s="1">
         <v>12</v>
       </c>
-      <c r="AO24" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP24" t="s">
+      <c r="AS24" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT24" t="s">
         <v>52</v>
       </c>
-      <c r="AQ24" s="1">
+      <c r="AU24" s="1">
         <v>8</v>
       </c>
-      <c r="AR24" s="1"/>
-      <c r="AS24" s="1"/>
-      <c r="AT24" s="1"/>
-      <c r="AU24" s="1"/>
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
       <c r="AX24" s="1"/>
@@ -7391,7 +7690,11 @@
       <c r="FO24" s="1"/>
       <c r="FP24" s="1"/>
       <c r="FQ24" s="1"/>
-      <c r="FR24" t="s">
+      <c r="FR24" s="1"/>
+      <c r="FS24" s="1"/>
+      <c r="FT24" s="1"/>
+      <c r="FU24" s="1"/>
+      <c r="FV24" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7463,20 +7766,20 @@
         <v>82</v>
       </c>
       <c r="W25" t="s">
+        <v>91</v>
+      </c>
+      <c r="X25" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA25" t="s">
         <v>90</v>
       </c>
-      <c r="X25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>89</v>
-      </c>
       <c r="AB25" t="s">
         <v>76</v>
       </c>
@@ -7499,28 +7802,28 @@
         <v>62</v>
       </c>
       <c r="AI25" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN25" t="s">
         <v>73</v>
       </c>
-      <c r="AK25" t="s">
-        <v>104</v>
-      </c>
-      <c r="AL25" t="s">
-        <v>118</v>
-      </c>
-      <c r="AM25" s="1">
-        <v>8</v>
-      </c>
-      <c r="AN25" s="1">
-        <v>8</v>
-      </c>
       <c r="AO25" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="AP25" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AQ25" s="1">
         <v>8</v>
@@ -7528,10 +7831,18 @@
       <c r="AR25" s="1">
         <v>8</v>
       </c>
-      <c r="AS25" s="1"/>
-      <c r="AT25" s="1"/>
-      <c r="AU25" s="1"/>
-      <c r="AV25" s="1"/>
+      <c r="AS25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU25" s="1">
+        <v>8</v>
+      </c>
+      <c r="AV25" s="1">
+        <v>8</v>
+      </c>
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
       <c r="AY25" s="1"/>
@@ -7657,7 +7968,11 @@
       <c r="FO25" s="1"/>
       <c r="FP25" s="1"/>
       <c r="FQ25" s="1"/>
-      <c r="FR25" t="s">
+      <c r="FR25" s="1"/>
+      <c r="FS25" s="1"/>
+      <c r="FT25" s="1"/>
+      <c r="FU25" s="1"/>
+      <c r="FV25" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7729,7 +8044,7 @@
         <v>82</v>
       </c>
       <c r="W26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X26" t="s">
         <v>76</v>
@@ -7765,39 +8080,47 @@
         <v>62</v>
       </c>
       <c r="AI26" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ26" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="AK26" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL26" t="s">
-        <v>118</v>
-      </c>
-      <c r="AM26" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>123</v>
+      </c>
+      <c r="AQ26" s="1">
         <v>21</v>
       </c>
-      <c r="AN26" s="1">
+      <c r="AR26" s="1">
         <v>21</v>
       </c>
-      <c r="AO26" t="s">
-        <v>124</v>
-      </c>
-      <c r="AP26" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ26" s="1">
+      <c r="AS26" t="s">
+        <v>129</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU26" s="1">
         <v>20</v>
       </c>
-      <c r="AR26" s="1">
+      <c r="AV26" s="1">
         <v>19</v>
       </c>
-      <c r="AS26" s="1"/>
-      <c r="AT26" s="1"/>
-      <c r="AU26" s="1"/>
-      <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
       <c r="AX26" s="1"/>
       <c r="AY26" s="1"/>
@@ -7923,8 +8246,12 @@
       <c r="FO26" s="1"/>
       <c r="FP26" s="1"/>
       <c r="FQ26" s="1"/>
-      <c r="FR26" t="s">
-        <v>262</v>
+      <c r="FR26" s="1"/>
+      <c r="FS26" s="1"/>
+      <c r="FT26" s="1"/>
+      <c r="FU26" s="1"/>
+      <c r="FV26" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="27">
@@ -7995,7 +8322,7 @@
         <v>82</v>
       </c>
       <c r="W27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X27" t="s">
         <v>76</v>
@@ -8031,31 +8358,39 @@
         <v>62</v>
       </c>
       <c r="AI27" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="AJ27" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="AK27" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL27" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM27" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>124</v>
+      </c>
+      <c r="AQ27" s="1">
         <v>3</v>
       </c>
-      <c r="AN27" s="1"/>
-      <c r="AO27" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP27" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ27" s="1"/>
       <c r="AR27" s="1"/>
-      <c r="AS27" s="1"/>
-      <c r="AT27" s="1"/>
+      <c r="AS27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>62</v>
+      </c>
       <c r="AU27" s="1"/>
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
@@ -8183,7 +8518,11 @@
       <c r="FO27" s="1"/>
       <c r="FP27" s="1"/>
       <c r="FQ27" s="1"/>
-      <c r="FR27" t="s">
+      <c r="FR27" s="1"/>
+      <c r="FS27" s="1"/>
+      <c r="FT27" s="1"/>
+      <c r="FU27" s="1"/>
+      <c r="FV27" t="s">
         <v>62</v>
       </c>
     </row>
@@ -8255,7 +8594,7 @@
         <v>82</v>
       </c>
       <c r="W28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X28" t="s">
         <v>76</v>
@@ -8291,31 +8630,39 @@
         <v>62</v>
       </c>
       <c r="AI28" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ28" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="AK28" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM28" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN28" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ28" s="1">
         <v>3</v>
       </c>
-      <c r="AN28" s="1"/>
-      <c r="AO28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
-      <c r="AS28" s="1"/>
-      <c r="AT28" s="1"/>
+      <c r="AS28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>62</v>
+      </c>
       <c r="AU28" s="1"/>
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
@@ -8443,8 +8790,12 @@
       <c r="FO28" s="1"/>
       <c r="FP28" s="1"/>
       <c r="FQ28" s="1"/>
-      <c r="FR28" t="s">
-        <v>263</v>
+      <c r="FR28" s="1"/>
+      <c r="FS28" s="1"/>
+      <c r="FT28" s="1"/>
+      <c r="FU28" s="1"/>
+      <c r="FV28" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="29">
@@ -8515,7 +8866,7 @@
         <v>82</v>
       </c>
       <c r="W29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X29" t="s">
         <v>76</v>
@@ -8551,31 +8902,39 @@
         <v>62</v>
       </c>
       <c r="AI29" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ29" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="AK29" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL29" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM29" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ29" s="1">
         <v>6</v>
       </c>
-      <c r="AN29" s="1"/>
-      <c r="AO29" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP29" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ29" s="1"/>
       <c r="AR29" s="1"/>
-      <c r="AS29" s="1"/>
-      <c r="AT29" s="1"/>
+      <c r="AS29" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT29" t="s">
+        <v>62</v>
+      </c>
       <c r="AU29" s="1"/>
       <c r="AV29" s="1"/>
       <c r="AW29" s="1"/>
@@ -8703,8 +9062,12 @@
       <c r="FO29" s="1"/>
       <c r="FP29" s="1"/>
       <c r="FQ29" s="1"/>
-      <c r="FR29" t="s">
-        <v>263</v>
+      <c r="FR29" s="1"/>
+      <c r="FS29" s="1"/>
+      <c r="FT29" s="1"/>
+      <c r="FU29" s="1"/>
+      <c r="FV29" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="30">
@@ -8775,7 +9138,7 @@
         <v>82</v>
       </c>
       <c r="W30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X30" t="s">
         <v>76</v>
@@ -8811,31 +9174,39 @@
         <v>62</v>
       </c>
       <c r="AI30" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ30" t="s">
         <v>62</v>
       </c>
       <c r="AK30" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL30" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM30" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ30" s="1">
         <v>12</v>
       </c>
-      <c r="AN30" s="1"/>
-      <c r="AO30" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP30" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ30" s="1"/>
       <c r="AR30" s="1"/>
-      <c r="AS30" s="1"/>
-      <c r="AT30" s="1"/>
+      <c r="AS30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>62</v>
+      </c>
       <c r="AU30" s="1"/>
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
@@ -8963,7 +9334,11 @@
       <c r="FO30" s="1"/>
       <c r="FP30" s="1"/>
       <c r="FQ30" s="1"/>
-      <c r="FR30" t="s">
+      <c r="FR30" s="1"/>
+      <c r="FS30" s="1"/>
+      <c r="FT30" s="1"/>
+      <c r="FU30" s="1"/>
+      <c r="FV30" t="s">
         <v>62</v>
       </c>
     </row>
@@ -9035,7 +9410,7 @@
         <v>82</v>
       </c>
       <c r="W31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X31" t="s">
         <v>76</v>
@@ -9071,31 +9446,39 @@
         <v>62</v>
       </c>
       <c r="AI31" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ31" t="s">
         <v>62</v>
       </c>
       <c r="AK31" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL31" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM31" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO31" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP31" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ31" s="1">
         <v>15</v>
       </c>
-      <c r="AN31" s="1"/>
-      <c r="AO31" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP31" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
-      <c r="AS31" s="1"/>
-      <c r="AT31" s="1"/>
+      <c r="AS31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>62</v>
+      </c>
       <c r="AU31" s="1"/>
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
@@ -9223,8 +9606,12 @@
       <c r="FO31" s="1"/>
       <c r="FP31" s="1"/>
       <c r="FQ31" s="1"/>
-      <c r="FR31" t="s">
-        <v>264</v>
+      <c r="FR31" s="1"/>
+      <c r="FS31" s="1"/>
+      <c r="FT31" s="1"/>
+      <c r="FU31" s="1"/>
+      <c r="FV31" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="32">
@@ -9295,7 +9682,7 @@
         <v>82</v>
       </c>
       <c r="W32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X32" t="s">
         <v>76</v>
@@ -9331,31 +9718,39 @@
         <v>62</v>
       </c>
       <c r="AI32" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ32" t="s">
         <v>62</v>
       </c>
       <c r="AK32" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL32" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM32" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN32" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO32" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP32" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ32" s="1">
         <v>11</v>
       </c>
-      <c r="AN32" s="1"/>
-      <c r="AO32" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP32" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ32" s="1"/>
       <c r="AR32" s="1"/>
-      <c r="AS32" s="1"/>
-      <c r="AT32" s="1"/>
+      <c r="AS32" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>62</v>
+      </c>
       <c r="AU32" s="1"/>
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
@@ -9483,8 +9878,12 @@
       <c r="FO32" s="1"/>
       <c r="FP32" s="1"/>
       <c r="FQ32" s="1"/>
-      <c r="FR32" t="s">
-        <v>265</v>
+      <c r="FR32" s="1"/>
+      <c r="FS32" s="1"/>
+      <c r="FT32" s="1"/>
+      <c r="FU32" s="1"/>
+      <c r="FV32" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="33">
@@ -9555,7 +9954,7 @@
         <v>82</v>
       </c>
       <c r="W33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X33" t="s">
         <v>76</v>
@@ -9591,31 +9990,39 @@
         <v>62</v>
       </c>
       <c r="AI33" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AJ33" t="s">
         <v>62</v>
       </c>
       <c r="AK33" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="AL33" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM33" s="1">
+        <v>62</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ33" s="1">
         <v>15</v>
       </c>
-      <c r="AN33" s="1"/>
-      <c r="AO33" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP33" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ33" s="1"/>
       <c r="AR33" s="1"/>
-      <c r="AS33" s="1"/>
-      <c r="AT33" s="1"/>
+      <c r="AS33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>62</v>
+      </c>
       <c r="AU33" s="1"/>
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
@@ -9743,8 +10150,12 @@
       <c r="FO33" s="1"/>
       <c r="FP33" s="1"/>
       <c r="FQ33" s="1"/>
-      <c r="FR33" t="s">
-        <v>264</v>
+      <c r="FR33" s="1"/>
+      <c r="FS33" s="1"/>
+      <c r="FT33" s="1"/>
+      <c r="FU33" s="1"/>
+      <c r="FV33" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="34">
@@ -9858,8 +10269,12 @@
       <c r="AL34" t="s">
         <v>62</v>
       </c>
-      <c r="AM34" s="1"/>
-      <c r="AN34" s="1"/>
+      <c r="AM34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN34" t="s">
+        <v>62</v>
+      </c>
       <c r="AO34" t="s">
         <v>62</v>
       </c>
@@ -9868,8 +10283,12 @@
       </c>
       <c r="AQ34" s="1"/>
       <c r="AR34" s="1"/>
-      <c r="AS34" s="1"/>
-      <c r="AT34" s="1"/>
+      <c r="AS34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>62</v>
+      </c>
       <c r="AU34" s="1"/>
       <c r="AV34" s="1"/>
       <c r="AW34" s="1"/>
@@ -9997,7 +10416,11 @@
       <c r="FO34" s="1"/>
       <c r="FP34" s="1"/>
       <c r="FQ34" s="1"/>
-      <c r="FR34" t="s">
+      <c r="FR34" s="1"/>
+      <c r="FS34" s="1"/>
+      <c r="FT34" s="1"/>
+      <c r="FU34" s="1"/>
+      <c r="FV34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -10112,8 +10535,12 @@
       <c r="AL35" t="s">
         <v>62</v>
       </c>
-      <c r="AM35" s="1"/>
-      <c r="AN35" s="1"/>
+      <c r="AM35" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN35" t="s">
+        <v>62</v>
+      </c>
       <c r="AO35" t="s">
         <v>62</v>
       </c>
@@ -10122,8 +10549,12 @@
       </c>
       <c r="AQ35" s="1"/>
       <c r="AR35" s="1"/>
-      <c r="AS35" s="1"/>
-      <c r="AT35" s="1"/>
+      <c r="AS35" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>62</v>
+      </c>
       <c r="AU35" s="1"/>
       <c r="AV35" s="1"/>
       <c r="AW35" s="1"/>
@@ -10251,7 +10682,11 @@
       <c r="FO35" s="1"/>
       <c r="FP35" s="1"/>
       <c r="FQ35" s="1"/>
-      <c r="FR35" t="s">
+      <c r="FR35" s="1"/>
+      <c r="FS35" s="1"/>
+      <c r="FT35" s="1"/>
+      <c r="FU35" s="1"/>
+      <c r="FV35" t="s">
         <v>62</v>
       </c>
     </row>
@@ -10366,8 +10801,12 @@
       <c r="AL36" t="s">
         <v>62</v>
       </c>
-      <c r="AM36" s="1"/>
-      <c r="AN36" s="1"/>
+      <c r="AM36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN36" t="s">
+        <v>62</v>
+      </c>
       <c r="AO36" t="s">
         <v>62</v>
       </c>
@@ -10376,8 +10815,12 @@
       </c>
       <c r="AQ36" s="1"/>
       <c r="AR36" s="1"/>
-      <c r="AS36" s="1"/>
-      <c r="AT36" s="1"/>
+      <c r="AS36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>62</v>
+      </c>
       <c r="AU36" s="1"/>
       <c r="AV36" s="1"/>
       <c r="AW36" s="1"/>
@@ -10505,7 +10948,11 @@
       <c r="FO36" s="1"/>
       <c r="FP36" s="1"/>
       <c r="FQ36" s="1"/>
-      <c r="FR36" t="s">
+      <c r="FR36" s="1"/>
+      <c r="FS36" s="1"/>
+      <c r="FT36" s="1"/>
+      <c r="FU36" s="1"/>
+      <c r="FV36" t="s">
         <v>62</v>
       </c>
     </row>
@@ -10620,8 +11067,12 @@
       <c r="AL37" t="s">
         <v>62</v>
       </c>
-      <c r="AM37" s="1"/>
-      <c r="AN37" s="1"/>
+      <c r="AM37" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>62</v>
+      </c>
       <c r="AO37" t="s">
         <v>62</v>
       </c>
@@ -10630,8 +11081,12 @@
       </c>
       <c r="AQ37" s="1"/>
       <c r="AR37" s="1"/>
-      <c r="AS37" s="1"/>
-      <c r="AT37" s="1"/>
+      <c r="AS37" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>62</v>
+      </c>
       <c r="AU37" s="1"/>
       <c r="AV37" s="1"/>
       <c r="AW37" s="1"/>
@@ -10759,7 +11214,11 @@
       <c r="FO37" s="1"/>
       <c r="FP37" s="1"/>
       <c r="FQ37" s="1"/>
-      <c r="FR37" t="s">
+      <c r="FR37" s="1"/>
+      <c r="FS37" s="1"/>
+      <c r="FT37" s="1"/>
+      <c r="FU37" s="1"/>
+      <c r="FV37" t="s">
         <v>62</v>
       </c>
     </row>
@@ -10874,8 +11333,12 @@
       <c r="AL38" t="s">
         <v>62</v>
       </c>
-      <c r="AM38" s="1"/>
-      <c r="AN38" s="1"/>
+      <c r="AM38" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN38" t="s">
+        <v>62</v>
+      </c>
       <c r="AO38" t="s">
         <v>62</v>
       </c>
@@ -10884,8 +11347,12 @@
       </c>
       <c r="AQ38" s="1"/>
       <c r="AR38" s="1"/>
-      <c r="AS38" s="1"/>
-      <c r="AT38" s="1"/>
+      <c r="AS38" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>62</v>
+      </c>
       <c r="AU38" s="1"/>
       <c r="AV38" s="1"/>
       <c r="AW38" s="1"/>
@@ -11013,7 +11480,11 @@
       <c r="FO38" s="1"/>
       <c r="FP38" s="1"/>
       <c r="FQ38" s="1"/>
-      <c r="FR38" t="s">
+      <c r="FR38" s="1"/>
+      <c r="FS38" s="1"/>
+      <c r="FT38" s="1"/>
+      <c r="FU38" s="1"/>
+      <c r="FV38" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11069,16 +11540,16 @@
         <v>82</v>
       </c>
       <c r="S39" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="T39" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="U39" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="V39" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="W39" t="s">
         <v>62</v>
@@ -11128,8 +11599,12 @@
       <c r="AL39" t="s">
         <v>62</v>
       </c>
-      <c r="AM39" s="1"/>
-      <c r="AN39" s="1"/>
+      <c r="AM39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>62</v>
+      </c>
       <c r="AO39" t="s">
         <v>62</v>
       </c>
@@ -11138,8 +11613,12 @@
       </c>
       <c r="AQ39" s="1"/>
       <c r="AR39" s="1"/>
-      <c r="AS39" s="1"/>
-      <c r="AT39" s="1"/>
+      <c r="AS39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>62</v>
+      </c>
       <c r="AU39" s="1"/>
       <c r="AV39" s="1"/>
       <c r="AW39" s="1"/>
@@ -11267,7 +11746,11 @@
       <c r="FO39" s="1"/>
       <c r="FP39" s="1"/>
       <c r="FQ39" s="1"/>
-      <c r="FR39" t="s">
+      <c r="FR39" s="1"/>
+      <c r="FS39" s="1"/>
+      <c r="FT39" s="1"/>
+      <c r="FU39" s="1"/>
+      <c r="FV39" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11323,16 +11806,16 @@
         <v>82</v>
       </c>
       <c r="S40" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="T40" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="U40" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="V40" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="W40" t="s">
         <v>62</v>
@@ -11382,8 +11865,12 @@
       <c r="AL40" t="s">
         <v>62</v>
       </c>
-      <c r="AM40" s="1"/>
-      <c r="AN40" s="1"/>
+      <c r="AM40" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN40" t="s">
+        <v>62</v>
+      </c>
       <c r="AO40" t="s">
         <v>62</v>
       </c>
@@ -11392,8 +11879,12 @@
       </c>
       <c r="AQ40" s="1"/>
       <c r="AR40" s="1"/>
-      <c r="AS40" s="1"/>
-      <c r="AT40" s="1"/>
+      <c r="AS40" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>62</v>
+      </c>
       <c r="AU40" s="1"/>
       <c r="AV40" s="1"/>
       <c r="AW40" s="1"/>
@@ -11521,7 +12012,11 @@
       <c r="FO40" s="1"/>
       <c r="FP40" s="1"/>
       <c r="FQ40" s="1"/>
-      <c r="FR40" t="s">
+      <c r="FR40" s="1"/>
+      <c r="FS40" s="1"/>
+      <c r="FT40" s="1"/>
+      <c r="FU40" s="1"/>
+      <c r="FV40" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11577,16 +12072,16 @@
         <v>82</v>
       </c>
       <c r="S41" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="T41" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="U41" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="V41" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="W41" t="s">
         <v>62</v>
@@ -11636,8 +12131,12 @@
       <c r="AL41" t="s">
         <v>62</v>
       </c>
-      <c r="AM41" s="1"/>
-      <c r="AN41" s="1"/>
+      <c r="AM41" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN41" t="s">
+        <v>62</v>
+      </c>
       <c r="AO41" t="s">
         <v>62</v>
       </c>
@@ -11646,8 +12145,12 @@
       </c>
       <c r="AQ41" s="1"/>
       <c r="AR41" s="1"/>
-      <c r="AS41" s="1"/>
-      <c r="AT41" s="1"/>
+      <c r="AS41" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>62</v>
+      </c>
       <c r="AU41" s="1"/>
       <c r="AV41" s="1"/>
       <c r="AW41" s="1"/>
@@ -11775,7 +12278,11 @@
       <c r="FO41" s="1"/>
       <c r="FP41" s="1"/>
       <c r="FQ41" s="1"/>
-      <c r="FR41" t="s">
+      <c r="FR41" s="1"/>
+      <c r="FS41" s="1"/>
+      <c r="FT41" s="1"/>
+      <c r="FU41" s="1"/>
+      <c r="FV41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11831,16 +12338,16 @@
         <v>82</v>
       </c>
       <c r="S42" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="T42" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="U42" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="V42" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="W42" t="s">
         <v>62</v>
@@ -11890,8 +12397,12 @@
       <c r="AL42" t="s">
         <v>62</v>
       </c>
-      <c r="AM42" s="1"/>
-      <c r="AN42" s="1"/>
+      <c r="AM42" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN42" t="s">
+        <v>62</v>
+      </c>
       <c r="AO42" t="s">
         <v>62</v>
       </c>
@@ -11900,8 +12411,12 @@
       </c>
       <c r="AQ42" s="1"/>
       <c r="AR42" s="1"/>
-      <c r="AS42" s="1"/>
-      <c r="AT42" s="1"/>
+      <c r="AS42" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT42" t="s">
+        <v>62</v>
+      </c>
       <c r="AU42" s="1"/>
       <c r="AV42" s="1"/>
       <c r="AW42" s="1"/>
@@ -12029,7 +12544,11 @@
       <c r="FO42" s="1"/>
       <c r="FP42" s="1"/>
       <c r="FQ42" s="1"/>
-      <c r="FR42" t="s">
+      <c r="FR42" s="1"/>
+      <c r="FS42" s="1"/>
+      <c r="FT42" s="1"/>
+      <c r="FU42" s="1"/>
+      <c r="FV42" t="s">
         <v>62</v>
       </c>
     </row>
@@ -12085,16 +12604,16 @@
         <v>82</v>
       </c>
       <c r="S43" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="T43" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="U43" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="V43" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="W43" t="s">
         <v>62</v>
@@ -12144,8 +12663,12 @@
       <c r="AL43" t="s">
         <v>62</v>
       </c>
-      <c r="AM43" s="1"/>
-      <c r="AN43" s="1"/>
+      <c r="AM43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>62</v>
+      </c>
       <c r="AO43" t="s">
         <v>62</v>
       </c>
@@ -12154,8 +12677,12 @@
       </c>
       <c r="AQ43" s="1"/>
       <c r="AR43" s="1"/>
-      <c r="AS43" s="1"/>
-      <c r="AT43" s="1"/>
+      <c r="AS43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT43" t="s">
+        <v>62</v>
+      </c>
       <c r="AU43" s="1"/>
       <c r="AV43" s="1"/>
       <c r="AW43" s="1"/>
@@ -12283,7 +12810,11 @@
       <c r="FO43" s="1"/>
       <c r="FP43" s="1"/>
       <c r="FQ43" s="1"/>
-      <c r="FR43" t="s">
+      <c r="FR43" s="1"/>
+      <c r="FS43" s="1"/>
+      <c r="FT43" s="1"/>
+      <c r="FU43" s="1"/>
+      <c r="FV43" t="s">
         <v>62</v>
       </c>
     </row>
@@ -12390,8 +12921,12 @@
       <c r="AL44" t="s">
         <v>62</v>
       </c>
-      <c r="AM44" s="1"/>
-      <c r="AN44" s="1"/>
+      <c r="AM44" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN44" t="s">
+        <v>62</v>
+      </c>
       <c r="AO44" t="s">
         <v>62</v>
       </c>
@@ -12400,8 +12935,12 @@
       </c>
       <c r="AQ44" s="1"/>
       <c r="AR44" s="1"/>
-      <c r="AS44" s="1"/>
-      <c r="AT44" s="1"/>
+      <c r="AS44" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT44" t="s">
+        <v>62</v>
+      </c>
       <c r="AU44" s="1"/>
       <c r="AV44" s="1"/>
       <c r="AW44" s="1"/>
@@ -12529,8 +13068,12 @@
       <c r="FO44" s="1"/>
       <c r="FP44" s="1"/>
       <c r="FQ44" s="1"/>
-      <c r="FR44" t="s">
-        <v>266</v>
+      <c r="FR44" s="1"/>
+      <c r="FS44" s="1"/>
+      <c r="FT44" s="1"/>
+      <c r="FU44" s="1"/>
+      <c r="FV44" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="45">
@@ -12636,8 +13179,12 @@
       <c r="AL45" t="s">
         <v>62</v>
       </c>
-      <c r="AM45" s="1"/>
-      <c r="AN45" s="1"/>
+      <c r="AM45" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN45" t="s">
+        <v>62</v>
+      </c>
       <c r="AO45" t="s">
         <v>62</v>
       </c>
@@ -12646,8 +13193,12 @@
       </c>
       <c r="AQ45" s="1"/>
       <c r="AR45" s="1"/>
-      <c r="AS45" s="1"/>
-      <c r="AT45" s="1"/>
+      <c r="AS45" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>62</v>
+      </c>
       <c r="AU45" s="1"/>
       <c r="AV45" s="1"/>
       <c r="AW45" s="1"/>
@@ -12775,8 +13326,12 @@
       <c r="FO45" s="1"/>
       <c r="FP45" s="1"/>
       <c r="FQ45" s="1"/>
-      <c r="FR45" t="s">
-        <v>266</v>
+      <c r="FR45" s="1"/>
+      <c r="FS45" s="1"/>
+      <c r="FT45" s="1"/>
+      <c r="FU45" s="1"/>
+      <c r="FV45" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="46">
@@ -12882,8 +13437,12 @@
       <c r="AL46" t="s">
         <v>62</v>
       </c>
-      <c r="AM46" s="1"/>
-      <c r="AN46" s="1"/>
+      <c r="AM46" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN46" t="s">
+        <v>62</v>
+      </c>
       <c r="AO46" t="s">
         <v>62</v>
       </c>
@@ -12892,8 +13451,12 @@
       </c>
       <c r="AQ46" s="1"/>
       <c r="AR46" s="1"/>
-      <c r="AS46" s="1"/>
-      <c r="AT46" s="1"/>
+      <c r="AS46" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT46" t="s">
+        <v>62</v>
+      </c>
       <c r="AU46" s="1"/>
       <c r="AV46" s="1"/>
       <c r="AW46" s="1"/>
@@ -13021,7 +13584,11 @@
       <c r="FO46" s="1"/>
       <c r="FP46" s="1"/>
       <c r="FQ46" s="1"/>
-      <c r="FR46" t="s">
+      <c r="FR46" s="1"/>
+      <c r="FS46" s="1"/>
+      <c r="FT46" s="1"/>
+      <c r="FU46" s="1"/>
+      <c r="FV46" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to 2024 crop and sales data
</commit_message>
<xml_diff>
--- a/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
+++ b/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="4988" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="5284" uniqueCount="351">
   <si>
     <t>crop</t>
   </si>
@@ -549,6 +549,9 @@
     <t>1-3-1</t>
   </si>
   <si>
+    <t>0-0-17</t>
+  </si>
+  <si>
     <t>fert_type_name_2</t>
   </si>
   <si>
@@ -558,6 +561,9 @@
     <t>Espoma- Organic Tomato! (liquid)</t>
   </si>
   <si>
+    <t>MaxiCrop Soluble Seaweed</t>
+  </si>
+  <si>
     <t>fert_date_2</t>
   </si>
   <si>
@@ -570,12 +576,18 @@
     <t>09jul2024</t>
   </si>
   <si>
+    <t>2024-07-28</t>
+  </si>
+  <si>
     <t>fert_amnt_per_2</t>
   </si>
   <si>
     <t>fert_unit_2</t>
   </si>
   <si>
+    <t>gallon</t>
+  </si>
+  <si>
     <t>fert_type_npk_3</t>
   </si>
   <si>
@@ -717,6 +729,9 @@
     <t>2024-06-15</t>
   </si>
   <si>
+    <t>2024-07-27</t>
+  </si>
+  <si>
     <t>2024-06-29</t>
   </si>
   <si>
@@ -744,6 +759,9 @@
     <t>2024-06-22</t>
   </si>
   <si>
+    <t>2024-07-25</t>
+  </si>
+  <si>
     <t>harvest_amnt_2</t>
   </si>
   <si>
@@ -769,9 +787,6 @@
   </si>
   <si>
     <t>harvest_date_5</t>
-  </si>
-  <si>
-    <t>2024-07-25</t>
   </si>
   <si>
     <t>harvest_amnt_5</t>
@@ -1268,376 +1283,376 @@
         <v>175</v>
       </c>
       <c r="BC1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="BD1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="BE1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="BF1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="BG1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="BH1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="BI1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="BJ1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="BK1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="BL1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="BM1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="BN1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="BO1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BP1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="BQ1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="BR1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="BS1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="BT1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="BU1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="BV1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="BW1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="BX1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="BY1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="BZ1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="CA1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="CB1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="CC1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="CD1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="CE1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="CF1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="CG1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="CH1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="CI1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="CJ1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="CK1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="CL1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="CM1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="CN1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="CO1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="CP1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="CQ1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="CR1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="CS1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="CT1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="CU1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="CV1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="CW1" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="CX1" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="CY1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="CZ1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="DA1" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="DB1" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="DC1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="DD1" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="DE1" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="DF1" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="DG1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="DH1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="DI1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="DJ1" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="DK1" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="DL1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="DM1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="DN1" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="DO1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="DP1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="DQ1" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="DR1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="DS1" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="DT1" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="DU1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="DV1" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="DW1" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="DX1" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="DY1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="DZ1" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="EA1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="EB1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="EC1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="ED1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="EE1" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="EF1" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="EG1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="EH1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="EI1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="EJ1" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="EK1" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="EL1" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="EM1" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="EN1" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="EO1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="EP1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="EQ1" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="ER1" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="ES1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="ET1" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="EU1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="EV1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="EW1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="EX1" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="EY1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="EZ1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="FA1" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="FB1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="FC1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="FD1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="FE1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="FF1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="FG1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="FH1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="FI1" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="FJ1" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="FK1" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="FL1" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="FM1" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="FN1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="FO1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="FP1" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="FQ1" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="FR1" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="FS1" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="FT1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="FU1" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="FV1" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
@@ -1851,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="CL2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM2" t="s">
         <v>63</v>
@@ -1860,7 +1875,7 @@
         <v>29</v>
       </c>
       <c r="CO2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP2" t="s">
         <v>77</v>
@@ -1883,12 +1898,20 @@
       <c r="CX2" t="s">
         <v>77</v>
       </c>
-      <c r="CY2" s="1"/>
+      <c r="CY2" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ2" s="1"/>
-      <c r="DA2" s="1"/>
-      <c r="DB2" s="1"/>
+      <c r="DA2" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>77</v>
+      </c>
       <c r="DC2" s="1"/>
-      <c r="DD2" s="1"/>
+      <c r="DD2" t="s">
+        <v>77</v>
+      </c>
       <c r="DE2" s="1"/>
       <c r="DF2" s="1"/>
       <c r="DG2" s="1"/>
@@ -2127,7 +2150,7 @@
         <v>94</v>
       </c>
       <c r="BD3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="BE3" s="1">
         <v>1</v>
@@ -2217,12 +2240,20 @@
       <c r="CX3" t="s">
         <v>77</v>
       </c>
-      <c r="CY3" s="1"/>
+      <c r="CY3" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
+      <c r="DA3" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>77</v>
+      </c>
       <c r="DC3" s="1"/>
-      <c r="DD3" s="1"/>
+      <c r="DD3" t="s">
+        <v>77</v>
+      </c>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
       <c r="DG3" s="1"/>
@@ -2543,12 +2574,20 @@
       <c r="CX4" t="s">
         <v>77</v>
       </c>
-      <c r="CY4" s="1"/>
+      <c r="CY4" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ4" s="1"/>
-      <c r="DA4" s="1"/>
-      <c r="DB4" s="1"/>
+      <c r="DA4" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB4" t="s">
+        <v>77</v>
+      </c>
       <c r="DC4" s="1"/>
-      <c r="DD4" s="1"/>
+      <c r="DD4" t="s">
+        <v>77</v>
+      </c>
       <c r="DE4" s="1"/>
       <c r="DF4" s="1"/>
       <c r="DG4" s="1"/>
@@ -2875,12 +2914,20 @@
       <c r="CX5" t="s">
         <v>77</v>
       </c>
-      <c r="CY5" s="1"/>
+      <c r="CY5" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ5" s="1"/>
-      <c r="DA5" s="1"/>
-      <c r="DB5" s="1"/>
+      <c r="DA5" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB5" t="s">
+        <v>77</v>
+      </c>
       <c r="DC5" s="1"/>
-      <c r="DD5" s="1"/>
+      <c r="DD5" t="s">
+        <v>77</v>
+      </c>
       <c r="DE5" s="1"/>
       <c r="DF5" s="1"/>
       <c r="DG5" s="1"/>
@@ -3207,12 +3254,20 @@
       <c r="CX6" t="s">
         <v>77</v>
       </c>
-      <c r="CY6" s="1"/>
+      <c r="CY6" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ6" s="1"/>
-      <c r="DA6" s="1"/>
-      <c r="DB6" s="1"/>
+      <c r="DA6" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB6" t="s">
+        <v>77</v>
+      </c>
       <c r="DC6" s="1"/>
-      <c r="DD6" s="1"/>
+      <c r="DD6" t="s">
+        <v>77</v>
+      </c>
       <c r="DE6" s="1"/>
       <c r="DF6" s="1"/>
       <c r="DG6" s="1"/>
@@ -3539,12 +3594,20 @@
       <c r="CX7" t="s">
         <v>77</v>
       </c>
-      <c r="CY7" s="1"/>
+      <c r="CY7" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ7" s="1"/>
-      <c r="DA7" s="1"/>
-      <c r="DB7" s="1"/>
+      <c r="DA7" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB7" t="s">
+        <v>77</v>
+      </c>
       <c r="DC7" s="1"/>
-      <c r="DD7" s="1"/>
+      <c r="DD7" t="s">
+        <v>77</v>
+      </c>
       <c r="DE7" s="1"/>
       <c r="DF7" s="1"/>
       <c r="DG7" s="1"/>
@@ -3871,12 +3934,20 @@
       <c r="CX8" t="s">
         <v>77</v>
       </c>
-      <c r="CY8" s="1"/>
+      <c r="CY8" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ8" s="1"/>
-      <c r="DA8" s="1"/>
-      <c r="DB8" s="1"/>
+      <c r="DA8" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB8" t="s">
+        <v>77</v>
+      </c>
       <c r="DC8" s="1"/>
-      <c r="DD8" s="1"/>
+      <c r="DD8" t="s">
+        <v>77</v>
+      </c>
       <c r="DE8" s="1"/>
       <c r="DF8" s="1"/>
       <c r="DG8" s="1"/>
@@ -4135,13 +4206,13 @@
         <v>77</v>
       </c>
       <c r="BL9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="BM9" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="BN9" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BO9" s="2"/>
       <c r="BP9" s="1"/>
@@ -4149,13 +4220,13 @@
       <c r="BR9" s="1"/>
       <c r="BS9" s="1"/>
       <c r="BT9" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="BU9" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="BV9" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW9" s="2"/>
       <c r="BX9" s="1"/>
@@ -4177,14 +4248,16 @@
         <v>5</v>
       </c>
       <c r="CL9" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM9" t="s">
-        <v>77</v>
-      </c>
-      <c r="CN9" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="CN9" s="1">
+        <v>5</v>
+      </c>
       <c r="CO9" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="CP9" t="s">
         <v>77</v>
@@ -4207,12 +4280,20 @@
       <c r="CX9" t="s">
         <v>77</v>
       </c>
-      <c r="CY9" s="1"/>
+      <c r="CY9" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ9" s="1"/>
-      <c r="DA9" s="1"/>
-      <c r="DB9" s="1"/>
+      <c r="DA9" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB9" t="s">
+        <v>77</v>
+      </c>
       <c r="DC9" s="1"/>
-      <c r="DD9" s="1"/>
+      <c r="DD9" t="s">
+        <v>77</v>
+      </c>
       <c r="DE9" s="1"/>
       <c r="DF9" s="1"/>
       <c r="DG9" s="1"/>
@@ -4283,7 +4364,7 @@
       <c r="FT9" s="1"/>
       <c r="FU9" s="1"/>
       <c r="FV9" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10">
@@ -4450,10 +4531,10 @@
         <v>176</v>
       </c>
       <c r="BC10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE10" s="1">
         <v>3</v>
@@ -4509,31 +4590,31 @@
       <c r="CH10" s="1"/>
       <c r="CI10" s="1"/>
       <c r="CJ10" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="CK10" s="1">
         <v>4</v>
       </c>
       <c r="CL10" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM10" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CN10" s="1">
         <v>2</v>
       </c>
       <c r="CO10" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP10" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="CQ10" s="1">
         <v>6</v>
       </c>
       <c r="CR10" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CS10" t="s">
         <v>77</v>
@@ -4549,12 +4630,20 @@
       <c r="CX10" t="s">
         <v>77</v>
       </c>
-      <c r="CY10" s="1"/>
+      <c r="CY10" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ10" s="1"/>
-      <c r="DA10" s="1"/>
-      <c r="DB10" s="1"/>
+      <c r="DA10" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB10" t="s">
+        <v>77</v>
+      </c>
       <c r="DC10" s="1"/>
-      <c r="DD10" s="1"/>
+      <c r="DD10" t="s">
+        <v>77</v>
+      </c>
       <c r="DE10" s="1"/>
       <c r="DF10" s="1"/>
       <c r="DG10" s="1"/>
@@ -4625,7 +4714,7 @@
       <c r="FT10" s="1"/>
       <c r="FU10" s="1"/>
       <c r="FV10" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11">
@@ -4792,10 +4881,10 @@
         <v>176</v>
       </c>
       <c r="BC11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD11" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE11" s="1">
         <v>3</v>
@@ -4885,12 +4974,20 @@
       <c r="CX11" t="s">
         <v>77</v>
       </c>
-      <c r="CY11" s="1"/>
+      <c r="CY11" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ11" s="1"/>
-      <c r="DA11" s="1"/>
-      <c r="DB11" s="1"/>
+      <c r="DA11" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB11" t="s">
+        <v>77</v>
+      </c>
       <c r="DC11" s="1"/>
-      <c r="DD11" s="1"/>
+      <c r="DD11" t="s">
+        <v>77</v>
+      </c>
       <c r="DE11" s="1"/>
       <c r="DF11" s="1"/>
       <c r="DG11" s="1"/>
@@ -4961,7 +5058,7 @@
       <c r="FT11" s="1"/>
       <c r="FU11" s="1"/>
       <c r="FV11" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12">
@@ -5128,10 +5225,10 @@
         <v>176</v>
       </c>
       <c r="BC12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD12" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE12" s="1">
         <v>3</v>
@@ -5187,13 +5284,13 @@
       <c r="CH12" s="1"/>
       <c r="CI12" s="1"/>
       <c r="CJ12" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CK12" s="1">
         <v>4</v>
       </c>
       <c r="CL12" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CM12" t="s">
         <v>165</v>
@@ -5202,16 +5299,16 @@
         <v>4</v>
       </c>
       <c r="CO12" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CP12" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="CQ12" s="1">
         <v>7</v>
       </c>
       <c r="CR12" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CS12" t="s">
         <v>77</v>
@@ -5227,12 +5324,20 @@
       <c r="CX12" t="s">
         <v>77</v>
       </c>
-      <c r="CY12" s="1"/>
+      <c r="CY12" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ12" s="1"/>
-      <c r="DA12" s="1"/>
-      <c r="DB12" s="1"/>
+      <c r="DA12" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB12" t="s">
+        <v>77</v>
+      </c>
       <c r="DC12" s="1"/>
-      <c r="DD12" s="1"/>
+      <c r="DD12" t="s">
+        <v>77</v>
+      </c>
       <c r="DE12" s="1"/>
       <c r="DF12" s="1"/>
       <c r="DG12" s="1"/>
@@ -5303,7 +5408,7 @@
       <c r="FT12" s="1"/>
       <c r="FU12" s="1"/>
       <c r="FV12" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13">
@@ -5470,10 +5575,10 @@
         <v>176</v>
       </c>
       <c r="BC13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD13" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE13" s="1">
         <v>3</v>
@@ -5529,13 +5634,13 @@
       <c r="CH13" s="1"/>
       <c r="CI13" s="1"/>
       <c r="CJ13" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CK13" s="1">
         <v>12</v>
       </c>
       <c r="CL13" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CM13" t="s">
         <v>165</v>
@@ -5544,23 +5649,23 @@
         <v>8</v>
       </c>
       <c r="CO13" t="s">
+        <v>243</v>
+      </c>
+      <c r="CP13" t="s">
+        <v>246</v>
+      </c>
+      <c r="CQ13" s="1">
+        <v>10</v>
+      </c>
+      <c r="CR13" t="s">
+        <v>243</v>
+      </c>
+      <c r="CS13" t="s">
         <v>238</v>
-      </c>
-      <c r="CP13" t="s">
-        <v>241</v>
-      </c>
-      <c r="CQ13" s="1">
-        <v>16</v>
-      </c>
-      <c r="CR13" t="s">
-        <v>238</v>
-      </c>
-      <c r="CS13" t="s">
-        <v>77</v>
       </c>
       <c r="CT13" s="1"/>
       <c r="CU13" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CV13" t="s">
         <v>77</v>
@@ -5569,12 +5674,20 @@
       <c r="CX13" t="s">
         <v>77</v>
       </c>
-      <c r="CY13" s="1"/>
+      <c r="CY13" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ13" s="1"/>
-      <c r="DA13" s="1"/>
-      <c r="DB13" s="1"/>
+      <c r="DA13" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB13" t="s">
+        <v>77</v>
+      </c>
       <c r="DC13" s="1"/>
-      <c r="DD13" s="1"/>
+      <c r="DD13" t="s">
+        <v>77</v>
+      </c>
       <c r="DE13" s="1"/>
       <c r="DF13" s="1"/>
       <c r="DG13" s="1"/>
@@ -5645,7 +5758,7 @@
       <c r="FT13" s="1"/>
       <c r="FU13" s="1"/>
       <c r="FV13" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14">
@@ -5812,10 +5925,10 @@
         <v>176</v>
       </c>
       <c r="BC14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD14" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE14" s="1">
         <v>3</v>
@@ -5871,13 +5984,13 @@
       <c r="CH14" s="1"/>
       <c r="CI14" s="1"/>
       <c r="CJ14" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CK14" s="1">
         <v>1</v>
       </c>
       <c r="CL14" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="CM14" t="s">
         <v>165</v>
@@ -5886,16 +5999,16 @@
         <v>8</v>
       </c>
       <c r="CO14" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CP14" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="CQ14" s="1">
         <v>5</v>
       </c>
       <c r="CR14" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CS14" t="s">
         <v>77</v>
@@ -5911,12 +6024,20 @@
       <c r="CX14" t="s">
         <v>77</v>
       </c>
-      <c r="CY14" s="1"/>
+      <c r="CY14" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ14" s="1"/>
-      <c r="DA14" s="1"/>
-      <c r="DB14" s="1"/>
+      <c r="DA14" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB14" t="s">
+        <v>77</v>
+      </c>
       <c r="DC14" s="1"/>
-      <c r="DD14" s="1"/>
+      <c r="DD14" t="s">
+        <v>77</v>
+      </c>
       <c r="DE14" s="1"/>
       <c r="DF14" s="1"/>
       <c r="DG14" s="1"/>
@@ -5987,7 +6108,7 @@
       <c r="FT14" s="1"/>
       <c r="FU14" s="1"/>
       <c r="FV14" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15">
@@ -6154,10 +6275,10 @@
         <v>176</v>
       </c>
       <c r="BC15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE15" s="1">
         <v>3</v>
@@ -6219,16 +6340,16 @@
         <v>2</v>
       </c>
       <c r="CL15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CM15" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="CN15" s="1">
         <v>3</v>
       </c>
       <c r="CO15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CP15" t="s">
         <v>77</v>
@@ -6251,12 +6372,20 @@
       <c r="CX15" t="s">
         <v>77</v>
       </c>
-      <c r="CY15" s="1"/>
+      <c r="CY15" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ15" s="1"/>
-      <c r="DA15" s="1"/>
-      <c r="DB15" s="1"/>
+      <c r="DA15" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB15" t="s">
+        <v>77</v>
+      </c>
       <c r="DC15" s="1"/>
-      <c r="DD15" s="1"/>
+      <c r="DD15" t="s">
+        <v>77</v>
+      </c>
       <c r="DE15" s="1"/>
       <c r="DF15" s="1"/>
       <c r="DG15" s="1"/>
@@ -6327,7 +6456,7 @@
       <c r="FT15" s="1"/>
       <c r="FU15" s="1"/>
       <c r="FV15" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16">
@@ -6494,10 +6623,10 @@
         <v>176</v>
       </c>
       <c r="BC16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE16" s="1">
         <v>3</v>
@@ -6587,12 +6716,20 @@
       <c r="CX16" t="s">
         <v>77</v>
       </c>
-      <c r="CY16" s="1"/>
+      <c r="CY16" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ16" s="1"/>
-      <c r="DA16" s="1"/>
-      <c r="DB16" s="1"/>
+      <c r="DA16" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB16" t="s">
+        <v>77</v>
+      </c>
       <c r="DC16" s="1"/>
-      <c r="DD16" s="1"/>
+      <c r="DD16" t="s">
+        <v>77</v>
+      </c>
       <c r="DE16" s="1"/>
       <c r="DF16" s="1"/>
       <c r="DG16" s="1"/>
@@ -6663,7 +6800,7 @@
       <c r="FT16" s="1"/>
       <c r="FU16" s="1"/>
       <c r="FV16" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17">
@@ -6830,10 +6967,10 @@
         <v>176</v>
       </c>
       <c r="BC17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD17" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE17" s="1">
         <v>3</v>
@@ -6923,12 +7060,20 @@
       <c r="CX17" t="s">
         <v>77</v>
       </c>
-      <c r="CY17" s="1"/>
+      <c r="CY17" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ17" s="1"/>
-      <c r="DA17" s="1"/>
-      <c r="DB17" s="1"/>
+      <c r="DA17" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB17" t="s">
+        <v>77</v>
+      </c>
       <c r="DC17" s="1"/>
-      <c r="DD17" s="1"/>
+      <c r="DD17" t="s">
+        <v>77</v>
+      </c>
       <c r="DE17" s="1"/>
       <c r="DF17" s="1"/>
       <c r="DG17" s="1"/>
@@ -6999,7 +7144,7 @@
       <c r="FT17" s="1"/>
       <c r="FU17" s="1"/>
       <c r="FV17" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18">
@@ -7166,10 +7311,10 @@
         <v>176</v>
       </c>
       <c r="BC18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD18" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE18" s="1">
         <v>3</v>
@@ -7259,12 +7404,20 @@
       <c r="CX18" t="s">
         <v>77</v>
       </c>
-      <c r="CY18" s="1"/>
+      <c r="CY18" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ18" s="1"/>
-      <c r="DA18" s="1"/>
-      <c r="DB18" s="1"/>
+      <c r="DA18" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB18" t="s">
+        <v>77</v>
+      </c>
       <c r="DC18" s="1"/>
-      <c r="DD18" s="1"/>
+      <c r="DD18" t="s">
+        <v>77</v>
+      </c>
       <c r="DE18" s="1"/>
       <c r="DF18" s="1"/>
       <c r="DG18" s="1"/>
@@ -7335,7 +7488,7 @@
       <c r="FT18" s="1"/>
       <c r="FU18" s="1"/>
       <c r="FV18" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19">
@@ -7502,10 +7655,10 @@
         <v>176</v>
       </c>
       <c r="BC19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD19" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE19" s="1">
         <v>3</v>
@@ -7595,12 +7748,20 @@
       <c r="CX19" t="s">
         <v>77</v>
       </c>
-      <c r="CY19" s="1"/>
+      <c r="CY19" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ19" s="1"/>
-      <c r="DA19" s="1"/>
-      <c r="DB19" s="1"/>
+      <c r="DA19" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB19" t="s">
+        <v>77</v>
+      </c>
       <c r="DC19" s="1"/>
-      <c r="DD19" s="1"/>
+      <c r="DD19" t="s">
+        <v>77</v>
+      </c>
       <c r="DE19" s="1"/>
       <c r="DF19" s="1"/>
       <c r="DG19" s="1"/>
@@ -7671,7 +7832,7 @@
       <c r="FT19" s="1"/>
       <c r="FU19" s="1"/>
       <c r="FV19" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20">
@@ -7838,10 +7999,10 @@
         <v>176</v>
       </c>
       <c r="BC20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BD20" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="BE20" s="1">
         <v>3</v>
@@ -7931,12 +8092,20 @@
       <c r="CX20" t="s">
         <v>77</v>
       </c>
-      <c r="CY20" s="1"/>
+      <c r="CY20" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ20" s="1"/>
-      <c r="DA20" s="1"/>
-      <c r="DB20" s="1"/>
+      <c r="DA20" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB20" t="s">
+        <v>77</v>
+      </c>
       <c r="DC20" s="1"/>
-      <c r="DD20" s="1"/>
+      <c r="DD20" t="s">
+        <v>77</v>
+      </c>
       <c r="DE20" s="1"/>
       <c r="DF20" s="1"/>
       <c r="DG20" s="1"/>
@@ -8007,7 +8176,7 @@
       <c r="FT20" s="1"/>
       <c r="FU20" s="1"/>
       <c r="FV20" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21">
@@ -8174,10 +8343,10 @@
         <v>177</v>
       </c>
       <c r="BC21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BD21" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="BE21" s="1">
         <v>1</v>
@@ -8189,7 +8358,7 @@
         <v>177</v>
       </c>
       <c r="BH21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BI21" s="2">
         <v>45491</v>
@@ -8201,13 +8370,13 @@
         <v>173</v>
       </c>
       <c r="BL21" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="BM21" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="BN21" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="BO21" s="2">
         <v>45474</v>
@@ -8217,13 +8386,13 @@
       <c r="BR21" s="1"/>
       <c r="BS21" s="1"/>
       <c r="BT21" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="BU21" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BV21" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="BW21" s="2">
         <v>45498</v>
@@ -8247,25 +8416,25 @@
         <v>8</v>
       </c>
       <c r="CL21" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CM21" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="CN21" s="1">
         <v>3</v>
       </c>
       <c r="CO21" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="CP21" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="CQ21" s="1">
         <v>1</v>
       </c>
       <c r="CR21" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="CS21" t="s">
         <v>77</v>
@@ -8281,12 +8450,20 @@
       <c r="CX21" t="s">
         <v>77</v>
       </c>
-      <c r="CY21" s="1"/>
+      <c r="CY21" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ21" s="1"/>
-      <c r="DA21" s="1"/>
-      <c r="DB21" s="1"/>
+      <c r="DA21" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB21" t="s">
+        <v>77</v>
+      </c>
       <c r="DC21" s="1"/>
-      <c r="DD21" s="1"/>
+      <c r="DD21" t="s">
+        <v>77</v>
+      </c>
       <c r="DE21" s="1"/>
       <c r="DF21" s="1"/>
       <c r="DG21" s="1"/>
@@ -8524,10 +8701,10 @@
         <v>177</v>
       </c>
       <c r="BC22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BD22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="BE22" s="1">
         <v>1</v>
@@ -8539,7 +8716,7 @@
         <v>177</v>
       </c>
       <c r="BH22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BI22" s="2">
         <v>45491</v>
@@ -8587,13 +8764,13 @@
       <c r="CH22" s="1"/>
       <c r="CI22" s="1"/>
       <c r="CJ22" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CK22" s="1">
         <v>7</v>
       </c>
       <c r="CL22" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CM22" t="s">
         <v>165</v>
@@ -8602,41 +8779,53 @@
         <v>22</v>
       </c>
       <c r="CO22" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CP22" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="CQ22" s="1">
         <v>59</v>
       </c>
       <c r="CR22" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CS22" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="CT22" s="1">
         <v>26</v>
       </c>
       <c r="CU22" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="CV22" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="CW22" s="1">
         <v>28</v>
       </c>
       <c r="CX22" t="s">
+        <v>243</v>
+      </c>
+      <c r="CY22" t="s">
         <v>238</v>
       </c>
-      <c r="CY22" s="1"/>
-      <c r="CZ22" s="1"/>
-      <c r="DA22" s="1"/>
-      <c r="DB22" s="1"/>
-      <c r="DC22" s="1"/>
-      <c r="DD22" s="1"/>
+      <c r="CZ22" s="1">
+        <v>51</v>
+      </c>
+      <c r="DA22" t="s">
+        <v>243</v>
+      </c>
+      <c r="DB22" t="s">
+        <v>187</v>
+      </c>
+      <c r="DC22" s="1">
+        <v>15</v>
+      </c>
+      <c r="DD22" t="s">
+        <v>243</v>
+      </c>
       <c r="DE22" s="1"/>
       <c r="DF22" s="1"/>
       <c r="DG22" s="1"/>
@@ -8874,10 +9063,10 @@
         <v>177</v>
       </c>
       <c r="BC23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BD23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="BE23" s="1">
         <v>1</v>
@@ -8889,7 +9078,7 @@
         <v>176</v>
       </c>
       <c r="BH23" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BI23" s="2">
         <v>45497</v>
@@ -8937,27 +9126,31 @@
       <c r="CH23" s="1"/>
       <c r="CI23" s="1"/>
       <c r="CJ23" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="CK23" s="1">
         <v>8</v>
       </c>
       <c r="CL23" t="s">
+        <v>243</v>
+      </c>
+      <c r="CM23" t="s">
         <v>238</v>
       </c>
-      <c r="CM23" t="s">
-        <v>77</v>
-      </c>
-      <c r="CN23" s="1"/>
+      <c r="CN23" s="1">
+        <v>38</v>
+      </c>
       <c r="CO23" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CP23" t="s">
-        <v>77</v>
-      </c>
-      <c r="CQ23" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="CQ23" s="1">
+        <v>55</v>
+      </c>
       <c r="CR23" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CS23" t="s">
         <v>77</v>
@@ -8973,12 +9166,20 @@
       <c r="CX23" t="s">
         <v>77</v>
       </c>
-      <c r="CY23" s="1"/>
+      <c r="CY23" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ23" s="1"/>
-      <c r="DA23" s="1"/>
-      <c r="DB23" s="1"/>
+      <c r="DA23" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB23" t="s">
+        <v>77</v>
+      </c>
       <c r="DC23" s="1"/>
-      <c r="DD23" s="1"/>
+      <c r="DD23" t="s">
+        <v>77</v>
+      </c>
       <c r="DE23" s="1"/>
       <c r="DF23" s="1"/>
       <c r="DG23" s="1"/>
@@ -9049,7 +9250,7 @@
       <c r="FT23" s="1"/>
       <c r="FU23" s="1"/>
       <c r="FV23" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24">
@@ -9216,10 +9417,10 @@
         <v>177</v>
       </c>
       <c r="BC24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BD24" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="BE24" s="1">
         <v>1</v>
@@ -9231,7 +9432,7 @@
         <v>177</v>
       </c>
       <c r="BH24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BI24" s="2">
         <v>45497</v>
@@ -9279,11 +9480,13 @@
       <c r="CH24" s="1"/>
       <c r="CI24" s="1"/>
       <c r="CJ24" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK24" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="CK24" s="1">
+        <v>104</v>
+      </c>
       <c r="CL24" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CM24" t="s">
         <v>77</v>
@@ -9313,12 +9516,20 @@
       <c r="CX24" t="s">
         <v>77</v>
       </c>
-      <c r="CY24" s="1"/>
+      <c r="CY24" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ24" s="1"/>
-      <c r="DA24" s="1"/>
-      <c r="DB24" s="1"/>
+      <c r="DA24" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB24" t="s">
+        <v>77</v>
+      </c>
       <c r="DC24" s="1"/>
-      <c r="DD24" s="1"/>
+      <c r="DD24" t="s">
+        <v>77</v>
+      </c>
       <c r="DE24" s="1"/>
       <c r="DF24" s="1"/>
       <c r="DG24" s="1"/>
@@ -9559,7 +9770,7 @@
         <v>94</v>
       </c>
       <c r="BD25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="BE25" s="1">
         <v>1</v>
@@ -9649,12 +9860,20 @@
       <c r="CX25" t="s">
         <v>77</v>
       </c>
-      <c r="CY25" s="1"/>
+      <c r="CY25" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ25" s="1"/>
-      <c r="DA25" s="1"/>
-      <c r="DB25" s="1"/>
+      <c r="DA25" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB25" t="s">
+        <v>77</v>
+      </c>
       <c r="DC25" s="1"/>
-      <c r="DD25" s="1"/>
+      <c r="DD25" t="s">
+        <v>77</v>
+      </c>
       <c r="DE25" s="1"/>
       <c r="DF25" s="1"/>
       <c r="DG25" s="1"/>
@@ -9983,12 +10202,20 @@
       <c r="CX26" t="s">
         <v>77</v>
       </c>
-      <c r="CY26" s="1"/>
+      <c r="CY26" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ26" s="1"/>
-      <c r="DA26" s="1"/>
-      <c r="DB26" s="1"/>
+      <c r="DA26" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB26" t="s">
+        <v>77</v>
+      </c>
       <c r="DC26" s="1"/>
-      <c r="DD26" s="1"/>
+      <c r="DD26" t="s">
+        <v>77</v>
+      </c>
       <c r="DE26" s="1"/>
       <c r="DF26" s="1"/>
       <c r="DG26" s="1"/>
@@ -10059,7 +10286,7 @@
       <c r="FT26" s="1"/>
       <c r="FU26" s="1"/>
       <c r="FV26" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27">
@@ -10313,12 +10540,20 @@
       <c r="CX27" t="s">
         <v>77</v>
       </c>
-      <c r="CY27" s="1"/>
+      <c r="CY27" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ27" s="1"/>
-      <c r="DA27" s="1"/>
-      <c r="DB27" s="1"/>
+      <c r="DA27" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB27" t="s">
+        <v>77</v>
+      </c>
       <c r="DC27" s="1"/>
-      <c r="DD27" s="1"/>
+      <c r="DD27" t="s">
+        <v>77</v>
+      </c>
       <c r="DE27" s="1"/>
       <c r="DF27" s="1"/>
       <c r="DG27" s="1"/>
@@ -10643,12 +10878,20 @@
       <c r="CX28" t="s">
         <v>77</v>
       </c>
-      <c r="CY28" s="1"/>
+      <c r="CY28" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ28" s="1"/>
-      <c r="DA28" s="1"/>
-      <c r="DB28" s="1"/>
+      <c r="DA28" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB28" t="s">
+        <v>77</v>
+      </c>
       <c r="DC28" s="1"/>
-      <c r="DD28" s="1"/>
+      <c r="DD28" t="s">
+        <v>77</v>
+      </c>
       <c r="DE28" s="1"/>
       <c r="DF28" s="1"/>
       <c r="DG28" s="1"/>
@@ -10719,7 +10962,7 @@
       <c r="FT28" s="1"/>
       <c r="FU28" s="1"/>
       <c r="FV28" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29">
@@ -10973,12 +11216,20 @@
       <c r="CX29" t="s">
         <v>77</v>
       </c>
-      <c r="CY29" s="1"/>
+      <c r="CY29" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ29" s="1"/>
-      <c r="DA29" s="1"/>
-      <c r="DB29" s="1"/>
+      <c r="DA29" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB29" t="s">
+        <v>77</v>
+      </c>
       <c r="DC29" s="1"/>
-      <c r="DD29" s="1"/>
+      <c r="DD29" t="s">
+        <v>77</v>
+      </c>
       <c r="DE29" s="1"/>
       <c r="DF29" s="1"/>
       <c r="DG29" s="1"/>
@@ -11049,7 +11300,7 @@
       <c r="FT29" s="1"/>
       <c r="FU29" s="1"/>
       <c r="FV29" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30">
@@ -11307,12 +11558,20 @@
       <c r="CX30" t="s">
         <v>77</v>
       </c>
-      <c r="CY30" s="1"/>
+      <c r="CY30" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ30" s="1"/>
-      <c r="DA30" s="1"/>
-      <c r="DB30" s="1"/>
+      <c r="DA30" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB30" t="s">
+        <v>77</v>
+      </c>
       <c r="DC30" s="1"/>
-      <c r="DD30" s="1"/>
+      <c r="DD30" t="s">
+        <v>77</v>
+      </c>
       <c r="DE30" s="1"/>
       <c r="DF30" s="1"/>
       <c r="DG30" s="1"/>
@@ -11383,7 +11642,7 @@
       <c r="FT30" s="1"/>
       <c r="FU30" s="1"/>
       <c r="FV30" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31">
@@ -11641,12 +11900,20 @@
       <c r="CX31" t="s">
         <v>77</v>
       </c>
-      <c r="CY31" s="1"/>
+      <c r="CY31" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ31" s="1"/>
-      <c r="DA31" s="1"/>
-      <c r="DB31" s="1"/>
+      <c r="DA31" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB31" t="s">
+        <v>77</v>
+      </c>
       <c r="DC31" s="1"/>
-      <c r="DD31" s="1"/>
+      <c r="DD31" t="s">
+        <v>77</v>
+      </c>
       <c r="DE31" s="1"/>
       <c r="DF31" s="1"/>
       <c r="DG31" s="1"/>
@@ -11717,7 +11984,7 @@
       <c r="FT31" s="1"/>
       <c r="FU31" s="1"/>
       <c r="FV31" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32">
@@ -11975,12 +12242,20 @@
       <c r="CX32" t="s">
         <v>77</v>
       </c>
-      <c r="CY32" s="1"/>
+      <c r="CY32" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ32" s="1"/>
-      <c r="DA32" s="1"/>
-      <c r="DB32" s="1"/>
+      <c r="DA32" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB32" t="s">
+        <v>77</v>
+      </c>
       <c r="DC32" s="1"/>
-      <c r="DD32" s="1"/>
+      <c r="DD32" t="s">
+        <v>77</v>
+      </c>
       <c r="DE32" s="1"/>
       <c r="DF32" s="1"/>
       <c r="DG32" s="1"/>
@@ -12051,7 +12326,7 @@
       <c r="FT32" s="1"/>
       <c r="FU32" s="1"/>
       <c r="FV32" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33">
@@ -12309,12 +12584,20 @@
       <c r="CX33" t="s">
         <v>77</v>
       </c>
-      <c r="CY33" s="1"/>
+      <c r="CY33" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ33" s="1"/>
-      <c r="DA33" s="1"/>
-      <c r="DB33" s="1"/>
+      <c r="DA33" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB33" t="s">
+        <v>77</v>
+      </c>
       <c r="DC33" s="1"/>
-      <c r="DD33" s="1"/>
+      <c r="DD33" t="s">
+        <v>77</v>
+      </c>
       <c r="DE33" s="1"/>
       <c r="DF33" s="1"/>
       <c r="DG33" s="1"/>
@@ -12385,7 +12668,7 @@
       <c r="FT33" s="1"/>
       <c r="FU33" s="1"/>
       <c r="FV33" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34">
@@ -12629,12 +12912,20 @@
       <c r="CX34" t="s">
         <v>77</v>
       </c>
-      <c r="CY34" s="1"/>
+      <c r="CY34" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ34" s="1"/>
-      <c r="DA34" s="1"/>
-      <c r="DB34" s="1"/>
+      <c r="DA34" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB34" t="s">
+        <v>77</v>
+      </c>
       <c r="DC34" s="1"/>
-      <c r="DD34" s="1"/>
+      <c r="DD34" t="s">
+        <v>77</v>
+      </c>
       <c r="DE34" s="1"/>
       <c r="DF34" s="1"/>
       <c r="DG34" s="1"/>
@@ -12705,7 +12996,7 @@
       <c r="FT34" s="1"/>
       <c r="FU34" s="1"/>
       <c r="FV34" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35">
@@ -12949,12 +13240,20 @@
       <c r="CX35" t="s">
         <v>77</v>
       </c>
-      <c r="CY35" s="1"/>
+      <c r="CY35" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ35" s="1"/>
-      <c r="DA35" s="1"/>
-      <c r="DB35" s="1"/>
+      <c r="DA35" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB35" t="s">
+        <v>77</v>
+      </c>
       <c r="DC35" s="1"/>
-      <c r="DD35" s="1"/>
+      <c r="DD35" t="s">
+        <v>77</v>
+      </c>
       <c r="DE35" s="1"/>
       <c r="DF35" s="1"/>
       <c r="DG35" s="1"/>
@@ -13025,7 +13324,7 @@
       <c r="FT35" s="1"/>
       <c r="FU35" s="1"/>
       <c r="FV35" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36">
@@ -13269,12 +13568,20 @@
       <c r="CX36" t="s">
         <v>77</v>
       </c>
-      <c r="CY36" s="1"/>
+      <c r="CY36" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ36" s="1"/>
-      <c r="DA36" s="1"/>
-      <c r="DB36" s="1"/>
+      <c r="DA36" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB36" t="s">
+        <v>77</v>
+      </c>
       <c r="DC36" s="1"/>
-      <c r="DD36" s="1"/>
+      <c r="DD36" t="s">
+        <v>77</v>
+      </c>
       <c r="DE36" s="1"/>
       <c r="DF36" s="1"/>
       <c r="DG36" s="1"/>
@@ -13345,7 +13652,7 @@
       <c r="FT36" s="1"/>
       <c r="FU36" s="1"/>
       <c r="FV36" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37">
@@ -13589,12 +13896,20 @@
       <c r="CX37" t="s">
         <v>77</v>
       </c>
-      <c r="CY37" s="1"/>
+      <c r="CY37" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ37" s="1"/>
-      <c r="DA37" s="1"/>
-      <c r="DB37" s="1"/>
+      <c r="DA37" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB37" t="s">
+        <v>77</v>
+      </c>
       <c r="DC37" s="1"/>
-      <c r="DD37" s="1"/>
+      <c r="DD37" t="s">
+        <v>77</v>
+      </c>
       <c r="DE37" s="1"/>
       <c r="DF37" s="1"/>
       <c r="DG37" s="1"/>
@@ -13665,7 +13980,7 @@
       <c r="FT37" s="1"/>
       <c r="FU37" s="1"/>
       <c r="FV37" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38">
@@ -13909,12 +14224,20 @@
       <c r="CX38" t="s">
         <v>77</v>
       </c>
-      <c r="CY38" s="1"/>
+      <c r="CY38" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ38" s="1"/>
-      <c r="DA38" s="1"/>
-      <c r="DB38" s="1"/>
+      <c r="DA38" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB38" t="s">
+        <v>77</v>
+      </c>
       <c r="DC38" s="1"/>
-      <c r="DD38" s="1"/>
+      <c r="DD38" t="s">
+        <v>77</v>
+      </c>
       <c r="DE38" s="1"/>
       <c r="DF38" s="1"/>
       <c r="DG38" s="1"/>
@@ -13985,7 +14308,7 @@
       <c r="FT38" s="1"/>
       <c r="FU38" s="1"/>
       <c r="FV38" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39">
@@ -14231,12 +14554,20 @@
       <c r="CX39" t="s">
         <v>77</v>
       </c>
-      <c r="CY39" s="1"/>
+      <c r="CY39" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ39" s="1"/>
-      <c r="DA39" s="1"/>
-      <c r="DB39" s="1"/>
+      <c r="DA39" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB39" t="s">
+        <v>77</v>
+      </c>
       <c r="DC39" s="1"/>
-      <c r="DD39" s="1"/>
+      <c r="DD39" t="s">
+        <v>77</v>
+      </c>
       <c r="DE39" s="1"/>
       <c r="DF39" s="1"/>
       <c r="DG39" s="1"/>
@@ -14553,12 +14884,20 @@
       <c r="CX40" t="s">
         <v>77</v>
       </c>
-      <c r="CY40" s="1"/>
+      <c r="CY40" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ40" s="1"/>
-      <c r="DA40" s="1"/>
-      <c r="DB40" s="1"/>
+      <c r="DA40" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB40" t="s">
+        <v>77</v>
+      </c>
       <c r="DC40" s="1"/>
-      <c r="DD40" s="1"/>
+      <c r="DD40" t="s">
+        <v>77</v>
+      </c>
       <c r="DE40" s="1"/>
       <c r="DF40" s="1"/>
       <c r="DG40" s="1"/>
@@ -14875,12 +15214,20 @@
       <c r="CX41" t="s">
         <v>77</v>
       </c>
-      <c r="CY41" s="1"/>
+      <c r="CY41" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ41" s="1"/>
-      <c r="DA41" s="1"/>
-      <c r="DB41" s="1"/>
+      <c r="DA41" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB41" t="s">
+        <v>77</v>
+      </c>
       <c r="DC41" s="1"/>
-      <c r="DD41" s="1"/>
+      <c r="DD41" t="s">
+        <v>77</v>
+      </c>
       <c r="DE41" s="1"/>
       <c r="DF41" s="1"/>
       <c r="DG41" s="1"/>
@@ -15197,12 +15544,20 @@
       <c r="CX42" t="s">
         <v>77</v>
       </c>
-      <c r="CY42" s="1"/>
+      <c r="CY42" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ42" s="1"/>
-      <c r="DA42" s="1"/>
-      <c r="DB42" s="1"/>
+      <c r="DA42" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB42" t="s">
+        <v>77</v>
+      </c>
       <c r="DC42" s="1"/>
-      <c r="DD42" s="1"/>
+      <c r="DD42" t="s">
+        <v>77</v>
+      </c>
       <c r="DE42" s="1"/>
       <c r="DF42" s="1"/>
       <c r="DG42" s="1"/>
@@ -15519,12 +15874,20 @@
       <c r="CX43" t="s">
         <v>77</v>
       </c>
-      <c r="CY43" s="1"/>
+      <c r="CY43" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ43" s="1"/>
-      <c r="DA43" s="1"/>
-      <c r="DB43" s="1"/>
+      <c r="DA43" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB43" t="s">
+        <v>77</v>
+      </c>
       <c r="DC43" s="1"/>
-      <c r="DD43" s="1"/>
+      <c r="DD43" t="s">
+        <v>77</v>
+      </c>
       <c r="DE43" s="1"/>
       <c r="DF43" s="1"/>
       <c r="DG43" s="1"/>
@@ -15805,20 +16168,20 @@
       <c r="CH44" s="1"/>
       <c r="CI44" s="1"/>
       <c r="CJ44" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="CK44" s="1">
         <v>12</v>
       </c>
       <c r="CL44" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM44" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CN44" s="1"/>
       <c r="CO44" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP44" t="s">
         <v>166</v>
@@ -15827,7 +16190,7 @@
         <v>9</v>
       </c>
       <c r="CR44" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CS44" t="s">
         <v>77</v>
@@ -15843,12 +16206,20 @@
       <c r="CX44" t="s">
         <v>77</v>
       </c>
-      <c r="CY44" s="1"/>
+      <c r="CY44" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ44" s="1"/>
-      <c r="DA44" s="1"/>
-      <c r="DB44" s="1"/>
+      <c r="DA44" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB44" t="s">
+        <v>77</v>
+      </c>
       <c r="DC44" s="1"/>
-      <c r="DD44" s="1"/>
+      <c r="DD44" t="s">
+        <v>77</v>
+      </c>
       <c r="DE44" s="1"/>
       <c r="DF44" s="1"/>
       <c r="DG44" s="1"/>
@@ -15919,7 +16290,7 @@
       <c r="FT44" s="1"/>
       <c r="FU44" s="1"/>
       <c r="FV44" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="45">
@@ -16129,20 +16500,20 @@
       <c r="CH45" s="1"/>
       <c r="CI45" s="1"/>
       <c r="CJ45" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="CK45" s="1">
         <v>26</v>
       </c>
       <c r="CL45" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM45" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CN45" s="1"/>
       <c r="CO45" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP45" t="s">
         <v>166</v>
@@ -16151,7 +16522,7 @@
         <v>26</v>
       </c>
       <c r="CR45" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CS45" t="s">
         <v>77</v>
@@ -16167,12 +16538,20 @@
       <c r="CX45" t="s">
         <v>77</v>
       </c>
-      <c r="CY45" s="1"/>
+      <c r="CY45" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ45" s="1"/>
-      <c r="DA45" s="1"/>
-      <c r="DB45" s="1"/>
+      <c r="DA45" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB45" t="s">
+        <v>77</v>
+      </c>
       <c r="DC45" s="1"/>
-      <c r="DD45" s="1"/>
+      <c r="DD45" t="s">
+        <v>77</v>
+      </c>
       <c r="DE45" s="1"/>
       <c r="DF45" s="1"/>
       <c r="DG45" s="1"/>
@@ -16243,7 +16622,7 @@
       <c r="FT45" s="1"/>
       <c r="FU45" s="1"/>
       <c r="FV45" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="46">
@@ -16453,31 +16832,31 @@
       <c r="CH46" s="1"/>
       <c r="CI46" s="1"/>
       <c r="CJ46" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="CK46" s="1">
         <v>6</v>
       </c>
       <c r="CL46" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM46" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="CN46" s="1">
         <v>17</v>
       </c>
       <c r="CO46" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP46" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="CQ46" s="1">
         <v>12</v>
       </c>
       <c r="CR46" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CS46" t="s">
         <v>77</v>
@@ -16493,12 +16872,20 @@
       <c r="CX46" t="s">
         <v>77</v>
       </c>
-      <c r="CY46" s="1"/>
+      <c r="CY46" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ46" s="1"/>
-      <c r="DA46" s="1"/>
-      <c r="DB46" s="1"/>
+      <c r="DA46" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB46" t="s">
+        <v>77</v>
+      </c>
       <c r="DC46" s="1"/>
-      <c r="DD46" s="1"/>
+      <c r="DD46" t="s">
+        <v>77</v>
+      </c>
       <c r="DE46" s="1"/>
       <c r="DF46" s="1"/>
       <c r="DG46" s="1"/>
@@ -16569,7 +16956,7 @@
       <c r="FT46" s="1"/>
       <c r="FU46" s="1"/>
       <c r="FV46" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="47">
@@ -16813,12 +17200,20 @@
       <c r="CX47" t="s">
         <v>77</v>
       </c>
-      <c r="CY47" s="1"/>
+      <c r="CY47" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ47" s="1"/>
-      <c r="DA47" s="1"/>
-      <c r="DB47" s="1"/>
+      <c r="DA47" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB47" t="s">
+        <v>77</v>
+      </c>
       <c r="DC47" s="1"/>
-      <c r="DD47" s="1"/>
+      <c r="DD47" t="s">
+        <v>77</v>
+      </c>
       <c r="DE47" s="1"/>
       <c r="DF47" s="1"/>
       <c r="DG47" s="1"/>
@@ -16889,7 +17284,7 @@
       <c r="FT47" s="1"/>
       <c r="FU47" s="1"/>
       <c r="FV47" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48">
@@ -17135,12 +17530,20 @@
       <c r="CX48" t="s">
         <v>77</v>
       </c>
-      <c r="CY48" s="1"/>
+      <c r="CY48" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ48" s="1"/>
-      <c r="DA48" s="1"/>
-      <c r="DB48" s="1"/>
+      <c r="DA48" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB48" t="s">
+        <v>77</v>
+      </c>
       <c r="DC48" s="1"/>
-      <c r="DD48" s="1"/>
+      <c r="DD48" t="s">
+        <v>77</v>
+      </c>
       <c r="DE48" s="1"/>
       <c r="DF48" s="1"/>
       <c r="DG48" s="1"/>
@@ -17211,7 +17614,7 @@
       <c r="FT48" s="1"/>
       <c r="FU48" s="1"/>
       <c r="FV48" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="49">
@@ -17455,12 +17858,20 @@
       <c r="CX49" t="s">
         <v>77</v>
       </c>
-      <c r="CY49" s="1"/>
+      <c r="CY49" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ49" s="1"/>
-      <c r="DA49" s="1"/>
-      <c r="DB49" s="1"/>
+      <c r="DA49" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB49" t="s">
+        <v>77</v>
+      </c>
       <c r="DC49" s="1"/>
-      <c r="DD49" s="1"/>
+      <c r="DD49" t="s">
+        <v>77</v>
+      </c>
       <c r="DE49" s="1"/>
       <c r="DF49" s="1"/>
       <c r="DG49" s="1"/>
@@ -17531,7 +17942,7 @@
       <c r="FT49" s="1"/>
       <c r="FU49" s="1"/>
       <c r="FV49" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="50">
@@ -17775,12 +18186,20 @@
       <c r="CX50" t="s">
         <v>77</v>
       </c>
-      <c r="CY50" s="1"/>
+      <c r="CY50" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ50" s="1"/>
-      <c r="DA50" s="1"/>
-      <c r="DB50" s="1"/>
+      <c r="DA50" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB50" t="s">
+        <v>77</v>
+      </c>
       <c r="DC50" s="1"/>
-      <c r="DD50" s="1"/>
+      <c r="DD50" t="s">
+        <v>77</v>
+      </c>
       <c r="DE50" s="1"/>
       <c r="DF50" s="1"/>
       <c r="DG50" s="1"/>
@@ -17851,7 +18270,7 @@
       <c r="FT50" s="1"/>
       <c r="FU50" s="1"/>
       <c r="FV50" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="51">
@@ -18095,12 +18514,20 @@
       <c r="CX51" t="s">
         <v>77</v>
       </c>
-      <c r="CY51" s="1"/>
+      <c r="CY51" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ51" s="1"/>
-      <c r="DA51" s="1"/>
-      <c r="DB51" s="1"/>
+      <c r="DA51" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB51" t="s">
+        <v>77</v>
+      </c>
       <c r="DC51" s="1"/>
-      <c r="DD51" s="1"/>
+      <c r="DD51" t="s">
+        <v>77</v>
+      </c>
       <c r="DE51" s="1"/>
       <c r="DF51" s="1"/>
       <c r="DG51" s="1"/>
@@ -18171,7 +18598,7 @@
       <c r="FT51" s="1"/>
       <c r="FU51" s="1"/>
       <c r="FV51" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52">
@@ -18415,12 +18842,20 @@
       <c r="CX52" t="s">
         <v>77</v>
       </c>
-      <c r="CY52" s="1"/>
+      <c r="CY52" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ52" s="1"/>
-      <c r="DA52" s="1"/>
-      <c r="DB52" s="1"/>
+      <c r="DA52" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB52" t="s">
+        <v>77</v>
+      </c>
       <c r="DC52" s="1"/>
-      <c r="DD52" s="1"/>
+      <c r="DD52" t="s">
+        <v>77</v>
+      </c>
       <c r="DE52" s="1"/>
       <c r="DF52" s="1"/>
       <c r="DG52" s="1"/>
@@ -18491,7 +18926,7 @@
       <c r="FT52" s="1"/>
       <c r="FU52" s="1"/>
       <c r="FV52" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="53">
@@ -18735,12 +19170,20 @@
       <c r="CX53" t="s">
         <v>77</v>
       </c>
-      <c r="CY53" s="1"/>
+      <c r="CY53" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ53" s="1"/>
-      <c r="DA53" s="1"/>
-      <c r="DB53" s="1"/>
+      <c r="DA53" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB53" t="s">
+        <v>77</v>
+      </c>
       <c r="DC53" s="1"/>
-      <c r="DD53" s="1"/>
+      <c r="DD53" t="s">
+        <v>77</v>
+      </c>
       <c r="DE53" s="1"/>
       <c r="DF53" s="1"/>
       <c r="DG53" s="1"/>
@@ -18811,7 +19254,7 @@
       <c r="FT53" s="1"/>
       <c r="FU53" s="1"/>
       <c r="FV53" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="54">
@@ -19055,12 +19498,20 @@
       <c r="CX54" t="s">
         <v>77</v>
       </c>
-      <c r="CY54" s="1"/>
+      <c r="CY54" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ54" s="1"/>
-      <c r="DA54" s="1"/>
-      <c r="DB54" s="1"/>
+      <c r="DA54" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB54" t="s">
+        <v>77</v>
+      </c>
       <c r="DC54" s="1"/>
-      <c r="DD54" s="1"/>
+      <c r="DD54" t="s">
+        <v>77</v>
+      </c>
       <c r="DE54" s="1"/>
       <c r="DF54" s="1"/>
       <c r="DG54" s="1"/>
@@ -19131,7 +19582,7 @@
       <c r="FT54" s="1"/>
       <c r="FU54" s="1"/>
       <c r="FV54" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55">
@@ -19377,12 +19828,20 @@
       <c r="CX55" t="s">
         <v>77</v>
       </c>
-      <c r="CY55" s="1"/>
+      <c r="CY55" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ55" s="1"/>
-      <c r="DA55" s="1"/>
-      <c r="DB55" s="1"/>
+      <c r="DA55" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB55" t="s">
+        <v>77</v>
+      </c>
       <c r="DC55" s="1"/>
-      <c r="DD55" s="1"/>
+      <c r="DD55" t="s">
+        <v>77</v>
+      </c>
       <c r="DE55" s="1"/>
       <c r="DF55" s="1"/>
       <c r="DG55" s="1"/>
@@ -19453,7 +19912,7 @@
       <c r="FT55" s="1"/>
       <c r="FU55" s="1"/>
       <c r="FV55" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="56">
@@ -19663,18 +20122,22 @@
       <c r="CH56" s="1"/>
       <c r="CI56" s="1"/>
       <c r="CJ56" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK56" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="CK56" s="1">
+        <v>24</v>
+      </c>
       <c r="CL56" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CM56" t="s">
-        <v>77</v>
-      </c>
-      <c r="CN56" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="CN56" s="1">
+        <v>43</v>
+      </c>
       <c r="CO56" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CP56" t="s">
         <v>77</v>
@@ -19697,12 +20160,20 @@
       <c r="CX56" t="s">
         <v>77</v>
       </c>
-      <c r="CY56" s="1"/>
+      <c r="CY56" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ56" s="1"/>
-      <c r="DA56" s="1"/>
-      <c r="DB56" s="1"/>
+      <c r="DA56" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB56" t="s">
+        <v>77</v>
+      </c>
       <c r="DC56" s="1"/>
-      <c r="DD56" s="1"/>
+      <c r="DD56" t="s">
+        <v>77</v>
+      </c>
       <c r="DE56" s="1"/>
       <c r="DF56" s="1"/>
       <c r="DG56" s="1"/>
@@ -19773,7 +20244,7 @@
       <c r="FT56" s="1"/>
       <c r="FU56" s="1"/>
       <c r="FV56" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57">
@@ -19983,18 +20454,22 @@
       <c r="CH57" s="1"/>
       <c r="CI57" s="1"/>
       <c r="CJ57" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK57" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="CK57" s="1">
+        <v>6</v>
+      </c>
       <c r="CL57" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CM57" t="s">
-        <v>77</v>
-      </c>
-      <c r="CN57" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="CN57" s="1">
+        <v>10</v>
+      </c>
       <c r="CO57" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="CP57" t="s">
         <v>77</v>
@@ -20017,12 +20492,20 @@
       <c r="CX57" t="s">
         <v>77</v>
       </c>
-      <c r="CY57" s="1"/>
+      <c r="CY57" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ57" s="1"/>
-      <c r="DA57" s="1"/>
-      <c r="DB57" s="1"/>
+      <c r="DA57" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB57" t="s">
+        <v>77</v>
+      </c>
       <c r="DC57" s="1"/>
-      <c r="DD57" s="1"/>
+      <c r="DD57" t="s">
+        <v>77</v>
+      </c>
       <c r="DE57" s="1"/>
       <c r="DF57" s="1"/>
       <c r="DG57" s="1"/>
@@ -20093,7 +20576,7 @@
       <c r="FT57" s="1"/>
       <c r="FU57" s="1"/>
       <c r="FV57" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="58">
@@ -20243,17 +20726,19 @@
         <v>174</v>
       </c>
       <c r="BB58" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="BC58" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="BD58" t="s">
-        <v>77</v>
-      </c>
-      <c r="BE58" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="BE58" s="1">
+        <v>1</v>
+      </c>
       <c r="BF58" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="BG58" t="s">
         <v>77</v>
@@ -20267,13 +20752,13 @@
         <v>77</v>
       </c>
       <c r="BL58" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="BM58" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="BN58" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="BO58" s="2">
         <v>45497</v>
@@ -20339,12 +20824,20 @@
       <c r="CX58" t="s">
         <v>77</v>
       </c>
-      <c r="CY58" s="1"/>
+      <c r="CY58" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ58" s="1"/>
-      <c r="DA58" s="1"/>
-      <c r="DB58" s="1"/>
+      <c r="DA58" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB58" t="s">
+        <v>77</v>
+      </c>
       <c r="DC58" s="1"/>
-      <c r="DD58" s="1"/>
+      <c r="DD58" t="s">
+        <v>77</v>
+      </c>
       <c r="DE58" s="1"/>
       <c r="DF58" s="1"/>
       <c r="DG58" s="1"/>
@@ -20565,17 +21058,19 @@
         <v>174</v>
       </c>
       <c r="BB59" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="BC59" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="BD59" t="s">
-        <v>77</v>
-      </c>
-      <c r="BE59" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="BE59" s="1">
+        <v>1</v>
+      </c>
       <c r="BF59" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="BG59" t="s">
         <v>77</v>
@@ -20589,13 +21084,13 @@
         <v>77</v>
       </c>
       <c r="BL59" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="BM59" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="BN59" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="BO59" s="2">
         <v>45497</v>
@@ -20661,12 +21156,20 @@
       <c r="CX59" t="s">
         <v>77</v>
       </c>
-      <c r="CY59" s="1"/>
+      <c r="CY59" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ59" s="1"/>
-      <c r="DA59" s="1"/>
-      <c r="DB59" s="1"/>
+      <c r="DA59" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB59" t="s">
+        <v>77</v>
+      </c>
       <c r="DC59" s="1"/>
-      <c r="DD59" s="1"/>
+      <c r="DD59" t="s">
+        <v>77</v>
+      </c>
       <c r="DE59" s="1"/>
       <c r="DF59" s="1"/>
       <c r="DG59" s="1"/>
@@ -20947,29 +21450,31 @@
       <c r="CH60" s="1"/>
       <c r="CI60" s="1"/>
       <c r="CJ60" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="CK60" s="1">
         <v>2</v>
       </c>
       <c r="CL60" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM60" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CN60" s="1">
         <v>24</v>
       </c>
       <c r="CO60" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP60" t="s">
-        <v>77</v>
-      </c>
-      <c r="CQ60" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="CQ60" s="1">
+        <v>6</v>
+      </c>
       <c r="CR60" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="CS60" t="s">
         <v>77</v>
@@ -20985,12 +21490,20 @@
       <c r="CX60" t="s">
         <v>77</v>
       </c>
-      <c r="CY60" s="1"/>
+      <c r="CY60" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ60" s="1"/>
-      <c r="DA60" s="1"/>
-      <c r="DB60" s="1"/>
+      <c r="DA60" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB60" t="s">
+        <v>77</v>
+      </c>
       <c r="DC60" s="1"/>
-      <c r="DD60" s="1"/>
+      <c r="DD60" t="s">
+        <v>77</v>
+      </c>
       <c r="DE60" s="1"/>
       <c r="DF60" s="1"/>
       <c r="DG60" s="1"/>
@@ -21061,7 +21574,7 @@
       <c r="FT60" s="1"/>
       <c r="FU60" s="1"/>
       <c r="FV60" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61">
@@ -21271,29 +21784,31 @@
       <c r="CH61" s="1"/>
       <c r="CI61" s="1"/>
       <c r="CJ61" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="CK61" s="1">
         <v>4</v>
       </c>
       <c r="CL61" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CM61" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="CN61" s="1">
         <v>11</v>
       </c>
       <c r="CO61" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="CP61" t="s">
-        <v>77</v>
-      </c>
-      <c r="CQ61" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="CQ61" s="1">
+        <v>15</v>
+      </c>
       <c r="CR61" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="CS61" t="s">
         <v>77</v>
@@ -21309,12 +21824,20 @@
       <c r="CX61" t="s">
         <v>77</v>
       </c>
-      <c r="CY61" s="1"/>
+      <c r="CY61" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ61" s="1"/>
-      <c r="DA61" s="1"/>
-      <c r="DB61" s="1"/>
+      <c r="DA61" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB61" t="s">
+        <v>77</v>
+      </c>
       <c r="DC61" s="1"/>
-      <c r="DD61" s="1"/>
+      <c r="DD61" t="s">
+        <v>77</v>
+      </c>
       <c r="DE61" s="1"/>
       <c r="DF61" s="1"/>
       <c r="DG61" s="1"/>
@@ -21385,7 +21908,7 @@
       <c r="FT61" s="1"/>
       <c r="FU61" s="1"/>
       <c r="FV61" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62">
@@ -21629,12 +22152,20 @@
       <c r="CX62" t="s">
         <v>77</v>
       </c>
-      <c r="CY62" s="1"/>
+      <c r="CY62" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ62" s="1"/>
-      <c r="DA62" s="1"/>
-      <c r="DB62" s="1"/>
+      <c r="DA62" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB62" t="s">
+        <v>77</v>
+      </c>
       <c r="DC62" s="1"/>
-      <c r="DD62" s="1"/>
+      <c r="DD62" t="s">
+        <v>77</v>
+      </c>
       <c r="DE62" s="1"/>
       <c r="DF62" s="1"/>
       <c r="DG62" s="1"/>
@@ -21949,12 +22480,20 @@
       <c r="CX63" t="s">
         <v>77</v>
       </c>
-      <c r="CY63" s="1"/>
+      <c r="CY63" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ63" s="1"/>
-      <c r="DA63" s="1"/>
-      <c r="DB63" s="1"/>
+      <c r="DA63" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB63" t="s">
+        <v>77</v>
+      </c>
       <c r="DC63" s="1"/>
-      <c r="DD63" s="1"/>
+      <c r="DD63" t="s">
+        <v>77</v>
+      </c>
       <c r="DE63" s="1"/>
       <c r="DF63" s="1"/>
       <c r="DG63" s="1"/>
@@ -22269,12 +22808,20 @@
       <c r="CX64" t="s">
         <v>77</v>
       </c>
-      <c r="CY64" s="1"/>
+      <c r="CY64" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ64" s="1"/>
-      <c r="DA64" s="1"/>
-      <c r="DB64" s="1"/>
+      <c r="DA64" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB64" t="s">
+        <v>77</v>
+      </c>
       <c r="DC64" s="1"/>
-      <c r="DD64" s="1"/>
+      <c r="DD64" t="s">
+        <v>77</v>
+      </c>
       <c r="DE64" s="1"/>
       <c r="DF64" s="1"/>
       <c r="DG64" s="1"/>
@@ -22555,25 +23102,31 @@
       <c r="CH65" s="1"/>
       <c r="CI65" s="1"/>
       <c r="CJ65" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK65" s="1"/>
+        <v>236</v>
+      </c>
+      <c r="CK65" s="1">
+        <v>4</v>
+      </c>
       <c r="CL65" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="CM65" t="s">
-        <v>77</v>
-      </c>
-      <c r="CN65" s="1"/>
+        <v>248</v>
+      </c>
+      <c r="CN65" s="1">
+        <v>4</v>
+      </c>
       <c r="CO65" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="CP65" t="s">
-        <v>77</v>
-      </c>
-      <c r="CQ65" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="CQ65" s="1">
+        <v>43</v>
+      </c>
       <c r="CR65" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="CS65" t="s">
         <v>77</v>
@@ -22589,12 +23142,20 @@
       <c r="CX65" t="s">
         <v>77</v>
       </c>
-      <c r="CY65" s="1"/>
+      <c r="CY65" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ65" s="1"/>
-      <c r="DA65" s="1"/>
-      <c r="DB65" s="1"/>
+      <c r="DA65" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB65" t="s">
+        <v>77</v>
+      </c>
       <c r="DC65" s="1"/>
-      <c r="DD65" s="1"/>
+      <c r="DD65" t="s">
+        <v>77</v>
+      </c>
       <c r="DE65" s="1"/>
       <c r="DF65" s="1"/>
       <c r="DG65" s="1"/>
@@ -22665,7 +23226,7 @@
       <c r="FT65" s="1"/>
       <c r="FU65" s="1"/>
       <c r="FV65" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="66">
@@ -22909,12 +23470,20 @@
       <c r="CX66" t="s">
         <v>77</v>
       </c>
-      <c r="CY66" s="1"/>
+      <c r="CY66" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ66" s="1"/>
-      <c r="DA66" s="1"/>
-      <c r="DB66" s="1"/>
+      <c r="DA66" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB66" t="s">
+        <v>77</v>
+      </c>
       <c r="DC66" s="1"/>
-      <c r="DD66" s="1"/>
+      <c r="DD66" t="s">
+        <v>77</v>
+      </c>
       <c r="DE66" s="1"/>
       <c r="DF66" s="1"/>
       <c r="DG66" s="1"/>
@@ -22985,7 +23554,7 @@
       <c r="FT66" s="1"/>
       <c r="FU66" s="1"/>
       <c r="FV66" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="67">
@@ -23229,12 +23798,20 @@
       <c r="CX67" t="s">
         <v>77</v>
       </c>
-      <c r="CY67" s="1"/>
+      <c r="CY67" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ67" s="1"/>
-      <c r="DA67" s="1"/>
-      <c r="DB67" s="1"/>
+      <c r="DA67" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB67" t="s">
+        <v>77</v>
+      </c>
       <c r="DC67" s="1"/>
-      <c r="DD67" s="1"/>
+      <c r="DD67" t="s">
+        <v>77</v>
+      </c>
       <c r="DE67" s="1"/>
       <c r="DF67" s="1"/>
       <c r="DG67" s="1"/>
@@ -23305,7 +23882,7 @@
       <c r="FT67" s="1"/>
       <c r="FU67" s="1"/>
       <c r="FV67" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68">
@@ -23549,12 +24126,20 @@
       <c r="CX68" t="s">
         <v>77</v>
       </c>
-      <c r="CY68" s="1"/>
+      <c r="CY68" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ68" s="1"/>
-      <c r="DA68" s="1"/>
-      <c r="DB68" s="1"/>
+      <c r="DA68" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB68" t="s">
+        <v>77</v>
+      </c>
       <c r="DC68" s="1"/>
-      <c r="DD68" s="1"/>
+      <c r="DD68" t="s">
+        <v>77</v>
+      </c>
       <c r="DE68" s="1"/>
       <c r="DF68" s="1"/>
       <c r="DG68" s="1"/>
@@ -23625,7 +24210,7 @@
       <c r="FT68" s="1"/>
       <c r="FU68" s="1"/>
       <c r="FV68" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69">
@@ -23869,12 +24454,20 @@
       <c r="CX69" t="s">
         <v>77</v>
       </c>
-      <c r="CY69" s="1"/>
+      <c r="CY69" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ69" s="1"/>
-      <c r="DA69" s="1"/>
-      <c r="DB69" s="1"/>
+      <c r="DA69" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB69" t="s">
+        <v>77</v>
+      </c>
       <c r="DC69" s="1"/>
-      <c r="DD69" s="1"/>
+      <c r="DD69" t="s">
+        <v>77</v>
+      </c>
       <c r="DE69" s="1"/>
       <c r="DF69" s="1"/>
       <c r="DG69" s="1"/>
@@ -23945,7 +24538,7 @@
       <c r="FT69" s="1"/>
       <c r="FU69" s="1"/>
       <c r="FV69" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70">
@@ -24189,12 +24782,20 @@
       <c r="CX70" t="s">
         <v>77</v>
       </c>
-      <c r="CY70" s="1"/>
+      <c r="CY70" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ70" s="1"/>
-      <c r="DA70" s="1"/>
-      <c r="DB70" s="1"/>
+      <c r="DA70" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB70" t="s">
+        <v>77</v>
+      </c>
       <c r="DC70" s="1"/>
-      <c r="DD70" s="1"/>
+      <c r="DD70" t="s">
+        <v>77</v>
+      </c>
       <c r="DE70" s="1"/>
       <c r="DF70" s="1"/>
       <c r="DG70" s="1"/>
@@ -24265,7 +24866,7 @@
       <c r="FT70" s="1"/>
       <c r="FU70" s="1"/>
       <c r="FV70" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71">
@@ -24509,12 +25110,20 @@
       <c r="CX71" t="s">
         <v>77</v>
       </c>
-      <c r="CY71" s="1"/>
+      <c r="CY71" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ71" s="1"/>
-      <c r="DA71" s="1"/>
-      <c r="DB71" s="1"/>
+      <c r="DA71" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB71" t="s">
+        <v>77</v>
+      </c>
       <c r="DC71" s="1"/>
-      <c r="DD71" s="1"/>
+      <c r="DD71" t="s">
+        <v>77</v>
+      </c>
       <c r="DE71" s="1"/>
       <c r="DF71" s="1"/>
       <c r="DG71" s="1"/>
@@ -24585,7 +25194,7 @@
       <c r="FT71" s="1"/>
       <c r="FU71" s="1"/>
       <c r="FV71" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="72">
@@ -24831,12 +25440,20 @@
       <c r="CX72" t="s">
         <v>77</v>
       </c>
-      <c r="CY72" s="1"/>
+      <c r="CY72" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ72" s="1"/>
-      <c r="DA72" s="1"/>
-      <c r="DB72" s="1"/>
+      <c r="DA72" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB72" t="s">
+        <v>77</v>
+      </c>
       <c r="DC72" s="1"/>
-      <c r="DD72" s="1"/>
+      <c r="DD72" t="s">
+        <v>77</v>
+      </c>
       <c r="DE72" s="1"/>
       <c r="DF72" s="1"/>
       <c r="DG72" s="1"/>
@@ -25153,12 +25770,20 @@
       <c r="CX73" t="s">
         <v>77</v>
       </c>
-      <c r="CY73" s="1"/>
+      <c r="CY73" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ73" s="1"/>
-      <c r="DA73" s="1"/>
-      <c r="DB73" s="1"/>
+      <c r="DA73" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB73" t="s">
+        <v>77</v>
+      </c>
       <c r="DC73" s="1"/>
-      <c r="DD73" s="1"/>
+      <c r="DD73" t="s">
+        <v>77</v>
+      </c>
       <c r="DE73" s="1"/>
       <c r="DF73" s="1"/>
       <c r="DG73" s="1"/>
@@ -25475,12 +26100,20 @@
       <c r="CX74" t="s">
         <v>77</v>
       </c>
-      <c r="CY74" s="1"/>
+      <c r="CY74" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ74" s="1"/>
-      <c r="DA74" s="1"/>
-      <c r="DB74" s="1"/>
+      <c r="DA74" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB74" t="s">
+        <v>77</v>
+      </c>
       <c r="DC74" s="1"/>
-      <c r="DD74" s="1"/>
+      <c r="DD74" t="s">
+        <v>77</v>
+      </c>
       <c r="DE74" s="1"/>
       <c r="DF74" s="1"/>
       <c r="DG74" s="1"/>
@@ -25797,12 +26430,20 @@
       <c r="CX75" t="s">
         <v>77</v>
       </c>
-      <c r="CY75" s="1"/>
+      <c r="CY75" t="s">
+        <v>77</v>
+      </c>
       <c r="CZ75" s="1"/>
-      <c r="DA75" s="1"/>
-      <c r="DB75" s="1"/>
+      <c r="DA75" t="s">
+        <v>77</v>
+      </c>
+      <c r="DB75" t="s">
+        <v>77</v>
+      </c>
       <c r="DC75" s="1"/>
-      <c r="DD75" s="1"/>
+      <c r="DD75" t="s">
+        <v>77</v>
+      </c>
       <c r="DE75" s="1"/>
       <c r="DF75" s="1"/>
       <c r="DG75" s="1"/>

</xml_diff>

<commit_message>
updates to 2024 crop data cleaning
</commit_message>
<xml_diff>
--- a/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
+++ b/analytics/raw_data/tbf_market_garden_data_2024_raw.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="7983" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="7983" uniqueCount="376">
   <si>
     <t>crop</t>
   </si>
@@ -666,12 +666,6 @@
     <t>path_ipm_date_1_1</t>
   </si>
   <si>
-    <t>24jul2024</t>
-  </si>
-  <si>
-    <t>18aug2024</t>
-  </si>
-  <si>
     <t>path_ipm_type_1_2</t>
   </si>
   <si>
@@ -702,7 +696,7 @@
     <t>2024-07-25</t>
   </si>
   <si>
-    <t>24aug2024</t>
+    <t>2024-08-24</t>
   </si>
   <si>
     <t>path_ipm_type_2_1</t>
@@ -781,9 +775,6 @@
   </si>
   <si>
     <t>2024-06-29</t>
-  </si>
-  <si>
-    <t>2024-08-24</t>
   </si>
   <si>
     <t>2024-08-02</t>
@@ -1421,337 +1412,337 @@
         <v>216</v>
       </c>
       <c r="BU1" t="s">
+        <v>217</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BW1" t="s">
         <v>219</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BX1" t="s">
         <v>220</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BY1" t="s">
         <v>221</v>
       </c>
-      <c r="BX1" t="s">
-        <v>222</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>223</v>
-      </c>
       <c r="BZ1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="CA1" t="s">
+        <v>228</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>229</v>
+      </c>
+      <c r="CC1" t="s">
         <v>230</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CD1" t="s">
         <v>231</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CE1" t="s">
         <v>232</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CF1" t="s">
         <v>233</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CG1" t="s">
         <v>234</v>
       </c>
-      <c r="CF1" t="s">
-        <v>235</v>
-      </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>236</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>238</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>240</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
+        <v>241</v>
+      </c>
+      <c r="CL1" t="s">
         <v>242</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CM1" t="s">
         <v>243</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CN1" t="s">
         <v>244</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CO1" t="s">
         <v>245</v>
       </c>
-      <c r="CN1" t="s">
-        <v>246</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>247</v>
-      </c>
       <c r="CP1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="CQ1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="CR1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="CS1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="CT1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="CU1" t="s">
+        <v>268</v>
+      </c>
+      <c r="CV1" t="s">
         <v>271</v>
       </c>
-      <c r="CV1" t="s">
-        <v>274</v>
-      </c>
       <c r="CW1" t="s">
+        <v>272</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>273</v>
+      </c>
+      <c r="CY1" t="s">
         <v>275</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CZ1" t="s">
         <v>276</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DA1" t="s">
+        <v>277</v>
+      </c>
+      <c r="DB1" t="s">
         <v>278</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DC1" t="s">
         <v>279</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DD1" t="s">
         <v>280</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DE1" t="s">
         <v>281</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DF1" t="s">
         <v>282</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DG1" t="s">
         <v>283</v>
       </c>
-      <c r="DE1" t="s">
-        <v>284</v>
-      </c>
-      <c r="DF1" t="s">
+      <c r="DH1" t="s">
         <v>285</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DI1" t="s">
         <v>286</v>
       </c>
-      <c r="DH1" t="s">
-        <v>288</v>
-      </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
+        <v>287</v>
+      </c>
+      <c r="DK1" t="s">
         <v>289</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DL1" t="s">
         <v>290</v>
       </c>
-      <c r="DK1" t="s">
-        <v>292</v>
-      </c>
-      <c r="DL1" t="s">
+      <c r="DM1" t="s">
+        <v>291</v>
+      </c>
+      <c r="DN1" t="s">
         <v>293</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DO1" t="s">
         <v>294</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DP1" t="s">
+        <v>295</v>
+      </c>
+      <c r="DQ1" t="s">
         <v>296</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DR1" t="s">
         <v>297</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DS1" t="s">
         <v>298</v>
       </c>
-      <c r="DQ1" t="s">
-        <v>299</v>
-      </c>
-      <c r="DR1" t="s">
+      <c r="DT1" t="s">
         <v>300</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DU1" t="s">
         <v>301</v>
       </c>
-      <c r="DT1" t="s">
-        <v>303</v>
-      </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
+        <v>302</v>
+      </c>
+      <c r="DW1" t="s">
         <v>304</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DX1" t="s">
         <v>305</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DY1" t="s">
+        <v>306</v>
+      </c>
+      <c r="DZ1" t="s">
         <v>307</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="EA1" t="s">
         <v>308</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="EB1" t="s">
         <v>309</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EC1" t="s">
         <v>310</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="ED1" t="s">
         <v>311</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EE1" t="s">
         <v>312</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="EF1" t="s">
         <v>313</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EG1" t="s">
         <v>314</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EH1" t="s">
         <v>315</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EI1" t="s">
         <v>316</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EJ1" t="s">
         <v>317</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EK1" t="s">
         <v>318</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EL1" t="s">
         <v>319</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EM1" t="s">
         <v>320</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EN1" t="s">
         <v>321</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EO1" t="s">
         <v>322</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EP1" t="s">
         <v>323</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EQ1" t="s">
         <v>324</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="ER1" t="s">
         <v>325</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="ES1" t="s">
         <v>326</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ET1" t="s">
         <v>327</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="EU1" t="s">
         <v>328</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="EV1" t="s">
         <v>329</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EW1" t="s">
         <v>330</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EX1" t="s">
         <v>331</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EY1" t="s">
         <v>332</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EZ1" t="s">
         <v>333</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="FA1" t="s">
         <v>334</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FB1" t="s">
         <v>335</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FC1" t="s">
         <v>336</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FD1" t="s">
         <v>337</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FE1" t="s">
         <v>338</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FF1" t="s">
         <v>339</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="FG1" t="s">
         <v>340</v>
       </c>
-      <c r="FE1" t="s">
+      <c r="FH1" t="s">
         <v>341</v>
       </c>
-      <c r="FF1" t="s">
+      <c r="FI1" t="s">
         <v>342</v>
       </c>
-      <c r="FG1" t="s">
+      <c r="FJ1" t="s">
         <v>343</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="FK1" t="s">
         <v>344</v>
       </c>
-      <c r="FI1" t="s">
+      <c r="FL1" t="s">
         <v>345</v>
       </c>
-      <c r="FJ1" t="s">
+      <c r="FM1" t="s">
         <v>346</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="FN1" t="s">
         <v>347</v>
       </c>
-      <c r="FL1" t="s">
+      <c r="FO1" t="s">
         <v>348</v>
       </c>
-      <c r="FM1" t="s">
+      <c r="FP1" t="s">
         <v>349</v>
       </c>
-      <c r="FN1" t="s">
+      <c r="FQ1" t="s">
         <v>350</v>
       </c>
-      <c r="FO1" t="s">
+      <c r="FR1" t="s">
         <v>351</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="FS1" t="s">
         <v>352</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="FT1" t="s">
         <v>353</v>
       </c>
-      <c r="FR1" t="s">
+      <c r="FU1" t="s">
         <v>354</v>
       </c>
-      <c r="FS1" t="s">
+      <c r="FV1" t="s">
         <v>355</v>
       </c>
-      <c r="FT1" t="s">
+      <c r="FW1" t="s">
         <v>356</v>
       </c>
-      <c r="FU1" t="s">
+      <c r="FX1" t="s">
         <v>357</v>
       </c>
-      <c r="FV1" t="s">
+      <c r="FY1" t="s">
         <v>358</v>
       </c>
-      <c r="FW1" t="s">
+      <c r="FZ1" t="s">
         <v>359</v>
       </c>
-      <c r="FX1" t="s">
+      <c r="GA1" t="s">
         <v>360</v>
-      </c>
-      <c r="FY1" t="s">
-        <v>361</v>
-      </c>
-      <c r="FZ1" t="s">
-        <v>362</v>
-      </c>
-      <c r="GA1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="2">
@@ -1992,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="CQ2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR2" t="s">
         <v>62</v>
@@ -2001,7 +1992,7 @@
         <v>29</v>
       </c>
       <c r="CT2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU2" t="s">
         <v>76</v>
@@ -4863,7 +4854,7 @@
       <c r="BW9" s="1"/>
       <c r="BX9" s="1"/>
       <c r="BY9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BZ9" t="s">
         <v>208</v>
@@ -4901,34 +4892,34 @@
         <v>5</v>
       </c>
       <c r="CQ9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CS9" s="1">
         <v>5</v>
       </c>
       <c r="CT9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CV9" s="1">
         <v>6</v>
       </c>
       <c r="CW9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY9" s="1">
         <v>10</v>
       </c>
       <c r="CZ9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA9" t="s">
         <v>101</v>
@@ -4937,7 +4928,7 @@
         <v>7</v>
       </c>
       <c r="DC9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DD9" t="s">
         <v>101</v>
@@ -4946,16 +4937,16 @@
         <v>12</v>
       </c>
       <c r="DF9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DG9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DH9" s="1">
         <v>6</v>
       </c>
       <c r="DI9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DJ9" t="s">
         <v>140</v>
@@ -4964,52 +4955,52 @@
         <v>14</v>
       </c>
       <c r="DL9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DM9" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DN9" s="1">
         <v>13</v>
       </c>
       <c r="DO9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DP9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DQ9" s="1">
         <v>5</v>
       </c>
       <c r="DR9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DS9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DT9" s="1">
         <v>9</v>
       </c>
       <c r="DU9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DV9" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="DW9" s="1">
         <v>14</v>
       </c>
       <c r="DX9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DY9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="DZ9" s="1">
         <v>6</v>
       </c>
       <c r="EA9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="EB9" t="s">
         <v>76</v>
@@ -5087,7 +5078,7 @@
       <c r="FY9" s="1"/>
       <c r="FZ9" s="1"/>
       <c r="GA9" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10">
@@ -5340,40 +5331,40 @@
       <c r="CM10" s="1"/>
       <c r="CN10" s="1"/>
       <c r="CO10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CP10" s="1">
         <v>4</v>
       </c>
       <c r="CQ10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CS10" s="1">
         <v>2</v>
       </c>
       <c r="CT10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="CV10" s="1">
         <v>6</v>
       </c>
       <c r="CW10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY10" s="1">
         <v>6</v>
       </c>
       <c r="CZ10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA10" t="s">
         <v>140</v>
@@ -5382,43 +5373,43 @@
         <v>22</v>
       </c>
       <c r="DC10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DD10" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DE10" s="1">
         <v>32</v>
       </c>
       <c r="DF10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DG10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DH10" s="1">
         <v>20</v>
       </c>
       <c r="DI10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DJ10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DK10" s="1">
         <v>9</v>
       </c>
       <c r="DL10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DM10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="DN10" s="1">
         <v>23</v>
       </c>
       <c r="DO10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DP10" t="s">
         <v>76</v>
@@ -5524,7 +5515,7 @@
       <c r="FY10" s="1"/>
       <c r="FZ10" s="1"/>
       <c r="GA10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11">
@@ -5943,7 +5934,7 @@
       <c r="FY11" s="1"/>
       <c r="FZ11" s="1"/>
       <c r="GA11" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12">
@@ -6196,13 +6187,13 @@
       <c r="CM12" s="1"/>
       <c r="CN12" s="1"/>
       <c r="CO12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CP12" s="1">
         <v>4</v>
       </c>
       <c r="CQ12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR12" t="s">
         <v>167</v>
@@ -6211,34 +6202,34 @@
         <v>4</v>
       </c>
       <c r="CT12" t="s">
+        <v>258</v>
+      </c>
+      <c r="CU12" t="s">
         <v>261</v>
-      </c>
-      <c r="CU12" t="s">
-        <v>264</v>
       </c>
       <c r="CV12" s="1">
         <v>7</v>
       </c>
       <c r="CW12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CY12" s="1">
         <v>6</v>
       </c>
       <c r="CZ12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="DB12" s="1">
         <v>15</v>
       </c>
       <c r="DC12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD12" t="s">
         <v>101</v>
@@ -6247,25 +6238,25 @@
         <v>5</v>
       </c>
       <c r="DF12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DH12" s="1">
         <v>8</v>
       </c>
       <c r="DI12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DK12" s="1">
         <v>15</v>
       </c>
       <c r="DL12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DM12" t="s">
         <v>140</v>
@@ -6274,52 +6265,52 @@
         <v>10</v>
       </c>
       <c r="DO12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DP12" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DQ12" s="1">
         <v>19</v>
       </c>
       <c r="DR12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DT12" s="1">
         <v>11</v>
       </c>
       <c r="DU12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DW12" s="1">
         <v>9</v>
       </c>
       <c r="DX12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DY12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DZ12" s="1">
         <v>15</v>
       </c>
       <c r="EA12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EB12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="EC12" s="1">
         <v>39</v>
       </c>
       <c r="ED12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EE12" t="s">
         <v>76</v>
@@ -6390,7 +6381,7 @@
       <c r="FY12" s="1"/>
       <c r="FZ12" s="1"/>
       <c r="GA12" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13">
@@ -6643,13 +6634,13 @@
       <c r="CM13" s="1"/>
       <c r="CN13" s="1"/>
       <c r="CO13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CP13" s="1">
         <v>12</v>
       </c>
       <c r="CQ13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR13" t="s">
         <v>167</v>
@@ -6658,70 +6649,70 @@
         <v>8</v>
       </c>
       <c r="CT13" t="s">
+        <v>258</v>
+      </c>
+      <c r="CU13" t="s">
         <v>261</v>
-      </c>
-      <c r="CU13" t="s">
-        <v>264</v>
       </c>
       <c r="CV13" s="1">
         <v>20</v>
       </c>
       <c r="CW13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CY13" s="1">
         <v>10</v>
       </c>
       <c r="CZ13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="DB13" s="1">
         <v>7</v>
       </c>
       <c r="DC13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="DE13" s="1">
         <v>77</v>
       </c>
       <c r="DF13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG13" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="DH13" s="1">
         <v>13</v>
       </c>
       <c r="DI13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ13" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DK13" s="1">
         <v>6</v>
       </c>
       <c r="DL13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DM13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DN13" s="1">
         <v>6.75</v>
       </c>
       <c r="DO13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DP13" t="s">
         <v>140</v>
@@ -6730,52 +6721,52 @@
         <v>99</v>
       </c>
       <c r="DR13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS13" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DT13" s="1">
         <v>99</v>
       </c>
       <c r="DU13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV13" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DW13" s="1">
         <v>74</v>
       </c>
       <c r="DX13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DY13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DZ13" s="1">
         <v>5</v>
       </c>
       <c r="EA13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="EB13" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="EC13" s="1">
         <v>45</v>
       </c>
       <c r="ED13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EE13" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="EF13" s="1">
         <v>50</v>
       </c>
       <c r="EG13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EH13" t="s">
         <v>76</v>
@@ -6839,7 +6830,7 @@
       <c r="FY13" s="1"/>
       <c r="FZ13" s="1"/>
       <c r="GA13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14">
@@ -7092,13 +7083,13 @@
       <c r="CM14" s="1"/>
       <c r="CN14" s="1"/>
       <c r="CO14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CP14" s="1">
         <v>1</v>
       </c>
       <c r="CQ14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="CR14" t="s">
         <v>167</v>
@@ -7107,34 +7098,34 @@
         <v>8</v>
       </c>
       <c r="CT14" t="s">
+        <v>258</v>
+      </c>
+      <c r="CU14" t="s">
         <v>261</v>
-      </c>
-      <c r="CU14" t="s">
-        <v>264</v>
       </c>
       <c r="CV14" s="1">
         <v>5</v>
       </c>
       <c r="CW14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CY14" s="1">
         <v>9</v>
       </c>
       <c r="CZ14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="DB14" s="1">
         <v>15</v>
       </c>
       <c r="DC14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD14" t="s">
         <v>101</v>
@@ -7143,25 +7134,25 @@
         <v>12</v>
       </c>
       <c r="DF14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DH14" s="1">
         <v>25</v>
       </c>
       <c r="DI14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DK14" s="1">
         <v>17</v>
       </c>
       <c r="DL14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DM14" t="s">
         <v>140</v>
@@ -7170,52 +7161,52 @@
         <v>4</v>
       </c>
       <c r="DO14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DP14" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DQ14" s="1">
         <v>25</v>
       </c>
       <c r="DR14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS14" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DT14" s="1">
         <v>35</v>
       </c>
       <c r="DU14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DW14" s="1">
         <v>16</v>
       </c>
       <c r="DX14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DY14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DZ14" s="1">
         <v>19</v>
       </c>
       <c r="EA14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EB14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="EC14" s="1">
         <v>24</v>
       </c>
       <c r="ED14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EE14" t="s">
         <v>76</v>
@@ -7286,7 +7277,7 @@
       <c r="FY14" s="1"/>
       <c r="FZ14" s="1"/>
       <c r="GA14" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15">
@@ -7545,52 +7536,52 @@
         <v>2</v>
       </c>
       <c r="CQ15" t="s">
+        <v>258</v>
+      </c>
+      <c r="CR15" t="s">
         <v>261</v>
-      </c>
-      <c r="CR15" t="s">
-        <v>264</v>
       </c>
       <c r="CS15" s="1">
         <v>3</v>
       </c>
       <c r="CT15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU15" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CV15" s="1">
         <v>7</v>
       </c>
       <c r="CW15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX15" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="CY15" s="1">
         <v>3</v>
       </c>
       <c r="CZ15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DB15" s="1">
         <v>13</v>
       </c>
       <c r="DC15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DE15" s="1">
         <v>13</v>
       </c>
       <c r="DF15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG15" t="s">
         <v>140</v>
@@ -7599,32 +7590,32 @@
         <v>15</v>
       </c>
       <c r="DI15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ15" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DK15" s="1"/>
       <c r="DL15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DM15" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DN15" s="1">
         <v>11</v>
       </c>
       <c r="DO15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DP15" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="DQ15" s="1">
         <v>11</v>
       </c>
       <c r="DR15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS15" t="s">
         <v>76</v>
@@ -7723,7 +7714,7 @@
       <c r="FY15" s="1"/>
       <c r="FZ15" s="1"/>
       <c r="GA15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16">
@@ -7976,31 +7967,31 @@
       <c r="CM16" s="1"/>
       <c r="CN16" s="1"/>
       <c r="CO16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CP16" s="1">
         <v>9</v>
       </c>
       <c r="CQ16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CS16" s="1">
         <v>9</v>
       </c>
       <c r="CT16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CV16" s="1">
         <v>13</v>
       </c>
       <c r="CW16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX16" t="s">
         <v>140</v>
@@ -8009,52 +8000,52 @@
         <v>13</v>
       </c>
       <c r="CZ16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA16" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DB16" s="1">
         <v>13</v>
       </c>
       <c r="DC16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD16" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DE16" s="1">
         <v>8</v>
       </c>
       <c r="DF16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DH16" s="1">
         <v>6</v>
       </c>
       <c r="DI16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ16" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DK16" s="1">
         <v>15</v>
       </c>
       <c r="DL16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DM16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="DN16" s="1">
         <v>23</v>
       </c>
       <c r="DO16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DP16" t="s">
         <v>76</v>
@@ -8160,7 +8151,7 @@
       <c r="FY16" s="1"/>
       <c r="FZ16" s="1"/>
       <c r="GA16" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17">
@@ -8413,13 +8404,13 @@
       <c r="CM17" s="1"/>
       <c r="CN17" s="1"/>
       <c r="CO17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CP17" s="1">
         <v>2</v>
       </c>
       <c r="CQ17" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR17" t="s">
         <v>76</v>
@@ -8581,7 +8572,7 @@
       <c r="FY17" s="1"/>
       <c r="FZ17" s="1"/>
       <c r="GA17" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18">
@@ -8834,22 +8825,22 @@
       <c r="CM18" s="1"/>
       <c r="CN18" s="1"/>
       <c r="CO18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CP18" s="1">
         <v>14</v>
       </c>
       <c r="CQ18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR18" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="CS18" s="1">
         <v>36</v>
       </c>
       <c r="CT18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU18" t="s">
         <v>76</v>
@@ -9004,7 +8995,7 @@
       <c r="FY18" s="1"/>
       <c r="FZ18" s="1"/>
       <c r="GA18" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19">
@@ -9257,22 +9248,22 @@
       <c r="CM19" s="1"/>
       <c r="CN19" s="1"/>
       <c r="CO19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CP19" s="1">
         <v>1</v>
       </c>
       <c r="CQ19" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR19" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="CS19" s="1">
         <v>17</v>
       </c>
       <c r="CT19" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU19" t="s">
         <v>76</v>
@@ -9427,7 +9418,7 @@
       <c r="FY19" s="1"/>
       <c r="FZ19" s="1"/>
       <c r="GA19" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20">
@@ -9680,22 +9671,22 @@
       <c r="CM20" s="1"/>
       <c r="CN20" s="1"/>
       <c r="CO20" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CP20" s="1">
         <v>6</v>
       </c>
       <c r="CQ20" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="CS20" s="1">
         <v>24</v>
       </c>
       <c r="CT20" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU20" t="s">
         <v>76</v>
@@ -9850,7 +9841,7 @@
       <c r="FY20" s="1"/>
       <c r="FZ20" s="1"/>
       <c r="GA20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21">
@@ -10077,29 +10068,29 @@
       <c r="BW21" s="1"/>
       <c r="BX21" s="1"/>
       <c r="BY21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="BZ21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="CA21" t="s">
         <v>212</v>
       </c>
       <c r="CB21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="CC21" s="1"/>
       <c r="CD21" s="1"/>
       <c r="CE21" s="1"/>
       <c r="CF21" s="1"/>
       <c r="CG21" t="s">
+        <v>235</v>
+      </c>
+      <c r="CH21" t="s">
         <v>237</v>
       </c>
-      <c r="CH21" t="s">
+      <c r="CI21" t="s">
         <v>239</v>
-      </c>
-      <c r="CI21" t="s">
-        <v>241</v>
       </c>
       <c r="CJ21" t="s">
         <v>210</v>
@@ -10115,34 +10106,34 @@
         <v>8</v>
       </c>
       <c r="CQ21" t="s">
+        <v>258</v>
+      </c>
+      <c r="CR21" t="s">
         <v>261</v>
-      </c>
-      <c r="CR21" t="s">
-        <v>264</v>
       </c>
       <c r="CS21" s="1">
         <v>3</v>
       </c>
       <c r="CT21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="CU21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="CV21" s="1">
         <v>1</v>
       </c>
       <c r="CW21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="CX21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY21" s="1">
         <v>5</v>
       </c>
       <c r="CZ21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DA21" t="s">
         <v>101</v>
@@ -10151,70 +10142,70 @@
         <v>13</v>
       </c>
       <c r="DC21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DE21" s="1">
         <v>20</v>
       </c>
       <c r="DF21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DH21" s="1">
         <v>74</v>
       </c>
       <c r="DI21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ21" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="DK21" s="1">
         <v>28</v>
       </c>
       <c r="DL21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DM21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="DN21" s="1">
         <v>4</v>
       </c>
       <c r="DO21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DP21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="DQ21" s="1">
         <v>84</v>
       </c>
       <c r="DR21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS21" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="DT21" s="1">
         <v>31</v>
       </c>
       <c r="DU21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV21" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="DW21" s="1">
         <v>28</v>
       </c>
       <c r="DX21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DY21" t="s">
         <v>76</v>
@@ -10558,13 +10549,13 @@
       <c r="CM22" s="1"/>
       <c r="CN22" s="1"/>
       <c r="CO22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CP22" s="1">
         <v>7</v>
       </c>
       <c r="CQ22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR22" t="s">
         <v>167</v>
@@ -10573,43 +10564,43 @@
         <v>22</v>
       </c>
       <c r="CT22" t="s">
+        <v>258</v>
+      </c>
+      <c r="CU22" t="s">
         <v>261</v>
-      </c>
-      <c r="CU22" t="s">
-        <v>264</v>
       </c>
       <c r="CV22" s="1">
         <v>59</v>
       </c>
       <c r="CW22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="CY22" s="1">
         <v>26</v>
       </c>
       <c r="CZ22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA22" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DB22" s="1">
         <v>28</v>
       </c>
       <c r="DC22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="DE22" s="1">
         <v>51</v>
       </c>
       <c r="DF22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG22" t="s">
         <v>88</v>
@@ -10618,7 +10609,7 @@
         <v>15</v>
       </c>
       <c r="DI22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DJ22" t="s">
         <v>101</v>
@@ -10627,106 +10618,106 @@
         <v>1</v>
       </c>
       <c r="DL22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DM22" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="DN22" s="1">
         <v>10</v>
       </c>
       <c r="DO22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DP22" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DQ22" s="1">
         <v>18</v>
       </c>
       <c r="DR22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DT22" s="1">
         <v>46</v>
       </c>
       <c r="DU22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DW22" s="1">
         <v>24</v>
       </c>
       <c r="DX22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DY22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DZ22" s="1">
         <v>18</v>
       </c>
       <c r="EA22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EB22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="EC22" s="1">
         <v>36</v>
       </c>
       <c r="ED22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EE22" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="EF22" s="1">
         <v>23</v>
       </c>
       <c r="EG22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EH22" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="EI22" s="1">
         <v>10</v>
       </c>
       <c r="EJ22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EK22" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="EL22" s="1">
         <v>19</v>
       </c>
       <c r="EM22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EN22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="EO22" s="1">
         <v>23</v>
       </c>
       <c r="EP22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EQ22" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="ER22" s="1">
         <v>19</v>
       </c>
       <c r="ES22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="ET22" s="1"/>
       <c r="EU22" s="1"/>
@@ -11017,22 +11008,22 @@
       <c r="CM23" s="1"/>
       <c r="CN23" s="1"/>
       <c r="CO23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="CP23" s="1">
         <v>8</v>
       </c>
       <c r="CQ23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CS23" s="1">
         <v>38</v>
       </c>
       <c r="CT23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU23" t="s">
         <v>88</v>
@@ -11041,25 +11032,25 @@
         <v>55</v>
       </c>
       <c r="CW23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CY23" s="1">
         <v>3</v>
       </c>
       <c r="CZ23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DA23" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="DB23" s="1">
         <v>4</v>
       </c>
       <c r="DC23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DD23" t="s">
         <v>101</v>
@@ -11068,25 +11059,25 @@
         <v>9</v>
       </c>
       <c r="DF23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DG23" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DH23" s="1">
         <v>19</v>
       </c>
       <c r="DI23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DJ23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DK23" s="1">
         <v>15</v>
       </c>
       <c r="DL23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DM23" t="s">
         <v>140</v>
@@ -11095,61 +11086,61 @@
         <v>141</v>
       </c>
       <c r="DO23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DP23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="DQ23" s="1">
         <v>12</v>
       </c>
       <c r="DR23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DS23" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DT23" s="1">
         <v>215</v>
       </c>
       <c r="DU23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV23" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DW23" s="1">
         <v>260</v>
       </c>
       <c r="DX23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DY23" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DZ23" s="1">
         <v>21</v>
       </c>
       <c r="EA23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="EB23" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="EC23" s="1">
         <v>100</v>
       </c>
       <c r="ED23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EE23" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="EF23" s="1">
         <v>4.5</v>
       </c>
       <c r="EG23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="EH23" t="s">
         <v>76</v>
@@ -11159,13 +11150,13 @@
         <v>76</v>
       </c>
       <c r="EK23" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="EL23" s="1">
         <v>75</v>
       </c>
       <c r="EM23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EN23" t="s">
         <v>76</v>
@@ -11215,7 +11206,7 @@
       <c r="FY23" s="1"/>
       <c r="FZ23" s="1"/>
       <c r="GA23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24">
@@ -11476,25 +11467,25 @@
         <v>104</v>
       </c>
       <c r="CQ24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CS24" s="1">
         <v>9</v>
       </c>
       <c r="CT24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="CU24" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CV24" s="1">
         <v>20</v>
       </c>
       <c r="CW24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="CX24" t="s">
         <v>101</v>
@@ -11503,7 +11494,7 @@
         <v>13</v>
       </c>
       <c r="CZ24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA24" t="s">
         <v>101</v>
@@ -11512,25 +11503,25 @@
         <v>12</v>
       </c>
       <c r="DC24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DD24" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DE24" s="1">
         <v>13.5</v>
       </c>
       <c r="DF24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DG24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DH24" s="1">
         <v>16.75</v>
       </c>
       <c r="DI24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DJ24" t="s">
         <v>140</v>
@@ -11539,52 +11530,52 @@
         <v>141</v>
       </c>
       <c r="DL24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DM24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="DN24" s="1">
         <v>15.5</v>
       </c>
       <c r="DO24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DP24" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="DQ24" s="1">
         <v>100</v>
       </c>
       <c r="DR24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DS24" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DT24" s="1">
         <v>254</v>
       </c>
       <c r="DU24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DV24" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="DW24" s="1">
         <v>8</v>
       </c>
       <c r="DX24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="DY24" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DZ24" s="1">
         <v>68</v>
       </c>
       <c r="EA24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="EB24" t="s">
         <v>76</v>
@@ -12500,7 +12491,7 @@
       <c r="FY26" s="1"/>
       <c r="FZ26" s="1"/>
       <c r="GA26" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27">
@@ -13326,7 +13317,7 @@
       <c r="FY28" s="1"/>
       <c r="FZ28" s="1"/>
       <c r="GA28" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29">
@@ -13739,7 +13730,7 @@
       <c r="FY29" s="1"/>
       <c r="FZ29" s="1"/>
       <c r="GA29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="30">
@@ -14156,7 +14147,7 @@
       <c r="FY30" s="1"/>
       <c r="FZ30" s="1"/>
       <c r="GA30" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="31">
@@ -14573,7 +14564,7 @@
       <c r="FY31" s="1"/>
       <c r="FZ31" s="1"/>
       <c r="GA31" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="32">
@@ -14990,7 +14981,7 @@
       <c r="FY32" s="1"/>
       <c r="FZ32" s="1"/>
       <c r="GA32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33">
@@ -15407,7 +15398,7 @@
       <c r="FY33" s="1"/>
       <c r="FZ33" s="1"/>
       <c r="GA33" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="34">
@@ -15810,7 +15801,7 @@
       <c r="FY34" s="1"/>
       <c r="FZ34" s="1"/>
       <c r="GA34" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35">
@@ -16213,7 +16204,7 @@
       <c r="FY35" s="1"/>
       <c r="FZ35" s="1"/>
       <c r="GA35" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="36">
@@ -16616,7 +16607,7 @@
       <c r="FY36" s="1"/>
       <c r="FZ36" s="1"/>
       <c r="GA36" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37">
@@ -17019,7 +17010,7 @@
       <c r="FY37" s="1"/>
       <c r="FZ37" s="1"/>
       <c r="GA37" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="38">
@@ -17422,7 +17413,7 @@
       <c r="FY38" s="1"/>
       <c r="FZ38" s="1"/>
       <c r="GA38" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39">
@@ -19684,20 +19675,20 @@
       <c r="CM44" s="1"/>
       <c r="CN44" s="1"/>
       <c r="CO44" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CP44" s="1">
         <v>12</v>
       </c>
       <c r="CQ44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR44" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CS44" s="1"/>
       <c r="CT44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU44" t="s">
         <v>168</v>
@@ -19706,7 +19697,7 @@
         <v>9</v>
       </c>
       <c r="CW44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX44" t="s">
         <v>76</v>
@@ -19854,7 +19845,7 @@
       <c r="FY44" s="1"/>
       <c r="FZ44" s="1"/>
       <c r="GA44" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="45">
@@ -20091,20 +20082,20 @@
       <c r="CM45" s="1"/>
       <c r="CN45" s="1"/>
       <c r="CO45" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CP45" s="1">
         <v>26</v>
       </c>
       <c r="CQ45" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR45" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CS45" s="1"/>
       <c r="CT45" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU45" t="s">
         <v>168</v>
@@ -20113,7 +20104,7 @@
         <v>26</v>
       </c>
       <c r="CW45" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX45" t="s">
         <v>76</v>
@@ -20261,7 +20252,7 @@
       <c r="FY45" s="1"/>
       <c r="FZ45" s="1"/>
       <c r="GA45" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="46">
@@ -20498,31 +20489,31 @@
       <c r="CM46" s="1"/>
       <c r="CN46" s="1"/>
       <c r="CO46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="CP46" s="1">
         <v>6</v>
       </c>
       <c r="CQ46" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR46" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="CS46" s="1">
         <v>17</v>
       </c>
       <c r="CT46" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU46" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="CV46" s="1">
         <v>12</v>
       </c>
       <c r="CW46" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX46" t="s">
         <v>76</v>
@@ -20670,7 +20661,7 @@
       <c r="FY46" s="1"/>
       <c r="FZ46" s="1"/>
       <c r="GA46" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47">
@@ -21073,7 +21064,7 @@
       <c r="FY47" s="1"/>
       <c r="FZ47" s="1"/>
       <c r="GA47" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48">
@@ -21312,40 +21303,40 @@
       <c r="CM48" s="1"/>
       <c r="CN48" s="1"/>
       <c r="CO48" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="CP48" s="1">
         <v>4</v>
       </c>
       <c r="CQ48" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="CS48" s="1">
         <v>4</v>
       </c>
       <c r="CT48" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU48" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CV48" s="1">
         <v>43</v>
       </c>
       <c r="CW48" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX48" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CY48" s="1">
         <v>15</v>
       </c>
       <c r="CZ48" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA48" t="s">
         <v>76</v>
@@ -21486,7 +21477,7 @@
       <c r="FY48" s="1"/>
       <c r="FZ48" s="1"/>
       <c r="GA48" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49">
@@ -21889,7 +21880,7 @@
       <c r="FY49" s="1"/>
       <c r="FZ49" s="1"/>
       <c r="GA49" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50">
@@ -22292,7 +22283,7 @@
       <c r="FY50" s="1"/>
       <c r="FZ50" s="1"/>
       <c r="GA50" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51">
@@ -22695,7 +22686,7 @@
       <c r="FY51" s="1"/>
       <c r="FZ51" s="1"/>
       <c r="GA51" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52">
@@ -23098,7 +23089,7 @@
       <c r="FY52" s="1"/>
       <c r="FZ52" s="1"/>
       <c r="GA52" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53">
@@ -23501,7 +23492,7 @@
       <c r="FY53" s="1"/>
       <c r="FZ53" s="1"/>
       <c r="GA53" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="54">
@@ -23904,7 +23895,7 @@
       <c r="FY54" s="1"/>
       <c r="FZ54" s="1"/>
       <c r="GA54" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="55">
@@ -24149,25 +24140,25 @@
         <v>20</v>
       </c>
       <c r="CQ55" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR55" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="CS55" s="1">
         <v>8</v>
       </c>
       <c r="CT55" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU55" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="CV55" s="1">
         <v>30</v>
       </c>
       <c r="CW55" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX55" t="s">
         <v>76</v>
@@ -24315,7 +24306,7 @@
       <c r="FY55" s="1"/>
       <c r="FZ55" s="1"/>
       <c r="GA55" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56">
@@ -24552,13 +24543,13 @@
       <c r="CM56" s="1"/>
       <c r="CN56" s="1"/>
       <c r="CO56" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CP56" s="1">
         <v>24</v>
       </c>
       <c r="CQ56" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR56" t="s">
         <v>88</v>
@@ -24567,25 +24558,25 @@
         <v>43</v>
       </c>
       <c r="CT56" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU56" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CV56" s="1">
         <v>37</v>
       </c>
       <c r="CW56" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX56" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY56" s="1">
         <v>59</v>
       </c>
       <c r="CZ56" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA56" t="s">
         <v>101</v>
@@ -24594,16 +24585,16 @@
         <v>62</v>
       </c>
       <c r="DC56" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD56" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DE56" s="1">
         <v>43</v>
       </c>
       <c r="DF56" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG56" t="s">
         <v>76</v>
@@ -24730,7 +24721,7 @@
       <c r="FY56" s="1"/>
       <c r="FZ56" s="1"/>
       <c r="GA56" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="57">
@@ -24967,13 +24958,13 @@
       <c r="CM57" s="1"/>
       <c r="CN57" s="1"/>
       <c r="CO57" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CP57" s="1">
         <v>6</v>
       </c>
       <c r="CQ57" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR57" t="s">
         <v>88</v>
@@ -24982,25 +24973,25 @@
         <v>10</v>
       </c>
       <c r="CT57" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU57" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CV57" s="1">
         <v>25</v>
       </c>
       <c r="CW57" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX57" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY57" s="1">
         <v>11</v>
       </c>
       <c r="CZ57" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DA57" t="s">
         <v>101</v>
@@ -25009,16 +25000,16 @@
         <v>15</v>
       </c>
       <c r="DC57" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DD57" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DE57" s="1">
         <v>13</v>
       </c>
       <c r="DF57" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="DG57" t="s">
         <v>76</v>
@@ -25145,7 +25136,7 @@
       <c r="FY57" s="1"/>
       <c r="FZ57" s="1"/>
       <c r="GA57" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58">
@@ -25343,7 +25334,7 @@
         <v>214</v>
       </c>
       <c r="BT58" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="BU58" t="s">
         <v>214</v>
@@ -25352,10 +25343,10 @@
       <c r="BW58" s="1"/>
       <c r="BX58" s="1"/>
       <c r="BY58" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="BZ58" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="CA58" t="s">
         <v>212</v>
@@ -25384,22 +25375,22 @@
       <c r="CM58" s="1"/>
       <c r="CN58" s="1"/>
       <c r="CO58" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CP58" s="1">
         <v>2</v>
       </c>
       <c r="CQ58" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR58" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="CS58" s="1">
         <v>4</v>
       </c>
       <c r="CT58" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU58" t="s">
         <v>76</v>
@@ -25752,7 +25743,7 @@
         <v>214</v>
       </c>
       <c r="BT59" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="BU59" t="s">
         <v>214</v>
@@ -25761,10 +25752,10 @@
       <c r="BW59" s="1"/>
       <c r="BX59" s="1"/>
       <c r="BY59" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="BZ59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="CA59" t="s">
         <v>212</v>
@@ -25793,22 +25784,22 @@
       <c r="CM59" s="1"/>
       <c r="CN59" s="1"/>
       <c r="CO59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CP59" s="1">
         <v>5</v>
       </c>
       <c r="CQ59" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR59" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="CS59" s="1">
         <v>7</v>
       </c>
       <c r="CT59" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU59" t="s">
         <v>76</v>
@@ -26200,49 +26191,49 @@
       <c r="CM60" s="1"/>
       <c r="CN60" s="1"/>
       <c r="CO60" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="CP60" s="1">
         <v>2</v>
       </c>
       <c r="CQ60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR60" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CS60" s="1">
         <v>24</v>
       </c>
       <c r="CT60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU60" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CV60" s="1">
         <v>6</v>
       </c>
       <c r="CW60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY60" s="1">
         <v>20</v>
       </c>
       <c r="CZ60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA60" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DB60" s="1">
         <v>18</v>
       </c>
       <c r="DC60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DD60" t="s">
         <v>76</v>
@@ -26376,7 +26367,7 @@
       <c r="FY60" s="1"/>
       <c r="FZ60" s="1"/>
       <c r="GA60" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="61">
@@ -26613,49 +26604,49 @@
       <c r="CM61" s="1"/>
       <c r="CN61" s="1"/>
       <c r="CO61" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="CP61" s="1">
         <v>4</v>
       </c>
       <c r="CQ61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR61" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CS61" s="1">
         <v>11</v>
       </c>
       <c r="CT61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU61" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CV61" s="1">
         <v>15</v>
       </c>
       <c r="CW61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX61" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CY61" s="1">
         <v>11</v>
       </c>
       <c r="CZ61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA61" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="DB61" s="1">
         <v>22</v>
       </c>
       <c r="DC61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DD61" t="s">
         <v>76</v>
@@ -26789,7 +26780,7 @@
       <c r="FY61" s="1"/>
       <c r="FZ61" s="1"/>
       <c r="GA61" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62">
@@ -28194,7 +28185,7 @@
         <v>215</v>
       </c>
       <c r="BT65" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="BU65" t="s">
         <v>76</v>
@@ -28235,13 +28226,13 @@
       <c r="CM65" s="1"/>
       <c r="CN65" s="1"/>
       <c r="CO65" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="CP65" s="1">
         <v>24</v>
       </c>
       <c r="CQ65" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR65" t="s">
         <v>76</v>
@@ -28403,7 +28394,7 @@
       <c r="FY65" s="1"/>
       <c r="FZ65" s="1"/>
       <c r="GA65" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66">
@@ -28806,7 +28797,7 @@
       <c r="FY66" s="1"/>
       <c r="FZ66" s="1"/>
       <c r="GA66" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="67">
@@ -29043,22 +29034,22 @@
       <c r="CM67" s="1"/>
       <c r="CN67" s="1"/>
       <c r="CO67" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="CP67" s="1">
         <v>10</v>
       </c>
       <c r="CQ67" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR67" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="CS67" s="1">
         <v>31</v>
       </c>
       <c r="CT67" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU67" t="s">
         <v>140</v>
@@ -29067,25 +29058,25 @@
         <v>35</v>
       </c>
       <c r="CW67" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX67" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="CY67" s="1">
         <v>21</v>
       </c>
       <c r="CZ67" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA67" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="DB67" s="1">
         <v>5</v>
       </c>
       <c r="DC67" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DD67" t="s">
         <v>76</v>
@@ -29219,7 +29210,7 @@
       <c r="FY67" s="1"/>
       <c r="FZ67" s="1"/>
       <c r="GA67" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="68">
@@ -29462,34 +29453,34 @@
         <v>35</v>
       </c>
       <c r="CQ68" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR68" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="CS68" s="1">
         <v>25</v>
       </c>
       <c r="CT68" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU68" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="CV68" s="1">
         <v>20</v>
       </c>
       <c r="CW68" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX68" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="CY68" s="1">
         <v>17</v>
       </c>
       <c r="CZ68" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA68" t="s">
         <v>76</v>
@@ -29630,7 +29621,7 @@
       <c r="FY68" s="1"/>
       <c r="FZ68" s="1"/>
       <c r="GA68" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69">
@@ -29873,34 +29864,34 @@
         <v>20</v>
       </c>
       <c r="CQ69" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CR69" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="CS69" s="1">
         <v>35</v>
       </c>
       <c r="CT69" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CU69" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="CV69" s="1">
         <v>6</v>
       </c>
       <c r="CW69" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="CX69" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="CY69" s="1">
         <v>14</v>
       </c>
       <c r="CZ69" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="DA69" t="s">
         <v>76</v>
@@ -30041,7 +30032,7 @@
       <c r="FY69" s="1"/>
       <c r="FZ69" s="1"/>
       <c r="GA69" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="70">
@@ -30278,13 +30269,13 @@
       <c r="CM70" s="1"/>
       <c r="CN70" s="1"/>
       <c r="CO70" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CP70" s="1">
         <v>24</v>
       </c>
       <c r="CQ70" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR70" t="s">
         <v>140</v>
@@ -30293,16 +30284,16 @@
         <v>15</v>
       </c>
       <c r="CT70" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU70" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="CV70" s="1">
         <v>21</v>
       </c>
       <c r="CW70" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX70" t="s">
         <v>76</v>
@@ -30450,7 +30441,7 @@
       <c r="FY70" s="1"/>
       <c r="FZ70" s="1"/>
       <c r="GA70" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="71">
@@ -30687,13 +30678,13 @@
       <c r="CM71" s="1"/>
       <c r="CN71" s="1"/>
       <c r="CO71" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="CP71" s="1">
         <v>28</v>
       </c>
       <c r="CQ71" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CR71" t="s">
         <v>140</v>
@@ -30702,16 +30693,16 @@
         <v>20</v>
       </c>
       <c r="CT71" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CU71" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="CV71" s="1">
         <v>11</v>
       </c>
       <c r="CW71" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="CX71" t="s">
         <v>76</v>
@@ -30859,7 +30850,7 @@
       <c r="FY71" s="1"/>
       <c r="FZ71" s="1"/>
       <c r="GA71" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72">

</xml_diff>